<commit_message>
add % data to citizenship by eng ability tables
</commit_message>
<xml_diff>
--- a/AAJC Vis/case_studies/citizenship_english_ability_tables.xlsx
+++ b/AAJC Vis/case_studies/citizenship_english_ability_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anamkhan/Documents/Demo Advisors/AAJC/AAJC Vis/case_studies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8EF8F5-5E42-8240-908A-07DB349C62D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83664FE8-79D3-AE49-A87A-12ADD29D7C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17220" activeTab="5" xr2:uid="{7F9E964A-6C9F-BE4C-A5F8-FD2379A71560}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17200" activeTab="3" xr2:uid="{7F9E964A-6C9F-BE4C-A5F8-FD2379A71560}"/>
   </bookViews>
   <sheets>
     <sheet name="Los Angeles CA" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="80">
   <si>
     <t>Citizenship</t>
   </si>
@@ -348,6 +348,78 @@
   <si>
     <t>Benton County</t>
   </si>
+  <si>
+    <t>county</t>
+  </si>
+  <si>
+    <t>Hawaii County, Hawaii</t>
+  </si>
+  <si>
+    <t>Honolulu County, Hawaii</t>
+  </si>
+  <si>
+    <t>Kalawao County, Hawaii</t>
+  </si>
+  <si>
+    <t>Kauai County, Hawaii</t>
+  </si>
+  <si>
+    <t>Maui County, Hawaii</t>
+  </si>
+  <si>
+    <t>tot nhpi pop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hawaii </t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>Salt Lake county</t>
+  </si>
+  <si>
+    <t>Utah county</t>
+  </si>
+  <si>
+    <t>tot asian pop</t>
+  </si>
+  <si>
+    <t>california</t>
+  </si>
+  <si>
+    <t>la county</t>
+  </si>
+  <si>
+    <t xml:space="preserve">us </t>
+  </si>
+  <si>
+    <t>harris county</t>
+  </si>
+  <si>
+    <t>King county</t>
+  </si>
+  <si>
+    <t>bronx</t>
+  </si>
+  <si>
+    <t>kings county</t>
+  </si>
+  <si>
+    <t xml:space="preserve">richmond </t>
+  </si>
+  <si>
+    <t>queens</t>
+  </si>
+  <si>
+    <t>manhattanny county</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>NYC</t>
+  </si>
 </sst>
 </file>
 
@@ -357,7 +429,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -459,6 +531,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -787,22 +865,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="7" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="9" fontId="7" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="9" fontId="7" fillId="5" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="9" fontId="7" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -903,6 +972,11 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="7" fillId="5" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1236,7 +1310,7 @@
   <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1247,47 +1321,63 @@
     <col min="9" max="9" width="10.83203125" style="49"/>
     <col min="10" max="10" width="14" customWidth="1"/>
     <col min="11" max="11" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:12" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="74"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="71"/>
+      <c r="L2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="3" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="K3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3">
+        <v>1488626</v>
+      </c>
     </row>
     <row r="4" spans="2:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="71"/>
-      <c r="C4" s="75" t="s">
+      <c r="B4" s="68"/>
+      <c r="C4" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="76"/>
-      <c r="E4" s="75" t="s">
+      <c r="D4" s="73"/>
+      <c r="E4" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="76"/>
-      <c r="G4" s="75" t="s">
+      <c r="F4" s="73"/>
+      <c r="G4" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="76"/>
+      <c r="H4" s="73"/>
+      <c r="K4" t="s">
+        <v>68</v>
+      </c>
+      <c r="L4">
+        <v>5834312</v>
+      </c>
     </row>
     <row r="5" spans="2:12" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="39" t="s">
@@ -1311,6 +1401,12 @@
       <c r="H5" s="52" t="s">
         <v>48</v>
       </c>
+      <c r="K5" t="s">
+        <v>70</v>
+      </c>
+      <c r="L5">
+        <v>18421637</v>
+      </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B6" s="24" t="s">
@@ -1319,20 +1415,23 @@
       <c r="C6" s="27">
         <v>523166</v>
       </c>
-      <c r="D6" s="54" t="s">
-        <v>12</v>
+      <c r="D6" s="54">
+        <f>C6/L3</f>
+        <v>0.35144220240678314</v>
       </c>
       <c r="E6" s="27">
         <v>2194401</v>
       </c>
-      <c r="F6" s="54" t="s">
-        <v>12</v>
+      <c r="F6" s="54">
+        <f>E6/L4</f>
+        <v>0.37611992639406328</v>
       </c>
       <c r="G6" s="27">
         <v>6384997</v>
       </c>
-      <c r="H6" s="57" t="s">
-        <v>12</v>
+      <c r="H6" s="60">
+        <f>G6/L5</f>
+        <v>0.34660312761564022</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="17" x14ac:dyDescent="0.2">
@@ -1367,7 +1466,7 @@
       <c r="G8" s="27">
         <v>3006846</v>
       </c>
-      <c r="H8" s="58">
+      <c r="H8" s="56">
         <f>G8/$G$6</f>
         <v>0.4709236355161952</v>
       </c>
@@ -1396,7 +1495,7 @@
       <c r="G9" s="27">
         <v>2452956</v>
       </c>
-      <c r="H9" s="58">
+      <c r="H9" s="56">
         <f t="shared" ref="H9:H11" si="2">G9/$G$6</f>
         <v>0.38417496515660071</v>
       </c>
@@ -1425,7 +1524,7 @@
       <c r="G10" s="27">
         <v>2058825</v>
       </c>
-      <c r="H10" s="58">
+      <c r="H10" s="56">
         <f t="shared" si="2"/>
         <v>0.32244729324070159</v>
       </c>
@@ -1454,7 +1553,7 @@
       <c r="G11" s="27">
         <v>394131</v>
       </c>
-      <c r="H11" s="58">
+      <c r="H11" s="56">
         <f t="shared" si="2"/>
         <v>6.1727671915899097E-2</v>
       </c>
@@ -1509,7 +1608,7 @@
       <c r="G13" s="27">
         <v>7100074</v>
       </c>
-      <c r="H13" s="58">
+      <c r="H13" s="56">
         <f>G13/$G$15</f>
         <v>0.58987175823153304</v>
       </c>
@@ -1535,7 +1634,7 @@
       <c r="G14" s="27">
         <v>4936566</v>
       </c>
-      <c r="H14" s="58">
+      <c r="H14" s="56">
         <f t="shared" ref="H14:H20" si="5">G14/$G$15</f>
         <v>0.41012824176846696</v>
       </c>
@@ -1548,21 +1647,24 @@
         <f>SUM(C13:C14)</f>
         <v>965460</v>
       </c>
-      <c r="D15" s="55" t="s">
-        <v>12</v>
+      <c r="D15" s="54">
+        <f>C15/L3</f>
+        <v>0.64855779759321686</v>
       </c>
       <c r="E15" s="27">
         <f t="shared" ref="E15" si="6">SUM(E13:E14)</f>
         <v>3639911</v>
       </c>
-      <c r="F15" s="55" t="s">
-        <v>12</v>
+      <c r="F15" s="54">
+        <f>E15/L4</f>
+        <v>0.62388007360593678</v>
       </c>
       <c r="G15" s="27">
         <v>12036640</v>
       </c>
-      <c r="H15" s="63" t="s">
-        <v>12</v>
+      <c r="H15" s="60">
+        <f>G15/L5</f>
+        <v>0.65339687238435973</v>
       </c>
     </row>
     <row r="16" spans="2:12" ht="17" x14ac:dyDescent="0.2">
@@ -1574,7 +1676,7 @@
       <c r="E16" s="30"/>
       <c r="F16" s="53"/>
       <c r="G16" s="30"/>
-      <c r="H16" s="58"/>
+      <c r="H16" s="56"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17" s="36" t="s">
@@ -1597,7 +1699,7 @@
       <c r="G17" s="27">
         <v>1552111</v>
       </c>
-      <c r="H17" s="58">
+      <c r="H17" s="56">
         <f t="shared" si="5"/>
         <v>0.12894885948238047</v>
       </c>
@@ -1623,7 +1725,7 @@
       <c r="G18" s="27">
         <v>10383822</v>
       </c>
-      <c r="H18" s="58">
+      <c r="H18" s="56">
         <f t="shared" si="5"/>
         <v>0.86268443685280938</v>
       </c>
@@ -1649,7 +1751,7 @@
       <c r="G19" s="27">
         <v>5231985</v>
       </c>
-      <c r="H19" s="58">
+      <c r="H19" s="56">
         <f t="shared" si="5"/>
         <v>0.43467155285860504</v>
       </c>
@@ -1661,21 +1763,21 @@
       <c r="C20" s="33">
         <v>504644</v>
       </c>
-      <c r="D20" s="64">
+      <c r="D20" s="61">
         <f t="shared" si="3"/>
         <v>0.52269798852360527</v>
       </c>
       <c r="E20" s="33">
         <v>1705924</v>
       </c>
-      <c r="F20" s="64">
+      <c r="F20" s="61">
         <f t="shared" si="4"/>
         <v>0.4686718988458784</v>
       </c>
       <c r="G20" s="33">
         <v>5151837</v>
       </c>
-      <c r="H20" s="60">
+      <c r="H20" s="57">
         <f t="shared" si="5"/>
         <v>0.42801288399420434</v>
       </c>
@@ -1688,43 +1790,46 @@
     </row>
     <row r="25" spans="2:12" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="26" spans="2:12" ht="21" x14ac:dyDescent="0.2">
-      <c r="B26" s="72" t="s">
+      <c r="B26" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="73"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="73"/>
-      <c r="F26" s="73"/>
-      <c r="G26" s="73"/>
-      <c r="H26" s="74"/>
+      <c r="C26" s="70"/>
+      <c r="D26" s="70"/>
+      <c r="E26" s="70"/>
+      <c r="F26" s="70"/>
+      <c r="G26" s="70"/>
+      <c r="H26" s="71"/>
     </row>
     <row r="27" spans="2:12" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="70" t="s">
+      <c r="B27" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="69" t="s">
+      <c r="C27" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="69"/>
-      <c r="E27" s="69"/>
-      <c r="F27" s="69"/>
-      <c r="G27" s="69"/>
-      <c r="H27" s="69"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="66"/>
+      <c r="F27" s="66"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="66"/>
     </row>
     <row r="28" spans="2:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="71"/>
-      <c r="C28" s="75" t="s">
+      <c r="B28" s="68"/>
+      <c r="C28" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="76"/>
-      <c r="E28" s="75" t="s">
+      <c r="D28" s="73"/>
+      <c r="E28" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="F28" s="76"/>
-      <c r="G28" s="75" t="s">
+      <c r="F28" s="73"/>
+      <c r="G28" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="H28" s="76"/>
+      <c r="H28" s="73"/>
+      <c r="L28" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="29" spans="2:12" ht="43" x14ac:dyDescent="0.2">
       <c r="B29" s="39" t="s">
@@ -1736,7 +1841,7 @@
       <c r="D29" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="E29" s="65" t="s">
+      <c r="E29" s="62" t="s">
         <v>47</v>
       </c>
       <c r="F29" s="52" t="s">
@@ -1747,6 +1852,12 @@
       </c>
       <c r="H29" s="52" t="s">
         <v>48</v>
+      </c>
+      <c r="K29" t="s">
+        <v>69</v>
+      </c>
+      <c r="L29">
+        <v>25068</v>
       </c>
     </row>
     <row r="30" spans="2:12" ht="19" x14ac:dyDescent="0.25">
@@ -1756,24 +1867,31 @@
       <c r="C30" s="27">
         <v>18934</v>
       </c>
-      <c r="D30" s="57" t="s">
-        <v>12</v>
+      <c r="D30" s="60">
+        <f>C30/L29</f>
+        <v>0.7553055688527206</v>
       </c>
       <c r="E30" s="27">
         <v>106871</v>
       </c>
-      <c r="F30" s="57" t="s">
-        <v>12</v>
+      <c r="F30" s="60">
+        <f>E30/L30</f>
+        <v>0.71420647437782347</v>
       </c>
       <c r="G30" s="27">
         <v>465799</v>
       </c>
-      <c r="H30" s="57" t="s">
-        <v>12</v>
+      <c r="H30" s="60">
+        <f>G30/L31</f>
+        <v>0.76185141085109032</v>
       </c>
       <c r="J30" s="25"/>
-      <c r="K30" s="25"/>
-      <c r="L30" s="25"/>
+      <c r="K30" t="s">
+        <v>68</v>
+      </c>
+      <c r="L30">
+        <v>149636</v>
+      </c>
     </row>
     <row r="31" spans="2:12" ht="19" x14ac:dyDescent="0.25">
       <c r="B31" s="35" t="s">
@@ -1786,8 +1904,12 @@
       <c r="G31" s="30"/>
       <c r="H31" s="32"/>
       <c r="J31" s="25"/>
-      <c r="K31" s="25"/>
-      <c r="L31" s="25"/>
+      <c r="K31" t="s">
+        <v>70</v>
+      </c>
+      <c r="L31">
+        <v>611404</v>
+      </c>
     </row>
     <row r="32" spans="2:12" ht="19" x14ac:dyDescent="0.25">
       <c r="B32" s="36" t="s">
@@ -1796,21 +1918,21 @@
       <c r="C32" s="27">
         <v>11244</v>
       </c>
-      <c r="D32" s="58">
+      <c r="D32" s="56">
         <f>C32/$C$30</f>
         <v>0.59385232914334007</v>
       </c>
       <c r="E32" s="27">
         <v>69262</v>
       </c>
-      <c r="F32" s="58">
+      <c r="F32" s="56">
         <f>E32/$E$30</f>
         <v>0.6480897530667814</v>
       </c>
       <c r="G32" s="27">
         <v>313546</v>
       </c>
-      <c r="H32" s="58">
+      <c r="H32" s="56">
         <f>G32/$G$30</f>
         <v>0.67313583756083628</v>
       </c>
@@ -1825,21 +1947,21 @@
       <c r="C33" s="27">
         <v>6340</v>
       </c>
-      <c r="D33" s="58">
+      <c r="D33" s="56">
         <f t="shared" ref="D33:D35" si="7">C33/$C$30</f>
         <v>0.33484736452941799</v>
       </c>
       <c r="E33" s="27">
         <v>30130</v>
       </c>
-      <c r="F33" s="58">
+      <c r="F33" s="56">
         <f t="shared" ref="F33:F35" si="8">E33/$E$30</f>
         <v>0.28192868037166302</v>
       </c>
       <c r="G33" s="27">
         <v>111647</v>
       </c>
-      <c r="H33" s="58">
+      <c r="H33" s="56">
         <f t="shared" ref="H33:H35" si="9">G33/$G$30</f>
         <v>0.23968922217523009</v>
       </c>
@@ -1854,21 +1976,21 @@
       <c r="C34" s="27">
         <v>5673</v>
       </c>
-      <c r="D34" s="58">
+      <c r="D34" s="56">
         <f t="shared" si="7"/>
         <v>0.29961973169958805</v>
       </c>
       <c r="E34" s="27">
         <v>25191</v>
       </c>
-      <c r="F34" s="58">
+      <c r="F34" s="56">
         <f t="shared" si="8"/>
         <v>0.23571408520552817</v>
       </c>
       <c r="G34" s="27">
         <v>92192</v>
       </c>
-      <c r="H34" s="58">
+      <c r="H34" s="56">
         <f t="shared" si="9"/>
         <v>0.19792227978162255</v>
       </c>
@@ -1880,21 +2002,21 @@
       <c r="C35" s="27">
         <v>667</v>
       </c>
-      <c r="D35" s="58">
+      <c r="D35" s="56">
         <f t="shared" si="7"/>
         <v>3.5227632829829936E-2</v>
       </c>
       <c r="E35" s="27">
         <v>4939</v>
       </c>
-      <c r="F35" s="58">
+      <c r="F35" s="56">
         <f t="shared" si="8"/>
         <v>4.6214595166134874E-2</v>
       </c>
       <c r="G35" s="27">
         <v>19455</v>
       </c>
-      <c r="H35" s="58">
+      <c r="H35" s="56">
         <f t="shared" si="9"/>
         <v>4.1766942393607544E-2</v>
       </c>
@@ -1929,21 +2051,21 @@
       <c r="C37" s="27">
         <v>3399</v>
       </c>
-      <c r="D37" s="58">
+      <c r="D37" s="56">
         <f>C37/$C$39</f>
         <v>0.5541245516791653</v>
       </c>
       <c r="E37" s="27">
         <v>25699</v>
       </c>
-      <c r="F37" s="58">
+      <c r="F37" s="56">
         <f>E37/$E$39</f>
         <v>0.60093534432362916</v>
       </c>
       <c r="G37" s="27">
         <v>59488</v>
       </c>
-      <c r="H37" s="58">
+      <c r="H37" s="56">
         <f>G37/$G$39</f>
         <v>0.4085573984409876</v>
       </c>
@@ -1955,21 +2077,21 @@
       <c r="C38" s="27">
         <v>2735</v>
       </c>
-      <c r="D38" s="58">
+      <c r="D38" s="56">
         <f t="shared" ref="D38:D44" si="10">C38/$C$39</f>
         <v>0.4458754483208347</v>
       </c>
       <c r="E38" s="27">
         <v>17066</v>
       </c>
-      <c r="F38" s="58">
+      <c r="F38" s="56">
         <f t="shared" ref="F38:F44" si="11">E38/$E$39</f>
         <v>0.39906465567637084</v>
       </c>
       <c r="G38" s="27">
         <v>86117</v>
       </c>
-      <c r="H38" s="58">
+      <c r="H38" s="56">
         <f t="shared" ref="H38:H44" si="12">G38/$G$39</f>
         <v>0.5914426015590124</v>
       </c>
@@ -1982,21 +2104,24 @@
         <f>SUM(C37:C38)</f>
         <v>6134</v>
       </c>
-      <c r="D39" s="63" t="s">
-        <v>12</v>
+      <c r="D39" s="60">
+        <f>C39/L29</f>
+        <v>0.2446944311472794</v>
       </c>
       <c r="E39" s="27">
         <f t="shared" ref="E39" si="13">SUM(E37:E38)</f>
         <v>42765</v>
       </c>
-      <c r="F39" s="63" t="s">
-        <v>12</v>
+      <c r="F39" s="60">
+        <f>E39/L30</f>
+        <v>0.28579352562217647</v>
       </c>
       <c r="G39" s="27">
         <v>145605</v>
       </c>
-      <c r="H39" s="63" t="s">
-        <v>12</v>
+      <c r="H39" s="60">
+        <f>G39/L31</f>
+        <v>0.23814858914890971</v>
       </c>
     </row>
     <row r="40" spans="2:12" ht="17" x14ac:dyDescent="0.2">
@@ -2004,11 +2129,11 @@
         <v>23</v>
       </c>
       <c r="C40" s="30"/>
-      <c r="D40" s="58"/>
+      <c r="D40" s="56"/>
       <c r="E40" s="30"/>
-      <c r="F40" s="58"/>
+      <c r="F40" s="56"/>
       <c r="G40" s="30"/>
-      <c r="H40" s="58"/>
+      <c r="H40" s="56"/>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B41" s="36" t="s">
@@ -2017,21 +2142,21 @@
       <c r="C41" s="27">
         <v>933</v>
       </c>
-      <c r="D41" s="58">
+      <c r="D41" s="56">
         <f t="shared" si="10"/>
         <v>0.1521030322791001</v>
       </c>
       <c r="E41" s="27">
         <v>6348</v>
       </c>
-      <c r="F41" s="58">
+      <c r="F41" s="56">
         <f t="shared" si="11"/>
         <v>0.14843914415994389</v>
       </c>
       <c r="G41" s="27">
         <v>27519</v>
       </c>
-      <c r="H41" s="58">
+      <c r="H41" s="56">
         <f t="shared" si="12"/>
         <v>0.18899763057587307</v>
       </c>
@@ -2043,21 +2168,21 @@
       <c r="C42" s="27">
         <v>5201</v>
       </c>
-      <c r="D42" s="58">
+      <c r="D42" s="56">
         <f t="shared" si="10"/>
         <v>0.84789696772089995</v>
       </c>
       <c r="E42" s="27">
         <v>36065</v>
       </c>
-      <c r="F42" s="58">
+      <c r="F42" s="56">
         <f t="shared" si="11"/>
         <v>0.84332982579211968</v>
       </c>
       <c r="G42" s="27">
         <v>116191</v>
       </c>
-      <c r="H42" s="58">
+      <c r="H42" s="56">
         <f t="shared" si="12"/>
         <v>0.79798770646612416</v>
       </c>
@@ -2069,21 +2194,21 @@
       <c r="C43" s="27">
         <v>3413</v>
       </c>
-      <c r="D43" s="58">
+      <c r="D43" s="56">
         <f t="shared" si="10"/>
         <v>0.55640691229214212</v>
       </c>
       <c r="E43" s="27">
         <v>23906</v>
       </c>
-      <c r="F43" s="58">
+      <c r="F43" s="56">
         <f t="shared" si="11"/>
         <v>0.55900853501695313</v>
       </c>
       <c r="G43" s="27">
         <v>64122</v>
       </c>
-      <c r="H43" s="58">
+      <c r="H43" s="56">
         <f t="shared" si="12"/>
         <v>0.44038322859791901</v>
       </c>
@@ -2095,21 +2220,21 @@
       <c r="C44" s="33">
         <v>1788</v>
       </c>
-      <c r="D44" s="60">
+      <c r="D44" s="57">
         <f t="shared" si="10"/>
         <v>0.29149005542875772</v>
       </c>
       <c r="E44" s="33">
         <v>12159</v>
       </c>
-      <c r="F44" s="60">
+      <c r="F44" s="57">
         <f t="shared" si="11"/>
         <v>0.2843212907751666</v>
       </c>
       <c r="G44" s="33">
         <v>52069</v>
       </c>
-      <c r="H44" s="60">
+      <c r="H44" s="57">
         <f t="shared" si="12"/>
         <v>0.3576044778682051</v>
       </c>
@@ -2137,10 +2262,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56457F3-9383-224C-A08C-7C956A652AA7}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:F5"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2155,43 +2280,43 @@
   <sheetData>
     <row r="1" spans="2:12" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:12" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="74"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="71"/>
     </row>
     <row r="3" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
     </row>
     <row r="4" spans="2:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="71"/>
-      <c r="C4" s="75" t="s">
+      <c r="B4" s="68"/>
+      <c r="C4" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="76"/>
-      <c r="E4" s="77" t="s">
+      <c r="D4" s="73"/>
+      <c r="E4" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="76"/>
-      <c r="G4" s="75" t="s">
+      <c r="F4" s="73"/>
+      <c r="G4" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="76"/>
+      <c r="H4" s="73"/>
     </row>
     <row r="5" spans="2:12" ht="43" x14ac:dyDescent="0.2">
       <c r="B5" s="39" t="s">
@@ -2223,20 +2348,23 @@
       <c r="C6" s="27">
         <v>101232</v>
       </c>
-      <c r="D6" s="57" t="s">
-        <v>12</v>
+      <c r="D6" s="60">
+        <f>C6/C24</f>
+        <v>0.30647666276123264</v>
       </c>
       <c r="E6" s="27">
         <v>452279</v>
       </c>
-      <c r="F6" s="57" t="s">
-        <v>12</v>
+      <c r="F6" s="60">
+        <f>E6/C25</f>
+        <v>0.31948188270663097</v>
       </c>
       <c r="G6" s="27">
         <v>6384997</v>
       </c>
-      <c r="H6" s="57" t="s">
-        <v>12</v>
+      <c r="H6" s="60">
+        <f>G6/C26</f>
+        <v>0.34660312761564022</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="17" x14ac:dyDescent="0.2">
@@ -2257,21 +2385,21 @@
       <c r="C8" s="27">
         <v>36276</v>
       </c>
-      <c r="D8" s="58">
+      <c r="D8" s="56">
         <f>C8/$C$6</f>
         <v>0.35834518729255571</v>
       </c>
       <c r="E8" s="27">
         <v>178909</v>
       </c>
-      <c r="F8" s="58">
+      <c r="F8" s="56">
         <f>E8/$E$6</f>
         <v>0.39557220211418176</v>
       </c>
       <c r="G8" s="27">
         <v>3006846</v>
       </c>
-      <c r="H8" s="58">
+      <c r="H8" s="56">
         <f>G8/$G$6</f>
         <v>0.4709236355161952</v>
       </c>
@@ -2286,21 +2414,21 @@
       <c r="C9" s="27">
         <v>47672</v>
       </c>
-      <c r="D9" s="58">
+      <c r="D9" s="56">
         <f t="shared" ref="D9:D11" si="0">C9/$C$6</f>
         <v>0.47091828670776037</v>
       </c>
       <c r="E9" s="27">
         <v>191522</v>
       </c>
-      <c r="F9" s="58">
+      <c r="F9" s="56">
         <f t="shared" ref="F9:F11" si="1">E9/$E$6</f>
         <v>0.42345985553165194</v>
       </c>
       <c r="G9" s="27">
         <v>2452956</v>
       </c>
-      <c r="H9" s="58">
+      <c r="H9" s="56">
         <f t="shared" ref="H9:H11" si="2">G9/$G$6</f>
         <v>0.38417496515660071</v>
       </c>
@@ -2315,21 +2443,21 @@
       <c r="C10" s="27">
         <v>40833</v>
       </c>
-      <c r="D10" s="58">
+      <c r="D10" s="56">
         <f t="shared" si="0"/>
         <v>0.40336059743954483</v>
       </c>
       <c r="E10" s="27">
         <v>165329</v>
       </c>
-      <c r="F10" s="58">
+      <c r="F10" s="56">
         <f t="shared" si="1"/>
         <v>0.3655464878979568</v>
       </c>
       <c r="G10" s="27">
         <v>2058825</v>
       </c>
-      <c r="H10" s="58">
+      <c r="H10" s="56">
         <f t="shared" si="2"/>
         <v>0.32244729324070159</v>
       </c>
@@ -2344,21 +2472,21 @@
       <c r="C11" s="27">
         <v>6839</v>
       </c>
-      <c r="D11" s="58">
+      <c r="D11" s="56">
         <f t="shared" si="0"/>
         <v>6.7557689268215579E-2</v>
       </c>
       <c r="E11" s="27">
         <v>26193</v>
       </c>
-      <c r="F11" s="58">
+      <c r="F11" s="56">
         <f t="shared" si="1"/>
         <v>5.7913367633695131E-2</v>
       </c>
       <c r="G11" s="27">
         <v>394131</v>
       </c>
-      <c r="H11" s="58">
+      <c r="H11" s="56">
         <f t="shared" si="2"/>
         <v>6.1727671915899097E-2</v>
       </c>
@@ -2399,21 +2527,21 @@
       <c r="C13" s="27">
         <v>135733</v>
       </c>
-      <c r="D13" s="58">
+      <c r="D13" s="56">
         <f>C13/$C$15</f>
         <v>0.59252129196732972</v>
       </c>
       <c r="E13" s="27">
         <v>533001</v>
       </c>
-      <c r="F13" s="58">
+      <c r="F13" s="56">
         <f>E13/$E$15</f>
         <v>0.55325856225704162</v>
       </c>
       <c r="G13" s="27">
         <v>7100074</v>
       </c>
-      <c r="H13" s="58">
+      <c r="H13" s="56">
         <f>G13/$G$15</f>
         <v>0.58987175823153304</v>
       </c>
@@ -2425,21 +2553,21 @@
       <c r="C14" s="27">
         <v>93344</v>
       </c>
-      <c r="D14" s="58">
+      <c r="D14" s="56">
         <f t="shared" ref="D14:D20" si="3">C14/$C$15</f>
         <v>0.40747870803267022</v>
       </c>
       <c r="E14" s="27">
         <v>430384</v>
       </c>
-      <c r="F14" s="58">
+      <c r="F14" s="56">
         <f t="shared" ref="F14:F20" si="4">E14/$E$15</f>
         <v>0.44674143774295844</v>
       </c>
       <c r="G14" s="27">
         <v>4936566</v>
       </c>
-      <c r="H14" s="58">
+      <c r="H14" s="56">
         <f t="shared" ref="H14:H20" si="5">G14/$G$15</f>
         <v>0.41012824176846696</v>
       </c>
@@ -2452,21 +2580,24 @@
         <f>SUM(C13:C14)</f>
         <v>229077</v>
       </c>
-      <c r="D15" s="63" t="s">
-        <v>12</v>
+      <c r="D15" s="60">
+        <f>C15/C24</f>
+        <v>0.69352333723876736</v>
       </c>
       <c r="E15" s="27">
         <f t="shared" ref="E15" si="6">SUM(E13:E14)</f>
         <v>963385</v>
       </c>
-      <c r="F15" s="63" t="s">
-        <v>12</v>
+      <c r="F15" s="60">
+        <f>E15/C25</f>
+        <v>0.68051811729336908</v>
       </c>
       <c r="G15" s="27">
         <v>12036640</v>
       </c>
-      <c r="H15" s="63" t="s">
-        <v>12</v>
+      <c r="H15" s="60">
+        <f>G15/C26</f>
+        <v>0.65339687238435973</v>
       </c>
     </row>
     <row r="16" spans="2:12" ht="17" x14ac:dyDescent="0.2">
@@ -2474,11 +2605,11 @@
         <v>23</v>
       </c>
       <c r="C16" s="27"/>
-      <c r="D16" s="58"/>
+      <c r="D16" s="56"/>
       <c r="E16" s="27"/>
-      <c r="F16" s="58"/>
+      <c r="F16" s="56"/>
       <c r="G16" s="27"/>
-      <c r="H16" s="58"/>
+      <c r="H16" s="56"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" s="36" t="s">
@@ -2487,21 +2618,21 @@
       <c r="C17" s="27">
         <v>22501</v>
       </c>
-      <c r="D17" s="58">
+      <c r="D17" s="56">
         <f t="shared" si="3"/>
         <v>9.8224614430955537E-2</v>
       </c>
       <c r="E17" s="27">
         <v>106935</v>
       </c>
-      <c r="F17" s="58">
+      <c r="F17" s="56">
         <f t="shared" si="4"/>
         <v>0.1109992370651401</v>
       </c>
       <c r="G17" s="27">
         <v>1552111</v>
       </c>
-      <c r="H17" s="58">
+      <c r="H17" s="56">
         <f t="shared" si="5"/>
         <v>0.12894885948238047</v>
       </c>
@@ -2513,21 +2644,21 @@
       <c r="C18" s="27">
         <v>203938</v>
       </c>
-      <c r="D18" s="58">
+      <c r="D18" s="56">
         <f t="shared" si="3"/>
         <v>0.89025960703169682</v>
       </c>
       <c r="E18" s="27">
         <v>845893</v>
       </c>
-      <c r="F18" s="58">
+      <c r="F18" s="56">
         <f t="shared" si="4"/>
         <v>0.87804252713089781</v>
       </c>
       <c r="G18" s="27">
         <v>10383822</v>
       </c>
-      <c r="H18" s="58">
+      <c r="H18" s="56">
         <f t="shared" si="5"/>
         <v>0.86268443685280938</v>
       </c>
@@ -2539,21 +2670,21 @@
       <c r="C19" s="27">
         <v>98551</v>
       </c>
-      <c r="D19" s="58">
+      <c r="D19" s="56">
         <f t="shared" si="3"/>
         <v>0.43020905634350021</v>
       </c>
       <c r="E19" s="27">
         <v>466614</v>
       </c>
-      <c r="F19" s="58">
+      <c r="F19" s="56">
         <f t="shared" si="4"/>
         <v>0.48434841729941819</v>
       </c>
       <c r="G19" s="27">
         <v>5231985</v>
       </c>
-      <c r="H19" s="58">
+      <c r="H19" s="56">
         <f t="shared" si="5"/>
         <v>0.43467155285860504</v>
       </c>
@@ -2565,26 +2696,55 @@
       <c r="C20" s="33">
         <v>105387</v>
       </c>
-      <c r="D20" s="60">
+      <c r="D20" s="57">
         <f t="shared" si="3"/>
         <v>0.46005055068819656</v>
       </c>
       <c r="E20" s="33">
         <v>379279</v>
       </c>
-      <c r="F20" s="60">
+      <c r="F20" s="57">
         <f t="shared" si="4"/>
         <v>0.39369410983147962</v>
       </c>
       <c r="G20" s="33">
         <v>5151837</v>
       </c>
-      <c r="H20" s="60">
+      <c r="H20" s="57">
         <f t="shared" si="5"/>
         <v>0.42801288399420434</v>
       </c>
     </row>
     <row r="21" spans="2:8" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24">
+        <v>330309</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25">
+        <v>1415664</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26">
+        <v>18421637</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="E4:F4"/>
@@ -2600,10 +2760,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4AA3A1D-E334-D84D-9200-08BB50724BC1}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2618,43 +2778,43 @@
   <sheetData>
     <row r="1" spans="2:12" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:12" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="74"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="71"/>
     </row>
     <row r="3" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
     </row>
     <row r="4" spans="2:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="71"/>
-      <c r="C4" s="75" t="s">
+      <c r="B4" s="68"/>
+      <c r="C4" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="76"/>
-      <c r="E4" s="75" t="s">
+      <c r="D4" s="73"/>
+      <c r="E4" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="76"/>
-      <c r="G4" s="75" t="s">
+      <c r="F4" s="73"/>
+      <c r="G4" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="76"/>
+      <c r="H4" s="73"/>
     </row>
     <row r="5" spans="2:12" ht="43" x14ac:dyDescent="0.2">
       <c r="B5" s="39" t="s">
@@ -2686,20 +2846,23 @@
       <c r="C6" s="27">
         <v>134861</v>
       </c>
-      <c r="D6" s="57" t="s">
-        <v>12</v>
+      <c r="D6" s="60">
+        <f>C6/C24</f>
+        <v>0.33047848695592508</v>
       </c>
       <c r="E6" s="27">
         <v>227055</v>
       </c>
-      <c r="F6" s="57" t="s">
-        <v>12</v>
+      <c r="F6" s="60">
+        <f>E6/C25</f>
+        <v>0.34251669175835947</v>
       </c>
       <c r="G6" s="27">
         <v>6384997</v>
       </c>
-      <c r="H6" s="57" t="s">
-        <v>12</v>
+      <c r="H6" s="60">
+        <f>G6/C26</f>
+        <v>0.34660312761564022</v>
       </c>
       <c r="J6" s="42"/>
       <c r="K6" s="42"/>
@@ -2726,21 +2889,21 @@
       <c r="C8" s="27">
         <v>68022</v>
       </c>
-      <c r="D8" s="58">
+      <c r="D8" s="56">
         <f>C8/$C$6</f>
         <v>0.50438599743439538</v>
       </c>
       <c r="E8" s="27">
         <v>118071</v>
       </c>
-      <c r="F8" s="58">
+      <c r="F8" s="56">
         <f>E8/$E$6</f>
         <v>0.5200105701261809</v>
       </c>
       <c r="G8" s="27">
         <v>3006846</v>
       </c>
-      <c r="H8" s="58">
+      <c r="H8" s="56">
         <f>G8/$G$6</f>
         <v>0.4709236355161952</v>
       </c>
@@ -2755,21 +2918,21 @@
       <c r="C9" s="27">
         <v>47128</v>
       </c>
-      <c r="D9" s="58">
+      <c r="D9" s="56">
         <f t="shared" ref="D9:D11" si="0">C9/$C$6</f>
         <v>0.34945610665796634</v>
       </c>
       <c r="E9" s="27">
         <v>78470</v>
       </c>
-      <c r="F9" s="58">
+      <c r="F9" s="56">
         <f t="shared" ref="F9:F11" si="1">E9/$E$6</f>
         <v>0.34559908392239763</v>
       </c>
       <c r="G9" s="27">
         <v>2452956</v>
       </c>
-      <c r="H9" s="58">
+      <c r="H9" s="56">
         <f t="shared" ref="H9:H11" si="2">G9/$G$6</f>
         <v>0.38417496515660071</v>
       </c>
@@ -2784,21 +2947,21 @@
       <c r="C10" s="27">
         <v>39953</v>
       </c>
-      <c r="D10" s="58">
+      <c r="D10" s="56">
         <f t="shared" si="0"/>
         <v>0.29625317919932376</v>
       </c>
       <c r="E10" s="27">
         <v>66322</v>
       </c>
-      <c r="F10" s="58">
+      <c r="F10" s="56">
         <f t="shared" si="1"/>
         <v>0.29209662857017021</v>
       </c>
       <c r="G10" s="27">
         <v>2058825</v>
       </c>
-      <c r="H10" s="58">
+      <c r="H10" s="56">
         <f t="shared" si="2"/>
         <v>0.32244729324070159</v>
       </c>
@@ -2813,21 +2976,21 @@
       <c r="C11" s="27">
         <v>7175</v>
       </c>
-      <c r="D11" s="58">
+      <c r="D11" s="56">
         <f t="shared" si="0"/>
         <v>5.32029274586426E-2</v>
       </c>
       <c r="E11" s="27">
         <v>12148</v>
       </c>
-      <c r="F11" s="58">
+      <c r="F11" s="56">
         <f t="shared" si="1"/>
         <v>5.3502455352227432E-2</v>
       </c>
       <c r="G11" s="27">
         <v>394131</v>
       </c>
-      <c r="H11" s="58">
+      <c r="H11" s="56">
         <f t="shared" si="2"/>
         <v>6.1727671915899097E-2</v>
       </c>
@@ -2868,21 +3031,21 @@
       <c r="C13" s="27">
         <v>135374</v>
       </c>
-      <c r="D13" s="58">
+      <c r="D13" s="56">
         <f>C13/$C$15</f>
         <v>0.49548161351599646</v>
       </c>
       <c r="E13" s="27">
         <v>237278</v>
       </c>
-      <c r="F13" s="58">
+      <c r="F13" s="56">
         <f>E13/$E$15</f>
         <v>0.54440663810924472</v>
       </c>
       <c r="G13" s="27">
         <v>7100074</v>
       </c>
-      <c r="H13" s="58">
+      <c r="H13" s="56">
         <f>G13/$G$15</f>
         <v>0.58987175823153304</v>
       </c>
@@ -2894,21 +3057,21 @@
       <c r="C14" s="27">
         <v>137843</v>
       </c>
-      <c r="D14" s="58">
+      <c r="D14" s="56">
         <f t="shared" ref="D14:D20" si="3">C14/$C$15</f>
         <v>0.5045183864840036</v>
       </c>
       <c r="E14" s="27">
         <v>198569</v>
       </c>
-      <c r="F14" s="58">
+      <c r="F14" s="56">
         <f t="shared" ref="F14:F20" si="4">E14/$E$15</f>
         <v>0.45559336189075522</v>
       </c>
       <c r="G14" s="27">
         <v>4936566</v>
       </c>
-      <c r="H14" s="58">
+      <c r="H14" s="56">
         <f t="shared" ref="H14:H20" si="5">G14/$G$15</f>
         <v>0.41012824176846696</v>
       </c>
@@ -2921,21 +3084,24 @@
         <f>SUM(C13:C14)</f>
         <v>273217</v>
       </c>
-      <c r="D15" s="63" t="s">
-        <v>12</v>
+      <c r="D15" s="60">
+        <f>C15/C24</f>
+        <v>0.66952151304407492</v>
       </c>
       <c r="E15" s="27">
         <f>SUM(E13:E14)</f>
         <v>435847</v>
       </c>
-      <c r="F15" s="63" t="s">
-        <v>12</v>
+      <c r="F15" s="60">
+        <f>E15/C25</f>
+        <v>0.65748330824164058</v>
       </c>
       <c r="G15" s="27">
         <v>12036640</v>
       </c>
-      <c r="H15" s="63" t="s">
-        <v>12</v>
+      <c r="H15" s="60">
+        <f>G15/C26</f>
+        <v>0.65339687238435973</v>
       </c>
     </row>
     <row r="16" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -2943,11 +3109,11 @@
         <v>23</v>
       </c>
       <c r="C16" s="27"/>
-      <c r="D16" s="58"/>
+      <c r="D16" s="56"/>
       <c r="E16" s="27"/>
-      <c r="F16" s="58"/>
+      <c r="F16" s="56"/>
       <c r="G16" s="27"/>
-      <c r="H16" s="58"/>
+      <c r="H16" s="56"/>
     </row>
     <row r="17" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="36" t="s">
@@ -2956,21 +3122,21 @@
       <c r="C17" s="27">
         <v>34045</v>
       </c>
-      <c r="D17" s="58">
+      <c r="D17" s="56">
         <f t="shared" si="3"/>
         <v>0.12460791239198146</v>
       </c>
       <c r="E17" s="27">
         <v>59266</v>
       </c>
-      <c r="F17" s="58">
+      <c r="F17" s="56">
         <f t="shared" si="4"/>
         <v>0.1359789100303547</v>
       </c>
       <c r="G17" s="27">
         <v>1552111</v>
       </c>
-      <c r="H17" s="58">
+      <c r="H17" s="56">
         <f t="shared" si="5"/>
         <v>0.12894885948238047</v>
       </c>
@@ -2982,21 +3148,21 @@
       <c r="C18" s="27">
         <v>236519</v>
       </c>
-      <c r="D18" s="58">
+      <c r="D18" s="56">
         <f t="shared" si="3"/>
         <v>0.86568185727828062</v>
       </c>
       <c r="E18" s="27">
         <v>373041</v>
       </c>
-      <c r="F18" s="58">
+      <c r="F18" s="56">
         <f t="shared" si="4"/>
         <v>0.85589897372243007</v>
       </c>
       <c r="G18" s="27">
         <v>10383822</v>
       </c>
-      <c r="H18" s="58">
+      <c r="H18" s="56">
         <f t="shared" si="5"/>
         <v>0.86268443685280938</v>
       </c>
@@ -3008,21 +3174,21 @@
       <c r="C19" s="27">
         <v>127154</v>
       </c>
-      <c r="D19" s="58">
+      <c r="D19" s="56">
         <f t="shared" si="3"/>
         <v>0.46539563789954502</v>
       </c>
       <c r="E19" s="27">
         <v>192966</v>
       </c>
-      <c r="F19" s="58">
+      <c r="F19" s="56">
         <f t="shared" si="4"/>
         <v>0.44273793326557254</v>
       </c>
       <c r="G19" s="27">
         <v>5231985</v>
       </c>
-      <c r="H19" s="58">
+      <c r="H19" s="56">
         <f t="shared" si="5"/>
         <v>0.43467155285860504</v>
       </c>
@@ -3034,26 +3200,50 @@
       <c r="C20" s="33">
         <v>109365</v>
       </c>
-      <c r="D20" s="60">
+      <c r="D20" s="57">
         <f t="shared" si="3"/>
         <v>0.4002862193787356</v>
       </c>
       <c r="E20" s="33">
         <v>180075</v>
       </c>
-      <c r="F20" s="60">
+      <c r="F20" s="57">
         <f t="shared" si="4"/>
         <v>0.41316104045685759</v>
       </c>
       <c r="G20" s="33">
         <v>5151837</v>
       </c>
-      <c r="H20" s="60">
+      <c r="H20" s="57">
         <f t="shared" si="5"/>
         <v>0.42801288399420434</v>
       </c>
     </row>
     <row r="21" spans="2:8" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24">
+        <v>408078</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25">
+        <v>662902</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26">
+        <v>18421637</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B2:H2"/>
@@ -3069,10 +3259,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55AFC039-7414-7645-9812-2C75554B8DE7}">
-  <dimension ref="A1:V21"/>
+  <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3102,92 +3292,92 @@
   <sheetData>
     <row r="1" spans="2:22" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:22" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="74"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="70"/>
+      <c r="R2" s="71"/>
     </row>
     <row r="3" spans="2:22" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-      <c r="L3" s="69"/>
-      <c r="M3" s="69"/>
-      <c r="N3" s="69"/>
-      <c r="O3" s="69"/>
-      <c r="P3" s="69"/>
-      <c r="Q3" s="69"/>
-      <c r="R3" s="69"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="66"/>
+      <c r="L3" s="66"/>
+      <c r="M3" s="66"/>
+      <c r="N3" s="66"/>
+      <c r="O3" s="66"/>
+      <c r="P3" s="66"/>
+      <c r="Q3" s="66"/>
+      <c r="R3" s="66"/>
     </row>
     <row r="4" spans="2:22" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="71"/>
-      <c r="C4" s="78" t="s">
+      <c r="B4" s="68"/>
+      <c r="C4" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="79"/>
-      <c r="E4" s="78" t="s">
+      <c r="D4" s="76"/>
+      <c r="E4" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="80"/>
-      <c r="G4" s="78" t="s">
+      <c r="F4" s="77"/>
+      <c r="G4" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="80"/>
-      <c r="I4" s="78" t="s">
+      <c r="H4" s="77"/>
+      <c r="I4" s="75" t="s">
         <v>45</v>
       </c>
-      <c r="J4" s="80"/>
-      <c r="K4" s="78" t="s">
+      <c r="J4" s="77"/>
+      <c r="K4" s="75" t="s">
         <v>46</v>
       </c>
-      <c r="L4" s="80"/>
-      <c r="M4" s="75" t="s">
+      <c r="L4" s="77"/>
+      <c r="M4" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="N4" s="76"/>
-      <c r="O4" s="75" t="s">
+      <c r="N4" s="73"/>
+      <c r="O4" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="P4" s="76"/>
-      <c r="Q4" s="77" t="s">
+      <c r="P4" s="73"/>
+      <c r="Q4" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="76"/>
+      <c r="R4" s="73"/>
     </row>
     <row r="5" spans="2:22" ht="43" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="65" t="s">
+      <c r="C5" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="66" t="s">
+      <c r="D5" s="63" t="s">
         <v>48</v>
       </c>
       <c r="E5" s="51" t="s">
@@ -3226,10 +3416,10 @@
       <c r="P5" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="Q5" s="65" t="s">
+      <c r="Q5" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="R5" s="56" t="s">
+      <c r="R5" s="55" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3240,50 +3430,58 @@
       <c r="C6" s="28">
         <v>17760</v>
       </c>
-      <c r="D6" s="54" t="s">
-        <v>12</v>
+      <c r="D6" s="54">
+        <f>C6/C24</f>
+        <v>0.32079765904410967</v>
       </c>
       <c r="E6" s="27">
         <v>101637</v>
       </c>
-      <c r="F6" s="57" t="s">
-        <v>12</v>
+      <c r="F6" s="60">
+        <f>E6/C25</f>
+        <v>0.33134468492963121</v>
       </c>
       <c r="G6" s="27">
         <v>67929</v>
       </c>
-      <c r="H6" s="59" t="s">
-        <v>12</v>
+      <c r="H6" s="96">
+        <f>G6/C26</f>
+        <v>0.34190499199710084</v>
       </c>
       <c r="I6" s="27">
         <v>15142</v>
       </c>
-      <c r="J6" s="57" t="s">
-        <v>12</v>
+      <c r="J6" s="60">
+        <f>I6/C27</f>
+        <v>0.31807583237054932</v>
       </c>
       <c r="K6" s="27">
         <v>162098</v>
       </c>
-      <c r="L6" s="57" t="s">
-        <v>12</v>
+      <c r="L6" s="60">
+        <f>K6/C28</f>
+        <v>0.27526724686902992</v>
       </c>
       <c r="M6" s="27">
         <v>364566</v>
       </c>
-      <c r="N6" s="57" t="s">
-        <v>12</v>
+      <c r="N6" s="60">
+        <f>M6/C29</f>
+        <v>0.30450002129861409</v>
       </c>
       <c r="O6" s="27">
         <v>522851</v>
       </c>
-      <c r="P6" s="57" t="s">
-        <v>12</v>
+      <c r="P6" s="60">
+        <f>O6/C30</f>
+        <v>0.31229602393000666</v>
       </c>
       <c r="Q6" s="28">
         <v>6384997</v>
       </c>
-      <c r="R6" s="59" t="s">
-        <v>12</v>
+      <c r="R6" s="96">
+        <f>Q6/C31</f>
+        <v>0.34660312761564022</v>
       </c>
       <c r="T6" s="42"/>
       <c r="U6" s="42"/>
@@ -3328,49 +3526,49 @@
       <c r="E8" s="27">
         <v>26353</v>
       </c>
-      <c r="F8" s="58">
+      <c r="F8" s="56">
         <f>E8/$E$6</f>
         <v>0.25928549642354654</v>
       </c>
       <c r="G8" s="27">
         <v>33061</v>
       </c>
-      <c r="H8" s="58">
+      <c r="H8" s="56">
         <f>G8/$G$6</f>
         <v>0.48669934784848884</v>
       </c>
       <c r="I8" s="27">
         <v>5356</v>
       </c>
-      <c r="J8" s="58">
+      <c r="J8" s="56">
         <f>I8/$I$6</f>
         <v>0.35371813498877297</v>
       </c>
       <c r="K8" s="27">
         <v>46567</v>
       </c>
-      <c r="L8" s="58">
+      <c r="L8" s="56">
         <f>K8/$K$6</f>
         <v>0.28727683253340569</v>
       </c>
       <c r="M8" s="27">
         <v>117157</v>
       </c>
-      <c r="N8" s="58">
+      <c r="N8" s="56">
         <f>M8/$M$6</f>
         <v>0.3213601926674457</v>
       </c>
       <c r="O8" s="27">
         <v>182826</v>
       </c>
-      <c r="P8" s="58">
+      <c r="P8" s="56">
         <f>O8/$O$6</f>
         <v>0.34967132127508604</v>
       </c>
       <c r="Q8" s="28">
         <v>3006846</v>
       </c>
-      <c r="R8" s="58">
+      <c r="R8" s="56">
         <f>Q8/$Q$6</f>
         <v>0.4709236355161952</v>
       </c>
@@ -3393,49 +3591,49 @@
       <c r="E9" s="27">
         <v>55962</v>
       </c>
-      <c r="F9" s="58">
+      <c r="F9" s="56">
         <f t="shared" ref="F9:F10" si="1">E9/$E$6</f>
         <v>0.55060657044186667</v>
       </c>
       <c r="G9" s="27">
         <v>28528</v>
       </c>
-      <c r="H9" s="58">
+      <c r="H9" s="56">
         <f t="shared" ref="H9:H11" si="2">G9/$G$6</f>
         <v>0.41996790766830072</v>
       </c>
       <c r="I9" s="27">
         <v>7322</v>
       </c>
-      <c r="J9" s="58">
+      <c r="J9" s="56">
         <f t="shared" ref="J9:J11" si="3">I9/$I$6</f>
         <v>0.48355567296262053</v>
       </c>
       <c r="K9" s="27">
         <v>80764</v>
       </c>
-      <c r="L9" s="58">
+      <c r="L9" s="56">
         <f t="shared" ref="L9:L11" si="4">K9/$K$6</f>
         <v>0.49824180434058407</v>
       </c>
       <c r="M9" s="27">
         <v>180979</v>
       </c>
-      <c r="N9" s="58">
+      <c r="N9" s="56">
         <f t="shared" ref="N9:N11" si="5">M9/$M$6</f>
         <v>0.49642314423177147</v>
       </c>
       <c r="O9" s="27">
         <v>248550</v>
       </c>
-      <c r="P9" s="58">
+      <c r="P9" s="56">
         <f t="shared" ref="P9:P11" si="6">O9/$O$6</f>
         <v>0.47537443745923791</v>
       </c>
       <c r="Q9" s="28">
         <v>2452956</v>
       </c>
-      <c r="R9" s="58">
+      <c r="R9" s="56">
         <f t="shared" ref="R9:R11" si="7">Q9/$Q$6</f>
         <v>0.38417496515660071</v>
       </c>
@@ -3458,49 +3656,49 @@
       <c r="E10" s="27">
         <v>43837</v>
       </c>
-      <c r="F10" s="58">
+      <c r="F10" s="56">
         <f t="shared" si="1"/>
         <v>0.43130946407312298</v>
       </c>
       <c r="G10" s="27">
         <v>24866</v>
       </c>
-      <c r="H10" s="58">
+      <c r="H10" s="56">
         <f t="shared" si="2"/>
         <v>0.36605867891474925</v>
       </c>
       <c r="I10" s="27">
         <v>5810</v>
       </c>
-      <c r="J10" s="58">
+      <c r="J10" s="56">
         <f t="shared" si="3"/>
         <v>0.38370096420552108</v>
       </c>
       <c r="K10" s="27">
         <v>63324</v>
       </c>
-      <c r="L10" s="58">
+      <c r="L10" s="56">
         <f t="shared" si="4"/>
         <v>0.39065256819948424</v>
       </c>
       <c r="M10" s="27">
         <v>144321</v>
       </c>
-      <c r="N10" s="58">
+      <c r="N10" s="56">
         <f t="shared" si="5"/>
         <v>0.39587070653873374</v>
       </c>
       <c r="O10" s="27">
         <v>202821</v>
       </c>
-      <c r="P10" s="58">
+      <c r="P10" s="56">
         <f t="shared" si="6"/>
         <v>0.38791357384799874</v>
       </c>
       <c r="Q10" s="28">
         <v>2058825</v>
       </c>
-      <c r="R10" s="58">
+      <c r="R10" s="56">
         <f t="shared" si="7"/>
         <v>0.32244729324070159</v>
       </c>
@@ -3523,49 +3721,49 @@
       <c r="E11" s="27">
         <v>12125</v>
       </c>
-      <c r="F11" s="58">
+      <c r="F11" s="56">
         <f>E11/$E$6</f>
         <v>0.11929710636874366</v>
       </c>
       <c r="G11" s="27">
         <v>3662</v>
       </c>
-      <c r="H11" s="60">
+      <c r="H11" s="57">
         <f t="shared" si="2"/>
         <v>5.3909228753551502E-2</v>
       </c>
       <c r="I11" s="27">
         <v>1512</v>
       </c>
-      <c r="J11" s="58">
+      <c r="J11" s="56">
         <f t="shared" si="3"/>
         <v>9.9854708757099453E-2</v>
       </c>
       <c r="K11" s="27">
         <v>17440</v>
       </c>
-      <c r="L11" s="58">
+      <c r="L11" s="56">
         <f t="shared" si="4"/>
         <v>0.10758923614109983</v>
       </c>
       <c r="M11" s="27">
         <v>36658</v>
       </c>
-      <c r="N11" s="58">
+      <c r="N11" s="56">
         <f t="shared" si="5"/>
         <v>0.10055243769303775</v>
       </c>
       <c r="O11" s="27">
         <v>45729</v>
       </c>
-      <c r="P11" s="58">
+      <c r="P11" s="56">
         <f t="shared" si="6"/>
         <v>8.7460863611239142E-2</v>
       </c>
       <c r="Q11" s="28">
         <v>394131</v>
       </c>
-      <c r="R11" s="60">
+      <c r="R11" s="57">
         <f t="shared" si="7"/>
         <v>6.1727671915899097E-2</v>
       </c>
@@ -3580,7 +3778,7 @@
       <c r="C12" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="66" t="s">
+      <c r="D12" s="63" t="s">
         <v>49</v>
       </c>
       <c r="E12" s="51" t="s">
@@ -3592,7 +3790,7 @@
       <c r="G12" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="61" t="s">
+      <c r="H12" s="58" t="s">
         <v>49</v>
       </c>
       <c r="I12" s="51" t="s">
@@ -3619,10 +3817,10 @@
       <c r="P12" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="Q12" s="65" t="s">
+      <c r="Q12" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="R12" s="61" t="s">
+      <c r="R12" s="58" t="s">
         <v>49</v>
       </c>
       <c r="T12" s="26"/>
@@ -3643,49 +3841,49 @@
       <c r="E13" s="27">
         <v>121202</v>
       </c>
-      <c r="F13" s="58">
+      <c r="F13" s="56">
         <f>E13/$E$15</f>
         <v>0.5909294796786021</v>
       </c>
       <c r="G13" s="27">
         <v>65534</v>
       </c>
-      <c r="H13" s="62">
+      <c r="H13" s="59">
         <f>G13/$G$15</f>
         <v>0.50121989460722449</v>
       </c>
       <c r="I13" s="27">
         <v>21776</v>
       </c>
-      <c r="J13" s="58">
+      <c r="J13" s="56">
         <f>I13/$I$15</f>
         <v>0.6707944429042294</v>
       </c>
       <c r="K13" s="27">
         <v>244128</v>
       </c>
-      <c r="L13" s="58">
+      <c r="L13" s="56">
         <f>K13/$K$15</f>
         <v>0.57202707737296055</v>
       </c>
       <c r="M13" s="27">
         <v>474226</v>
       </c>
-      <c r="N13" s="58">
+      <c r="N13" s="56">
         <f>M13/$M$15</f>
         <v>0.56950744270110909</v>
       </c>
       <c r="O13" s="27">
         <v>664664</v>
       </c>
-      <c r="P13" s="58">
+      <c r="P13" s="56">
         <f>O13/$O$15</f>
         <v>0.57728348525445883</v>
       </c>
       <c r="Q13" s="28">
         <v>7100074</v>
       </c>
-      <c r="R13" s="62">
+      <c r="R13" s="59">
         <f>Q13/$Q$15</f>
         <v>0.58987175823153304</v>
       </c>
@@ -3704,49 +3902,49 @@
       <c r="E14" s="27">
         <v>83902</v>
       </c>
-      <c r="F14" s="58">
+      <c r="F14" s="56">
         <f t="shared" ref="F14:F20" si="9">E14/$E$15</f>
         <v>0.4090705203213979</v>
       </c>
       <c r="G14" s="27">
         <v>65215</v>
       </c>
-      <c r="H14" s="58">
+      <c r="H14" s="56">
         <f t="shared" ref="H14:H20" si="10">G14/$G$15</f>
         <v>0.49878010539277545</v>
       </c>
       <c r="I14" s="27">
         <v>10687</v>
       </c>
-      <c r="J14" s="58">
+      <c r="J14" s="56">
         <f t="shared" ref="J14:J20" si="11">I14/$I$15</f>
         <v>0.3292055570957706</v>
       </c>
       <c r="K14" s="27">
         <v>182649</v>
       </c>
-      <c r="L14" s="58">
+      <c r="L14" s="56">
         <f t="shared" ref="L14:L20" si="12">K14/$K$15</f>
         <v>0.4279729226270394</v>
       </c>
       <c r="M14" s="27">
         <v>358469</v>
       </c>
-      <c r="N14" s="58">
+      <c r="N14" s="56">
         <f>M14/$M$15</f>
         <v>0.43049255729889097</v>
       </c>
       <c r="O14" s="27">
         <v>486701</v>
       </c>
-      <c r="P14" s="58">
+      <c r="P14" s="56">
         <f t="shared" ref="P14:P20" si="13">O14/$O$15</f>
         <v>0.42271651474554117</v>
       </c>
       <c r="Q14" s="28">
         <v>4936566</v>
       </c>
-      <c r="R14" s="58">
+      <c r="R14" s="56">
         <f t="shared" ref="R14:R20" si="14">Q14/$Q$15</f>
         <v>0.41012824176846696</v>
       </c>
@@ -3759,57 +3957,65 @@
         <f>SUM(C13:C14)</f>
         <v>37602</v>
       </c>
-      <c r="D15" s="55" t="s">
-        <v>12</v>
+      <c r="D15" s="54">
+        <f>C15/C24</f>
+        <v>0.67920234095589027</v>
       </c>
       <c r="E15" s="27">
         <f>SUM(E13:E14)</f>
         <v>205104</v>
       </c>
-      <c r="F15" s="63" t="s">
-        <v>12</v>
+      <c r="F15" s="60">
+        <f>E15/C25</f>
+        <v>0.66865531507036879</v>
       </c>
       <c r="G15" s="27">
         <f>SUM(G13:G14)</f>
         <v>130749</v>
       </c>
-      <c r="H15" s="63" t="s">
-        <v>12</v>
+      <c r="H15" s="60">
+        <f>G15/C26</f>
+        <v>0.65809500800289922</v>
       </c>
       <c r="I15" s="27">
         <f>SUM(I13:I14)</f>
         <v>32463</v>
       </c>
-      <c r="J15" s="63" t="s">
-        <v>12</v>
+      <c r="J15" s="60">
+        <f>I15/C27</f>
+        <v>0.68192416762945074</v>
       </c>
       <c r="K15" s="27">
         <f>SUM(K13:K14)</f>
         <v>426777</v>
       </c>
-      <c r="L15" s="63" t="s">
-        <v>12</v>
+      <c r="L15" s="60">
+        <f>K15/C28</f>
+        <v>0.72473275313097008</v>
       </c>
       <c r="M15" s="27">
         <f>SUM(M13:M14)</f>
         <v>832695</v>
       </c>
-      <c r="N15" s="63" t="s">
-        <v>12</v>
+      <c r="N15" s="60">
+        <f>M15/C29</f>
+        <v>0.69549997870138591</v>
       </c>
       <c r="O15" s="27">
         <f>SUM(O13:O14)</f>
         <v>1151365</v>
       </c>
-      <c r="P15" s="63" t="s">
-        <v>12</v>
+      <c r="P15" s="60">
+        <f>O15/C30</f>
+        <v>0.68770397606999334</v>
       </c>
       <c r="Q15" s="28">
         <f t="shared" ref="Q15" si="15">SUM(Q13:Q14)</f>
         <v>12036640</v>
       </c>
-      <c r="R15" s="63" t="s">
-        <v>12</v>
+      <c r="R15" s="60">
+        <f>Q15/C31</f>
+        <v>0.65339687238435973</v>
       </c>
     </row>
     <row r="16" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -3819,19 +4025,19 @@
       <c r="C16" s="28"/>
       <c r="D16" s="53"/>
       <c r="E16" s="27"/>
-      <c r="F16" s="58"/>
+      <c r="F16" s="56"/>
       <c r="G16" s="27"/>
-      <c r="H16" s="58"/>
+      <c r="H16" s="56"/>
       <c r="I16" s="27"/>
-      <c r="J16" s="58"/>
+      <c r="J16" s="56"/>
       <c r="K16" s="27"/>
-      <c r="L16" s="58"/>
+      <c r="L16" s="56"/>
       <c r="M16" s="27"/>
-      <c r="N16" s="58"/>
+      <c r="N16" s="56"/>
       <c r="O16" s="27"/>
-      <c r="P16" s="58"/>
+      <c r="P16" s="56"/>
       <c r="Q16" s="28"/>
-      <c r="R16" s="58"/>
+      <c r="R16" s="56"/>
     </row>
     <row r="17" spans="2:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="46" t="s">
@@ -3847,49 +4053,49 @@
       <c r="E17" s="27">
         <v>18488</v>
       </c>
-      <c r="F17" s="58">
+      <c r="F17" s="56">
         <f t="shared" si="9"/>
         <v>9.0139636477104296E-2</v>
       </c>
       <c r="G17" s="27">
         <v>23389</v>
       </c>
-      <c r="H17" s="58">
+      <c r="H17" s="56">
         <f t="shared" si="10"/>
         <v>0.17888473334404087</v>
       </c>
       <c r="I17" s="27">
         <v>3146</v>
       </c>
-      <c r="J17" s="58">
+      <c r="J17" s="56">
         <f t="shared" si="11"/>
         <v>9.6910328681883998E-2</v>
       </c>
       <c r="K17" s="27">
         <v>53067</v>
       </c>
-      <c r="L17" s="58">
+      <c r="L17" s="56">
         <f t="shared" si="12"/>
         <v>0.12434362676526617</v>
       </c>
       <c r="M17" s="27">
         <v>103577</v>
       </c>
-      <c r="N17" s="58">
+      <c r="N17" s="56">
         <f t="shared" ref="N17:N20" si="16">M17/$M$15</f>
         <v>0.12438768096361813</v>
       </c>
       <c r="O17" s="27">
         <v>153570</v>
       </c>
-      <c r="P17" s="58">
+      <c r="P17" s="56">
         <f t="shared" si="13"/>
         <v>0.13338081320866971</v>
       </c>
       <c r="Q17" s="28">
         <v>1552111</v>
       </c>
-      <c r="R17" s="58">
+      <c r="R17" s="56">
         <f t="shared" si="14"/>
         <v>0.12894885948238047</v>
       </c>
@@ -3908,49 +4114,49 @@
       <c r="E18" s="27">
         <v>185284</v>
       </c>
-      <c r="F18" s="58">
+      <c r="F18" s="56">
         <f t="shared" si="9"/>
         <v>0.90336609719946959</v>
       </c>
       <c r="G18" s="27">
         <v>106693</v>
       </c>
-      <c r="H18" s="58">
+      <c r="H18" s="56">
         <f t="shared" si="10"/>
         <v>0.81601388920756568</v>
       </c>
       <c r="I18" s="27">
         <v>29202</v>
       </c>
-      <c r="J18" s="58">
+      <c r="J18" s="56">
         <f t="shared" si="11"/>
         <v>0.89954717678587925</v>
       </c>
       <c r="K18" s="27">
         <v>371384</v>
       </c>
-      <c r="L18" s="58">
+      <c r="L18" s="56">
         <f t="shared" si="12"/>
         <v>0.87020622011026838</v>
       </c>
       <c r="M18" s="27">
         <v>724358</v>
       </c>
-      <c r="N18" s="58">
+      <c r="N18" s="56">
         <f t="shared" si="16"/>
         <v>0.86989594029026229</v>
       </c>
       <c r="O18" s="27">
         <v>990319</v>
       </c>
-      <c r="P18" s="58">
+      <c r="P18" s="56">
         <f t="shared" si="13"/>
         <v>0.86012602432764584</v>
       </c>
       <c r="Q18" s="28">
         <v>10383822</v>
       </c>
-      <c r="R18" s="58">
+      <c r="R18" s="56">
         <f t="shared" si="14"/>
         <v>0.86268443685280938</v>
       </c>
@@ -3969,49 +4175,49 @@
       <c r="E19" s="27">
         <v>44982</v>
       </c>
-      <c r="F19" s="58">
+      <c r="F19" s="56">
         <f t="shared" si="9"/>
         <v>0.21931312894921601</v>
       </c>
       <c r="G19" s="27">
         <v>46788</v>
       </c>
-      <c r="H19" s="58">
+      <c r="H19" s="56">
         <f t="shared" si="10"/>
         <v>0.35784594910859741</v>
       </c>
       <c r="I19" s="27">
         <v>11586</v>
       </c>
-      <c r="J19" s="58">
+      <c r="J19" s="56">
         <f t="shared" si="11"/>
         <v>0.35689862304777747</v>
       </c>
       <c r="K19" s="27">
         <v>118565</v>
       </c>
-      <c r="L19" s="58">
+      <c r="L19" s="56">
         <f t="shared" si="12"/>
         <v>0.27781487755900625</v>
       </c>
       <c r="M19" s="27">
         <v>233269</v>
       </c>
-      <c r="N19" s="58">
+      <c r="N19" s="56">
         <f t="shared" si="16"/>
         <v>0.28013738523709159</v>
       </c>
       <c r="O19" s="27">
         <v>373144</v>
       </c>
-      <c r="P19" s="58">
+      <c r="P19" s="56">
         <f t="shared" si="13"/>
         <v>0.32408836468018398</v>
       </c>
       <c r="Q19" s="28">
         <v>5231985</v>
       </c>
-      <c r="R19" s="58">
+      <c r="R19" s="56">
         <f t="shared" si="14"/>
         <v>0.43467155285860504</v>
       </c>
@@ -4023,61 +4229,126 @@
       <c r="C20" s="34">
         <v>20447</v>
       </c>
-      <c r="D20" s="64">
+      <c r="D20" s="61">
         <f t="shared" si="8"/>
         <v>0.54377426732620604</v>
       </c>
       <c r="E20" s="33">
         <v>140302</v>
       </c>
-      <c r="F20" s="60">
+      <c r="F20" s="57">
         <f t="shared" si="9"/>
         <v>0.68405296825025352</v>
       </c>
       <c r="G20" s="33">
         <v>59905</v>
       </c>
-      <c r="H20" s="60">
+      <c r="H20" s="57">
         <f t="shared" si="10"/>
         <v>0.45816794009896827</v>
       </c>
       <c r="I20" s="33">
         <v>17616</v>
       </c>
-      <c r="J20" s="60">
+      <c r="J20" s="57">
         <f t="shared" si="11"/>
         <v>0.54264855373810184</v>
       </c>
       <c r="K20" s="33">
         <v>252819</v>
       </c>
-      <c r="L20" s="60">
+      <c r="L20" s="57">
         <f t="shared" si="12"/>
         <v>0.59239134255126213</v>
       </c>
       <c r="M20" s="33">
         <v>491089</v>
       </c>
-      <c r="N20" s="60">
+      <c r="N20" s="57">
         <f t="shared" si="16"/>
         <v>0.58975855505317076</v>
       </c>
       <c r="O20" s="33">
         <v>617175</v>
       </c>
-      <c r="P20" s="60">
+      <c r="P20" s="57">
         <f t="shared" si="13"/>
         <v>0.53603765964746197</v>
       </c>
       <c r="Q20" s="34">
         <v>5151837</v>
       </c>
-      <c r="R20" s="60">
+      <c r="R20" s="57">
         <f t="shared" si="14"/>
         <v>0.42801288399420434</v>
       </c>
     </row>
     <row r="21" spans="2:18" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24">
+        <v>55362</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25">
+        <v>306741</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26">
+        <v>198678</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27">
+        <v>47605</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28">
+        <v>588875</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29">
+        <f>SUM(C24:C28)</f>
+        <v>1197261</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30">
+        <v>1674216</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31">
+        <v>18421637</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="B2:R2"/>
@@ -4098,10 +4369,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B48D4E-D75D-404D-AC01-9AD0F7A038FD}">
-  <dimension ref="A1:T21"/>
+  <dimension ref="A1:T32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:J5"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4116,75 +4387,75 @@
   <sheetData>
     <row r="1" spans="2:20" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:20" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="74"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="71"/>
     </row>
     <row r="3" spans="2:20" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="82" t="s">
+      <c r="C3" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="82"/>
-      <c r="N3" s="82"/>
-      <c r="O3" s="82"/>
-      <c r="P3" s="69"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="79"/>
+      <c r="O3" s="79"/>
+      <c r="P3" s="66"/>
     </row>
     <row r="4" spans="2:20" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="81"/>
-      <c r="C4" s="75" t="s">
+      <c r="B4" s="78"/>
+      <c r="C4" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="76"/>
-      <c r="E4" s="75" t="s">
+      <c r="D4" s="73"/>
+      <c r="E4" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="76"/>
-      <c r="G4" s="75" t="s">
+      <c r="F4" s="73"/>
+      <c r="G4" s="72" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="77"/>
-      <c r="I4" s="75" t="s">
+      <c r="H4" s="74"/>
+      <c r="I4" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="J4" s="76"/>
-      <c r="K4" s="75" t="s">
+      <c r="J4" s="73"/>
+      <c r="K4" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="L4" s="76"/>
-      <c r="M4" s="75" t="s">
+      <c r="L4" s="73"/>
+      <c r="M4" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="N4" s="76"/>
-      <c r="O4" s="77" t="s">
+      <c r="N4" s="73"/>
+      <c r="O4" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="76"/>
+      <c r="P4" s="73"/>
     </row>
     <row r="5" spans="2:20" ht="43" x14ac:dyDescent="0.25">
       <c r="B5" s="39" t="s">
@@ -4205,7 +4476,7 @@
       <c r="G5" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="66" t="s">
+      <c r="H5" s="63" t="s">
         <v>48</v>
       </c>
       <c r="I5" s="51" t="s">
@@ -4244,44 +4515,51 @@
       <c r="C6" s="27">
         <v>21033</v>
       </c>
-      <c r="D6" s="57" t="s">
-        <v>12</v>
+      <c r="D6" s="60">
+        <f>C6/C26</f>
+        <v>0.87010300748769287</v>
       </c>
       <c r="E6" s="27">
         <v>79622</v>
       </c>
-      <c r="F6" s="57" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="67">
+      <c r="F6" s="60">
+        <f>E6/C27</f>
+        <v>0.81295052173735471</v>
+      </c>
+      <c r="G6" s="64">
         <v>269</v>
       </c>
-      <c r="H6" s="57" t="s">
-        <v>12</v>
+      <c r="H6" s="60">
+        <f>G6/C28</f>
+        <v>0.99261992619926198</v>
       </c>
       <c r="I6" s="27">
         <v>5908</v>
       </c>
-      <c r="J6" s="57" t="s">
-        <v>12</v>
+      <c r="J6" s="60">
+        <f>I6/C29</f>
+        <v>0.89978678038379534</v>
       </c>
       <c r="K6" s="27">
         <v>16210</v>
       </c>
-      <c r="L6" s="57" t="s">
-        <v>12</v>
+      <c r="L6" s="60">
+        <f>K6/C30</f>
+        <v>0.86471780646537932</v>
       </c>
       <c r="M6" s="27">
         <v>123042</v>
       </c>
-      <c r="N6" s="57" t="s">
-        <v>12</v>
+      <c r="N6" s="60">
+        <f>M6/C31</f>
+        <v>0.83306476729542711</v>
       </c>
       <c r="O6" s="27">
         <v>465799</v>
       </c>
-      <c r="P6" s="57" t="s">
-        <v>12</v>
+      <c r="P6" s="60">
+        <f>O6/C32</f>
+        <v>0.76185141085109032</v>
       </c>
       <c r="Q6" s="50"/>
       <c r="R6" s="42"/>
@@ -4296,7 +4574,7 @@
       <c r="D7" s="29"/>
       <c r="E7" s="30"/>
       <c r="F7" s="29"/>
-      <c r="G7" s="67"/>
+      <c r="G7" s="64"/>
       <c r="H7" s="29"/>
       <c r="I7" s="30"/>
       <c r="J7" s="29"/>
@@ -4318,49 +4596,49 @@
       <c r="C8" s="27">
         <v>13270</v>
       </c>
-      <c r="D8" s="58">
+      <c r="D8" s="56">
         <f>C8/$C$6</f>
         <v>0.63091332667712641</v>
       </c>
       <c r="E8" s="27">
         <v>55956</v>
       </c>
-      <c r="F8" s="58">
+      <c r="F8" s="56">
         <f>E8/$E$6</f>
         <v>0.7027705910426767</v>
       </c>
-      <c r="G8" s="67">
+      <c r="G8" s="64">
         <v>266</v>
       </c>
-      <c r="H8" s="58">
+      <c r="H8" s="56">
         <f>G8/$G$6</f>
         <v>0.98884758364312264</v>
       </c>
       <c r="I8" s="27">
         <v>4520</v>
       </c>
-      <c r="J8" s="58">
+      <c r="J8" s="56">
         <f>I8/$I$6</f>
         <v>0.76506431956668919</v>
       </c>
       <c r="K8" s="27">
         <v>12862</v>
       </c>
-      <c r="L8" s="58">
+      <c r="L8" s="56">
         <f>K8/$K$6</f>
         <v>0.79346082665021589</v>
       </c>
       <c r="M8" s="27">
         <v>86874</v>
       </c>
-      <c r="N8" s="58">
+      <c r="N8" s="56">
         <f>M8/$M$6</f>
         <v>0.70605159213926949</v>
       </c>
       <c r="O8" s="27">
         <v>313546</v>
       </c>
-      <c r="P8" s="58">
+      <c r="P8" s="56">
         <f>O8/$O$6</f>
         <v>0.67313583756083628</v>
       </c>
@@ -4376,49 +4654,49 @@
       <c r="C9" s="27">
         <v>6308</v>
       </c>
-      <c r="D9" s="58">
+      <c r="D9" s="56">
         <f t="shared" ref="D9:D11" si="0">C9/$C$6</f>
         <v>0.29990966576332428</v>
       </c>
       <c r="E9" s="27">
         <v>15700</v>
       </c>
-      <c r="F9" s="58">
+      <c r="F9" s="56">
         <f t="shared" ref="F9:F11" si="1">E9/$E$6</f>
         <v>0.19718168345432166</v>
       </c>
-      <c r="G9" s="67">
+      <c r="G9" s="64">
         <v>3</v>
       </c>
-      <c r="H9" s="58">
+      <c r="H9" s="56">
         <f t="shared" ref="H9:H11" si="2">G9/$G$6</f>
         <v>1.1152416356877323E-2</v>
       </c>
       <c r="I9" s="27">
         <v>865</v>
       </c>
-      <c r="J9" s="58">
+      <c r="J9" s="56">
         <f t="shared" ref="J9:J11" si="3">I9/$I$6</f>
         <v>0.1464116452268111</v>
       </c>
       <c r="K9" s="27">
         <v>2147</v>
       </c>
-      <c r="L9" s="58">
+      <c r="L9" s="56">
         <f t="shared" ref="L9:L11" si="4">K9/$K$6</f>
         <v>0.13244910549043801</v>
       </c>
       <c r="M9" s="27">
         <v>25023</v>
       </c>
-      <c r="N9" s="58">
+      <c r="N9" s="56">
         <f t="shared" ref="N9:N11" si="5">M9/$M$6</f>
         <v>0.20336958111864242</v>
       </c>
       <c r="O9" s="27">
         <v>111647</v>
       </c>
-      <c r="P9" s="58">
+      <c r="P9" s="56">
         <f t="shared" ref="P9:P11" si="6">O9/$O$6</f>
         <v>0.23968922217523009</v>
       </c>
@@ -4434,49 +4712,49 @@
       <c r="C10" s="27">
         <v>5162</v>
       </c>
-      <c r="D10" s="58">
+      <c r="D10" s="56">
         <f t="shared" si="0"/>
         <v>0.2454238577473494</v>
       </c>
       <c r="E10" s="27">
         <v>12057</v>
       </c>
-      <c r="F10" s="58">
+      <c r="F10" s="56">
         <f t="shared" si="1"/>
         <v>0.15142799728718193</v>
       </c>
-      <c r="G10" s="67">
+      <c r="G10" s="64">
         <v>3</v>
       </c>
-      <c r="H10" s="58">
+      <c r="H10" s="56">
         <f t="shared" si="2"/>
         <v>1.1152416356877323E-2</v>
       </c>
       <c r="I10" s="27">
         <v>762</v>
       </c>
-      <c r="J10" s="58">
+      <c r="J10" s="56">
         <f t="shared" si="3"/>
         <v>0.12897765741367637</v>
       </c>
       <c r="K10" s="27">
         <v>1938</v>
       </c>
-      <c r="L10" s="58">
+      <c r="L10" s="56">
         <f t="shared" si="4"/>
         <v>0.11955582973473165</v>
       </c>
       <c r="M10" s="27">
         <v>19922</v>
       </c>
-      <c r="N10" s="58">
+      <c r="N10" s="56">
         <f t="shared" si="5"/>
         <v>0.1619121925846459</v>
       </c>
       <c r="O10" s="27">
         <v>92192</v>
       </c>
-      <c r="P10" s="58">
+      <c r="P10" s="56">
         <f t="shared" si="6"/>
         <v>0.19792227978162255</v>
       </c>
@@ -4489,49 +4767,49 @@
       <c r="C11" s="27">
         <v>1146</v>
       </c>
-      <c r="D11" s="58">
+      <c r="D11" s="56">
         <f t="shared" si="0"/>
         <v>5.4485808015974899E-2</v>
       </c>
       <c r="E11" s="27">
         <v>3643</v>
       </c>
-      <c r="F11" s="58">
+      <c r="F11" s="56">
         <f t="shared" si="1"/>
         <v>4.5753686167139734E-2</v>
       </c>
-      <c r="G11" s="67">
+      <c r="G11" s="64">
         <v>0</v>
       </c>
-      <c r="H11" s="58">
+      <c r="H11" s="56">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I11" s="27">
         <v>103</v>
       </c>
-      <c r="J11" s="58">
+      <c r="J11" s="56">
         <f t="shared" si="3"/>
         <v>1.7433987813134731E-2</v>
       </c>
       <c r="K11" s="27">
         <v>209</v>
       </c>
-      <c r="L11" s="58">
+      <c r="L11" s="56">
         <f t="shared" si="4"/>
         <v>1.2893275755706354E-2</v>
       </c>
       <c r="M11" s="27">
         <v>5101</v>
       </c>
-      <c r="N11" s="58">
+      <c r="N11" s="56">
         <f t="shared" si="5"/>
         <v>4.1457388533996518E-2</v>
       </c>
       <c r="O11" s="27">
         <v>19455</v>
       </c>
-      <c r="P11" s="58">
+      <c r="P11" s="56">
         <f t="shared" si="6"/>
         <v>4.1766942393607544E-2</v>
       </c>
@@ -4592,49 +4870,49 @@
       <c r="C13" s="27">
         <v>322</v>
       </c>
-      <c r="D13" s="58">
+      <c r="D13" s="56">
         <f>C13/$C$15</f>
         <v>0.10254777070063695</v>
       </c>
       <c r="E13" s="27">
         <v>4280</v>
       </c>
-      <c r="F13" s="58">
+      <c r="F13" s="56">
         <f>E13/$E$15</f>
         <v>0.23362445414847161</v>
       </c>
-      <c r="G13" s="67">
+      <c r="G13" s="64">
         <v>2</v>
       </c>
-      <c r="H13" s="58">
+      <c r="H13" s="56">
         <f>G13/$G$15</f>
         <v>1</v>
       </c>
       <c r="I13" s="27">
         <v>130</v>
       </c>
-      <c r="J13" s="58">
+      <c r="J13" s="56">
         <f>I13/$I$15</f>
         <v>0.19756838905775076</v>
       </c>
       <c r="K13" s="27">
         <v>465</v>
       </c>
-      <c r="L13" s="58">
+      <c r="L13" s="56">
         <f>K13/$K$15</f>
         <v>0.1833596214511041</v>
       </c>
       <c r="M13" s="27">
         <v>5199</v>
       </c>
-      <c r="N13" s="58">
+      <c r="N13" s="56">
         <f>M13/$M$15</f>
         <v>0.21086145360155742</v>
       </c>
       <c r="O13" s="27">
         <v>59488</v>
       </c>
-      <c r="P13" s="58">
+      <c r="P13" s="56">
         <f>O13/$O$15</f>
         <v>0.4085573984409876</v>
       </c>
@@ -4646,49 +4924,49 @@
       <c r="C14" s="27">
         <v>2818</v>
       </c>
-      <c r="D14" s="58">
+      <c r="D14" s="56">
         <f>C14/$C$15</f>
         <v>0.89745222929936308</v>
       </c>
       <c r="E14" s="27">
         <v>14040</v>
       </c>
-      <c r="F14" s="58">
+      <c r="F14" s="56">
         <f t="shared" ref="F14:F20" si="7">E14/$E$15</f>
         <v>0.76637554585152834</v>
       </c>
-      <c r="G14" s="67">
+      <c r="G14" s="64">
         <v>0</v>
       </c>
-      <c r="H14" s="58">
+      <c r="H14" s="56">
         <f t="shared" ref="H14:H20" si="8">G14/$G$15</f>
         <v>0</v>
       </c>
       <c r="I14" s="27">
         <v>528</v>
       </c>
-      <c r="J14" s="58">
+      <c r="J14" s="56">
         <f t="shared" ref="J14:J20" si="9">I14/$I$15</f>
         <v>0.80243161094224924</v>
       </c>
       <c r="K14" s="27">
         <v>2071</v>
       </c>
-      <c r="L14" s="58">
+      <c r="L14" s="56">
         <f t="shared" ref="L14:L20" si="10">K14/$K$15</f>
         <v>0.81664037854889593</v>
       </c>
       <c r="M14" s="27">
         <v>19457</v>
       </c>
-      <c r="N14" s="58">
+      <c r="N14" s="56">
         <f t="shared" ref="N14:N20" si="11">M14/$M$15</f>
         <v>0.78913854639844261</v>
       </c>
       <c r="O14" s="27">
         <v>86117</v>
       </c>
-      <c r="P14" s="58">
+      <c r="P14" s="56">
         <f t="shared" ref="P14:P20" si="12">O14/$O$15</f>
         <v>0.5914426015590124</v>
       </c>
@@ -4701,50 +4979,57 @@
         <f>SUM(C13:C14)</f>
         <v>3140</v>
       </c>
-      <c r="D15" s="63" t="s">
-        <v>12</v>
+      <c r="D15" s="60">
+        <f>C15/C26</f>
+        <v>0.12989699251230713</v>
       </c>
       <c r="E15" s="27">
         <f>SUM(E13:E14)</f>
         <v>18320</v>
       </c>
-      <c r="F15" s="63" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="67">
+      <c r="F15" s="60">
+        <f>E15/C27</f>
+        <v>0.18704947826264523</v>
+      </c>
+      <c r="G15" s="64">
         <f>SUM(G13:G14)</f>
         <v>2</v>
       </c>
-      <c r="H15" s="63" t="s">
-        <v>12</v>
+      <c r="H15" s="60">
+        <f>G15/C28</f>
+        <v>7.3800738007380072E-3</v>
       </c>
       <c r="I15" s="27">
         <f>SUM(I13:I14)</f>
         <v>658</v>
       </c>
-      <c r="J15" s="63" t="s">
-        <v>12</v>
+      <c r="J15" s="60">
+        <f>I15/C29</f>
+        <v>0.10021321961620469</v>
       </c>
       <c r="K15" s="27">
         <f>SUM(K13:K14)</f>
         <v>2536</v>
       </c>
-      <c r="L15" s="63" t="s">
-        <v>12</v>
+      <c r="L15" s="60">
+        <f>K15/C30</f>
+        <v>0.13528219353462073</v>
       </c>
       <c r="M15" s="27">
         <f>SUM(M13:M14)</f>
         <v>24656</v>
       </c>
-      <c r="N15" s="63" t="s">
-        <v>12</v>
+      <c r="N15" s="60">
+        <f>M15/C31</f>
+        <v>0.16693523270457283</v>
       </c>
       <c r="O15" s="27">
         <f t="shared" ref="O15" si="13">SUM(O13:O14)</f>
         <v>145605</v>
       </c>
-      <c r="P15" s="63" t="s">
-        <v>12</v>
+      <c r="P15" s="60">
+        <f>O15/C32</f>
+        <v>0.23814858914890971</v>
       </c>
     </row>
     <row r="16" spans="2:20" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -4752,19 +5037,19 @@
         <v>23</v>
       </c>
       <c r="C16" s="27"/>
-      <c r="D16" s="58"/>
+      <c r="D16" s="56"/>
       <c r="E16" s="30"/>
-      <c r="F16" s="58"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="58"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="64"/>
+      <c r="H16" s="56"/>
       <c r="I16" s="30"/>
-      <c r="J16" s="58"/>
+      <c r="J16" s="56"/>
       <c r="K16" s="27"/>
-      <c r="L16" s="58"/>
+      <c r="L16" s="56"/>
       <c r="M16" s="27"/>
-      <c r="N16" s="58"/>
+      <c r="N16" s="56"/>
       <c r="O16" s="30"/>
-      <c r="P16" s="58"/>
+      <c r="P16" s="56"/>
     </row>
     <row r="17" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="36" t="s">
@@ -4773,49 +5058,49 @@
       <c r="C17" s="27">
         <v>175</v>
       </c>
-      <c r="D17" s="58">
+      <c r="D17" s="56">
         <f t="shared" ref="D17:D20" si="14">C17/$C$15</f>
         <v>5.5732484076433123E-2</v>
       </c>
       <c r="E17" s="27">
         <v>2159</v>
       </c>
-      <c r="F17" s="58">
+      <c r="F17" s="56">
         <f t="shared" si="7"/>
         <v>0.11784934497816595</v>
       </c>
-      <c r="G17" s="67">
+      <c r="G17" s="64">
         <v>0</v>
       </c>
-      <c r="H17" s="58">
+      <c r="H17" s="56">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I17" s="27">
         <v>122</v>
       </c>
-      <c r="J17" s="58">
+      <c r="J17" s="56">
         <f t="shared" si="9"/>
         <v>0.18541033434650456</v>
       </c>
       <c r="K17" s="27">
         <v>831</v>
       </c>
-      <c r="L17" s="58">
+      <c r="L17" s="56">
         <f t="shared" si="10"/>
         <v>0.32768138801261831</v>
       </c>
       <c r="M17" s="27">
         <v>3287</v>
       </c>
-      <c r="N17" s="58">
+      <c r="N17" s="56">
         <f t="shared" si="11"/>
         <v>0.13331440622972096</v>
       </c>
       <c r="O17" s="27">
         <v>27519</v>
       </c>
-      <c r="P17" s="58">
+      <c r="P17" s="56">
         <f t="shared" si="12"/>
         <v>0.18899763057587307</v>
       </c>
@@ -4829,49 +5114,49 @@
       <c r="C18" s="27">
         <v>2965</v>
       </c>
-      <c r="D18" s="58">
+      <c r="D18" s="56">
         <f t="shared" si="14"/>
         <v>0.94426751592356684</v>
       </c>
       <c r="E18" s="27">
         <v>15887</v>
       </c>
-      <c r="F18" s="58">
+      <c r="F18" s="56">
         <f t="shared" si="7"/>
         <v>0.86719432314410483</v>
       </c>
-      <c r="G18" s="67">
+      <c r="G18" s="64">
         <v>2</v>
       </c>
-      <c r="H18" s="58">
+      <c r="H18" s="56">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="I18" s="27">
         <v>505</v>
       </c>
-      <c r="J18" s="58">
+      <c r="J18" s="56">
         <f t="shared" si="9"/>
         <v>0.76747720364741645</v>
       </c>
       <c r="K18" s="27">
         <v>1705</v>
       </c>
-      <c r="L18" s="58">
+      <c r="L18" s="56">
         <f t="shared" si="10"/>
         <v>0.67231861198738174</v>
       </c>
       <c r="M18" s="27">
         <v>21064</v>
       </c>
-      <c r="N18" s="58">
+      <c r="N18" s="56">
         <f t="shared" si="11"/>
         <v>0.85431537962362103</v>
       </c>
       <c r="O18" s="27">
         <v>116191</v>
       </c>
-      <c r="P18" s="58">
+      <c r="P18" s="56">
         <f t="shared" si="12"/>
         <v>0.79798770646612416</v>
       </c>
@@ -4883,49 +5168,49 @@
       <c r="C19" s="27">
         <v>1470</v>
       </c>
-      <c r="D19" s="58">
+      <c r="D19" s="56">
         <f t="shared" si="14"/>
         <v>0.46815286624203822</v>
       </c>
       <c r="E19" s="27">
         <v>6333</v>
       </c>
-      <c r="F19" s="58">
+      <c r="F19" s="56">
         <f t="shared" si="7"/>
         <v>0.34568777292576419</v>
       </c>
-      <c r="G19" s="67">
+      <c r="G19" s="64">
         <v>0</v>
       </c>
-      <c r="H19" s="58">
+      <c r="H19" s="56">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I19" s="27">
         <v>165</v>
       </c>
-      <c r="J19" s="58">
+      <c r="J19" s="56">
         <f t="shared" si="9"/>
         <v>0.25075987841945291</v>
       </c>
       <c r="K19" s="27">
         <v>922</v>
       </c>
-      <c r="L19" s="58">
+      <c r="L19" s="56">
         <f t="shared" si="10"/>
         <v>0.3635646687697161</v>
       </c>
       <c r="M19" s="27">
         <v>8890</v>
       </c>
-      <c r="N19" s="58">
+      <c r="N19" s="56">
         <f t="shared" si="11"/>
         <v>0.3605613238157041</v>
       </c>
       <c r="O19" s="27">
         <v>64122</v>
       </c>
-      <c r="P19" s="58">
+      <c r="P19" s="56">
         <f t="shared" si="12"/>
         <v>0.44038322859791901</v>
       </c>
@@ -4937,49 +5222,49 @@
       <c r="C20" s="33">
         <v>1495</v>
       </c>
-      <c r="D20" s="60">
+      <c r="D20" s="57">
         <f t="shared" si="14"/>
         <v>0.47611464968152867</v>
       </c>
       <c r="E20" s="33">
         <v>9554</v>
       </c>
-      <c r="F20" s="60">
+      <c r="F20" s="57">
         <f t="shared" si="7"/>
         <v>0.52150655021834058</v>
       </c>
-      <c r="G20" s="68">
+      <c r="G20" s="65">
         <v>2</v>
       </c>
-      <c r="H20" s="60">
+      <c r="H20" s="57">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="I20" s="33">
         <v>340</v>
       </c>
-      <c r="J20" s="60">
+      <c r="J20" s="57">
         <f t="shared" si="9"/>
         <v>0.51671732522796354</v>
       </c>
       <c r="K20" s="33">
         <v>783</v>
       </c>
-      <c r="L20" s="60">
+      <c r="L20" s="57">
         <f t="shared" si="10"/>
         <v>0.30875394321766564</v>
       </c>
       <c r="M20" s="33">
         <v>12174</v>
       </c>
-      <c r="N20" s="60">
+      <c r="N20" s="57">
         <f t="shared" si="11"/>
         <v>0.49375405580791693</v>
       </c>
       <c r="O20" s="33">
         <v>52069</v>
       </c>
-      <c r="P20" s="60">
+      <c r="P20" s="57">
         <f t="shared" si="12"/>
         <v>0.3576044778682051</v>
       </c>
@@ -4987,6 +5272,79 @@
     <row r="21" spans="2:19" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="R21"/>
       <c r="S21"/>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B25" s="95" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="95" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B26" s="94" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="94">
+        <v>24173</v>
+      </c>
+      <c r="D26" s="94"/>
+      <c r="E26" s="94"/>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B27" s="94" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="94">
+        <v>97942</v>
+      </c>
+      <c r="D27" s="94"/>
+      <c r="E27" s="94"/>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B28" s="94" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="94">
+        <v>271</v>
+      </c>
+      <c r="D28" s="94"/>
+      <c r="E28" s="94"/>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B29" s="94" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="94">
+        <v>6566</v>
+      </c>
+      <c r="D29" s="94"/>
+      <c r="E29" s="94"/>
+    </row>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B30" s="94" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="94">
+        <v>18746</v>
+      </c>
+    </row>
+    <row r="31" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B31" s="94" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31">
+        <f>SUM(C26:C30)</f>
+        <v>147698</v>
+      </c>
+    </row>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B32" s="94" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32">
+        <v>611404</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -5007,10 +5365,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A245BA8C-D3B6-1C4D-B04A-36E023573BAA}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5025,43 +5383,43 @@
   <sheetData>
     <row r="1" spans="2:12" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:12" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="74"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="71"/>
     </row>
     <row r="3" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="82" t="s">
+      <c r="C3" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="69"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="66"/>
     </row>
     <row r="4" spans="2:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="71"/>
-      <c r="C4" s="75" t="s">
+      <c r="B4" s="68"/>
+      <c r="C4" s="72" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="76"/>
-      <c r="E4" s="75" t="s">
+      <c r="D4" s="73"/>
+      <c r="E4" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="76"/>
-      <c r="G4" s="75" t="s">
+      <c r="F4" s="73"/>
+      <c r="G4" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="76"/>
+      <c r="H4" s="73"/>
     </row>
     <row r="5" spans="2:12" ht="43" x14ac:dyDescent="0.25">
       <c r="B5" s="43" t="s">
@@ -5097,20 +5455,23 @@
       <c r="C6" s="27">
         <v>495</v>
       </c>
-      <c r="D6" s="57" t="s">
-        <v>12</v>
+      <c r="D6" s="60">
+        <f>C6/C24</f>
+        <v>0.27108433734939757</v>
       </c>
       <c r="E6" s="27">
         <v>3882</v>
       </c>
-      <c r="F6" s="57" t="s">
-        <v>12</v>
+      <c r="F6" s="60">
+        <f>E6/C25</f>
+        <v>0.37130559540889524</v>
       </c>
       <c r="G6" s="27">
         <v>465799</v>
       </c>
-      <c r="H6" s="57" t="s">
-        <v>12</v>
+      <c r="H6" s="60">
+        <f>G6/C26</f>
+        <v>0.76185141085109032</v>
       </c>
       <c r="I6" s="50"/>
       <c r="J6" s="42"/>
@@ -5139,21 +5500,21 @@
       <c r="C8" s="27">
         <v>166</v>
       </c>
-      <c r="D8" s="58">
+      <c r="D8" s="56">
         <f>C8/$C$6</f>
         <v>0.33535353535353535</v>
       </c>
       <c r="E8" s="27">
         <v>1341</v>
       </c>
-      <c r="F8" s="58">
+      <c r="F8" s="56">
         <f>E8/$E$6</f>
         <v>0.34544049459041731</v>
       </c>
       <c r="G8" s="27">
         <v>313546</v>
       </c>
-      <c r="H8" s="58">
+      <c r="H8" s="56">
         <f>G8/$G$6</f>
         <v>0.67313583756083628</v>
       </c>
@@ -5169,21 +5530,21 @@
       <c r="C9" s="27">
         <v>207</v>
       </c>
-      <c r="D9" s="58">
+      <c r="D9" s="56">
         <f t="shared" ref="D9:D11" si="0">C9/$C$6</f>
         <v>0.41818181818181815</v>
       </c>
       <c r="E9" s="27">
         <v>1601</v>
       </c>
-      <c r="F9" s="58">
+      <c r="F9" s="56">
         <f t="shared" ref="F9:F11" si="1">E9/$E$6</f>
         <v>0.41241628026790317</v>
       </c>
       <c r="G9" s="27">
         <v>111647</v>
       </c>
-      <c r="H9" s="58">
+      <c r="H9" s="56">
         <f t="shared" ref="H9:H11" si="2">G9/$G$6</f>
         <v>0.23968922217523009</v>
       </c>
@@ -5199,21 +5560,21 @@
       <c r="C10" s="27">
         <v>138</v>
       </c>
-      <c r="D10" s="58">
+      <c r="D10" s="56">
         <f t="shared" si="0"/>
         <v>0.27878787878787881</v>
       </c>
       <c r="E10" s="27">
         <v>1263</v>
       </c>
-      <c r="F10" s="58">
+      <c r="F10" s="56">
         <f t="shared" si="1"/>
         <v>0.32534775888717155</v>
       </c>
       <c r="G10" s="27">
         <v>92192</v>
       </c>
-      <c r="H10" s="58">
+      <c r="H10" s="56">
         <f t="shared" si="2"/>
         <v>0.19792227978162255</v>
       </c>
@@ -5229,21 +5590,21 @@
       <c r="C11" s="27">
         <v>69</v>
       </c>
-      <c r="D11" s="58">
+      <c r="D11" s="56">
         <f t="shared" si="0"/>
         <v>0.1393939393939394</v>
       </c>
       <c r="E11" s="27">
         <v>338</v>
       </c>
-      <c r="F11" s="58">
+      <c r="F11" s="56">
         <f t="shared" si="1"/>
         <v>8.7068521380731581E-2</v>
       </c>
       <c r="G11" s="27">
         <v>19455</v>
       </c>
-      <c r="H11" s="58">
+      <c r="H11" s="56">
         <f t="shared" si="2"/>
         <v>4.1766942393607544E-2</v>
       </c>
@@ -5284,21 +5645,21 @@
       <c r="C13" s="27">
         <v>60</v>
       </c>
-      <c r="D13" s="58">
+      <c r="D13" s="56">
         <f>C13/$C$15</f>
         <v>4.5078888054094664E-2</v>
       </c>
       <c r="E13" s="27">
         <v>707</v>
       </c>
-      <c r="F13" s="58">
+      <c r="F13" s="56">
         <f>E13/$E$15</f>
         <v>0.10756123535676251</v>
       </c>
       <c r="G13" s="27">
         <v>59488</v>
       </c>
-      <c r="H13" s="58">
+      <c r="H13" s="56">
         <f>G13/$G$15</f>
         <v>0.4085573984409876</v>
       </c>
@@ -5310,21 +5671,21 @@
       <c r="C14" s="27">
         <v>1271</v>
       </c>
-      <c r="D14" s="58">
+      <c r="D14" s="56">
         <f t="shared" ref="D14:D20" si="3">C14/$C$15</f>
         <v>0.95492111194590534</v>
       </c>
       <c r="E14" s="27">
         <v>5866</v>
       </c>
-      <c r="F14" s="58">
+      <c r="F14" s="56">
         <f>E14/$E$15</f>
         <v>0.89243876464323746</v>
       </c>
       <c r="G14" s="27">
         <v>86117</v>
       </c>
-      <c r="H14" s="58">
+      <c r="H14" s="56">
         <f t="shared" ref="H14:H20" si="4">G14/$G$15</f>
         <v>0.5914426015590124</v>
       </c>
@@ -5337,21 +5698,24 @@
         <f>SUM(C13:C14)</f>
         <v>1331</v>
       </c>
-      <c r="D15" s="63" t="s">
-        <v>12</v>
+      <c r="D15" s="60">
+        <f>C15/C24</f>
+        <v>0.72891566265060237</v>
       </c>
       <c r="E15" s="27">
         <f>SUM(E13:E14)</f>
         <v>6573</v>
       </c>
-      <c r="F15" s="63" t="s">
-        <v>12</v>
+      <c r="F15" s="60">
+        <f>E15/C25</f>
+        <v>0.62869440459110471</v>
       </c>
       <c r="G15" s="27">
         <v>145605</v>
       </c>
-      <c r="H15" s="63" t="s">
-        <v>12</v>
+      <c r="H15" s="60">
+        <f>G15/C26</f>
+        <v>0.23814858914890971</v>
       </c>
     </row>
     <row r="16" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5359,11 +5723,11 @@
         <v>23</v>
       </c>
       <c r="C16" s="27"/>
-      <c r="D16" s="58"/>
+      <c r="D16" s="56"/>
       <c r="E16" s="27"/>
-      <c r="F16" s="58"/>
+      <c r="F16" s="56"/>
       <c r="G16" s="27"/>
-      <c r="H16" s="58"/>
+      <c r="H16" s="56"/>
     </row>
     <row r="17" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="46" t="s">
@@ -5372,21 +5736,21 @@
       <c r="C17" s="27">
         <v>175</v>
       </c>
-      <c r="D17" s="58">
+      <c r="D17" s="56">
         <f t="shared" si="3"/>
         <v>0.13148009015777612</v>
       </c>
       <c r="E17" s="27">
         <v>326</v>
       </c>
-      <c r="F17" s="58">
+      <c r="F17" s="56">
         <f>E17/$E$15</f>
         <v>4.9596835539327554E-2</v>
       </c>
       <c r="G17" s="27">
         <v>27519</v>
       </c>
-      <c r="H17" s="58">
+      <c r="H17" s="56">
         <f t="shared" si="4"/>
         <v>0.18899763057587307</v>
       </c>
@@ -5398,21 +5762,21 @@
       <c r="C18" s="27">
         <v>1121</v>
       </c>
-      <c r="D18" s="58">
+      <c r="D18" s="56">
         <f t="shared" si="3"/>
         <v>0.8422238918106687</v>
       </c>
       <c r="E18" s="27">
         <v>6043</v>
       </c>
-      <c r="F18" s="58">
+      <c r="F18" s="56">
         <f t="shared" ref="F18:F19" si="5">E18/$E$15</f>
         <v>0.91936710786551046</v>
       </c>
       <c r="G18" s="27">
         <v>116191</v>
       </c>
-      <c r="H18" s="58">
+      <c r="H18" s="56">
         <f t="shared" si="4"/>
         <v>0.79798770646612416</v>
       </c>
@@ -5424,21 +5788,21 @@
       <c r="C19" s="27">
         <v>327</v>
       </c>
-      <c r="D19" s="58">
+      <c r="D19" s="56">
         <f t="shared" si="3"/>
         <v>0.24567993989481593</v>
       </c>
       <c r="E19" s="27">
         <v>2167</v>
       </c>
-      <c r="F19" s="58">
+      <c r="F19" s="56">
         <f t="shared" si="5"/>
         <v>0.32968203255743189</v>
       </c>
       <c r="G19" s="27">
         <v>64122</v>
       </c>
-      <c r="H19" s="58">
+      <c r="H19" s="56">
         <f t="shared" si="4"/>
         <v>0.44038322859791901</v>
       </c>
@@ -5450,26 +5814,55 @@
       <c r="C20" s="33">
         <v>69</v>
       </c>
-      <c r="D20" s="60">
+      <c r="D20" s="57">
         <f t="shared" si="3"/>
         <v>5.1840721262208865E-2</v>
       </c>
       <c r="E20" s="33">
         <v>3876</v>
       </c>
-      <c r="F20" s="60">
+      <c r="F20" s="57">
         <f>E20/$E$15</f>
         <v>0.58968507530807845</v>
       </c>
       <c r="G20" s="33">
         <v>52069</v>
       </c>
-      <c r="H20" s="60">
+      <c r="H20" s="57">
         <f t="shared" si="4"/>
         <v>0.3576044778682051</v>
       </c>
     </row>
     <row r="21" spans="2:8" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C23" s="95" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25">
+        <v>10455</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26">
+        <v>611404</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B2:H2"/>
@@ -5485,10 +5878,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6087B295-164D-4F4E-913D-9E8EE4331FFD}">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5503,51 +5896,51 @@
   <sheetData>
     <row r="1" spans="2:14" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:14" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="74"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="71"/>
     </row>
     <row r="3" spans="2:14" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
     </row>
     <row r="4" spans="2:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="71"/>
-      <c r="C4" s="75" t="s">
+      <c r="B4" s="68"/>
+      <c r="C4" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="76"/>
-      <c r="E4" s="75" t="s">
+      <c r="D4" s="73"/>
+      <c r="E4" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="76"/>
-      <c r="G4" s="75" t="s">
+      <c r="F4" s="73"/>
+      <c r="G4" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="76"/>
-      <c r="I4" s="75" t="s">
+      <c r="H4" s="73"/>
+      <c r="I4" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="76"/>
+      <c r="J4" s="73"/>
     </row>
     <row r="5" spans="2:14" ht="43" x14ac:dyDescent="0.2">
       <c r="B5" s="39" t="s">
@@ -5585,26 +5978,30 @@
       <c r="C6" s="27">
         <v>12309</v>
       </c>
-      <c r="D6" s="57" t="s">
-        <v>12</v>
+      <c r="D6" s="60">
+        <f>C6/C25</f>
+        <v>0.6901984972524392</v>
       </c>
       <c r="E6" s="27">
         <v>3795</v>
       </c>
-      <c r="F6" s="57" t="s">
-        <v>12</v>
+      <c r="F6" s="60">
+        <f>E6/C26</f>
+        <v>0.72052401746724892</v>
       </c>
       <c r="G6" s="27">
         <v>20759</v>
       </c>
-      <c r="H6" s="57" t="s">
-        <v>12</v>
+      <c r="H6" s="60">
+        <f>G6/C27</f>
+        <v>0.70488964346349747</v>
       </c>
       <c r="I6" s="27">
         <v>465799</v>
       </c>
-      <c r="J6" s="57" t="s">
-        <v>12</v>
+      <c r="J6" s="60">
+        <f>I6/C28</f>
+        <v>0.76185141085109032</v>
       </c>
       <c r="L6" s="42"/>
       <c r="M6" s="42"/>
@@ -5634,28 +6031,28 @@
       <c r="C8" s="27">
         <v>7218</v>
       </c>
-      <c r="D8" s="58">
+      <c r="D8" s="56">
         <f>C8/$C$6</f>
         <v>0.58640019497928342</v>
       </c>
       <c r="E8" s="27">
         <v>2244</v>
       </c>
-      <c r="F8" s="58">
+      <c r="F8" s="56">
         <f>E8/$E$6</f>
         <v>0.59130434782608698</v>
       </c>
       <c r="G8" s="27">
         <v>12806</v>
       </c>
-      <c r="H8" s="58">
+      <c r="H8" s="56">
         <f>G8/$G$6</f>
         <v>0.61688906016667466</v>
       </c>
       <c r="I8" s="27">
         <v>313546</v>
       </c>
-      <c r="J8" s="58">
+      <c r="J8" s="56">
         <f>I8/$I$6</f>
         <v>0.67313583756083628</v>
       </c>
@@ -5671,28 +6068,28 @@
       <c r="C9" s="27">
         <v>3344</v>
       </c>
-      <c r="D9" s="58">
+      <c r="D9" s="56">
         <f t="shared" ref="D9:D11" si="0">C9/$C$6</f>
         <v>0.27167113494191242</v>
       </c>
       <c r="E9" s="27">
         <v>1104</v>
       </c>
-      <c r="F9" s="58">
+      <c r="F9" s="56">
         <f t="shared" ref="F9:F11" si="1">E9/$E$6</f>
         <v>0.29090909090909089</v>
       </c>
       <c r="G9" s="27">
         <v>5482</v>
       </c>
-      <c r="H9" s="58">
+      <c r="H9" s="56">
         <f t="shared" ref="H9:H11" si="2">G9/$G$6</f>
         <v>0.26407823112866707</v>
       </c>
       <c r="I9" s="27">
         <v>111647</v>
       </c>
-      <c r="J9" s="58">
+      <c r="J9" s="56">
         <f t="shared" ref="J9:J11" si="3">I9/$I$6</f>
         <v>0.23968922217523009</v>
       </c>
@@ -5708,28 +6105,28 @@
       <c r="C10" s="27">
         <v>3163</v>
       </c>
-      <c r="D10" s="58">
+      <c r="D10" s="56">
         <f t="shared" si="0"/>
         <v>0.25696644731497276</v>
       </c>
       <c r="E10" s="27">
         <v>1048</v>
       </c>
-      <c r="F10" s="58">
+      <c r="F10" s="56">
         <f t="shared" si="1"/>
         <v>0.2761528326745718</v>
       </c>
       <c r="G10" s="27">
         <v>5195</v>
       </c>
-      <c r="H10" s="58">
+      <c r="H10" s="56">
         <f t="shared" si="2"/>
         <v>0.25025290235560482</v>
       </c>
       <c r="I10" s="27">
         <v>92192</v>
       </c>
-      <c r="J10" s="58">
+      <c r="J10" s="56">
         <f t="shared" si="3"/>
         <v>0.19792227978162255</v>
       </c>
@@ -5745,28 +6142,28 @@
       <c r="C11" s="27">
         <v>181</v>
       </c>
-      <c r="D11" s="58">
+      <c r="D11" s="56">
         <f t="shared" si="0"/>
         <v>1.4704687626939638E-2</v>
       </c>
       <c r="E11" s="27">
         <v>56</v>
       </c>
-      <c r="F11" s="58">
+      <c r="F11" s="56">
         <f t="shared" si="1"/>
         <v>1.4756258234519103E-2</v>
       </c>
       <c r="G11" s="27">
         <v>287</v>
       </c>
-      <c r="H11" s="58">
+      <c r="H11" s="56">
         <f t="shared" si="2"/>
         <v>1.3825328773062286E-2</v>
       </c>
       <c r="I11" s="27">
         <v>19455</v>
       </c>
-      <c r="J11" s="58">
+      <c r="J11" s="56">
         <f t="shared" si="3"/>
         <v>4.1766942393607544E-2</v>
       </c>
@@ -5813,28 +6210,28 @@
       <c r="C13" s="27">
         <v>3049</v>
       </c>
-      <c r="D13" s="58">
+      <c r="D13" s="56">
         <f>C13/$C$15</f>
         <v>0.55185520361990947</v>
       </c>
       <c r="E13" s="27">
         <v>882</v>
       </c>
-      <c r="F13" s="58">
+      <c r="F13" s="56">
         <f>E13/$E$15</f>
         <v>0.59918478260869568</v>
       </c>
       <c r="G13" s="27">
         <v>4760</v>
       </c>
-      <c r="H13" s="58">
+      <c r="H13" s="56">
         <f>G13/$G$15</f>
         <v>0.54769301576343343</v>
       </c>
       <c r="I13" s="27">
         <v>59488</v>
       </c>
-      <c r="J13" s="58">
+      <c r="J13" s="56">
         <f>I13/$I$15</f>
         <v>0.4085573984409876</v>
       </c>
@@ -5846,28 +6243,28 @@
       <c r="C14" s="27">
         <v>2476</v>
       </c>
-      <c r="D14" s="58">
+      <c r="D14" s="56">
         <f t="shared" ref="D14:D20" si="4">C14/$C$15</f>
         <v>0.44814479638009047</v>
       </c>
       <c r="E14" s="27">
         <v>590</v>
       </c>
-      <c r="F14" s="58">
+      <c r="F14" s="56">
         <f t="shared" ref="F14:F20" si="5">E14/$E$15</f>
         <v>0.40081521739130432</v>
       </c>
       <c r="G14" s="27">
         <v>3931</v>
       </c>
-      <c r="H14" s="58">
+      <c r="H14" s="56">
         <f t="shared" ref="H14:H20" si="6">G14/$G$15</f>
         <v>0.45230698423656657</v>
       </c>
       <c r="I14" s="27">
         <v>86117</v>
       </c>
-      <c r="J14" s="58">
+      <c r="J14" s="56">
         <f t="shared" ref="J14:J20" si="7">I14/$I$15</f>
         <v>0.5914426015590124</v>
       </c>
@@ -5880,28 +6277,32 @@
         <f>SUM(C13:C14)</f>
         <v>5525</v>
       </c>
-      <c r="D15" s="63" t="s">
-        <v>12</v>
+      <c r="D15" s="60">
+        <f>C15/C25</f>
+        <v>0.30980150274756085</v>
       </c>
       <c r="E15" s="27">
         <f t="shared" ref="E15:G15" si="8">SUM(E13:E14)</f>
         <v>1472</v>
       </c>
-      <c r="F15" s="63" t="s">
-        <v>12</v>
+      <c r="F15" s="60">
+        <f>E15/C26</f>
+        <v>0.27947598253275108</v>
       </c>
       <c r="G15" s="27">
         <f t="shared" si="8"/>
         <v>8691</v>
       </c>
-      <c r="H15" s="63" t="s">
-        <v>12</v>
+      <c r="H15" s="60">
+        <f>G15/C27</f>
+        <v>0.29511035653650253</v>
       </c>
       <c r="I15" s="27">
         <v>145605</v>
       </c>
-      <c r="J15" s="63" t="s">
-        <v>12</v>
+      <c r="J15" s="60">
+        <f>I15/C28</f>
+        <v>0.23814858914890971</v>
       </c>
     </row>
     <row r="16" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5909,13 +6310,13 @@
         <v>23</v>
       </c>
       <c r="C16" s="27"/>
-      <c r="D16" s="58"/>
+      <c r="D16" s="56"/>
       <c r="E16" s="27"/>
-      <c r="F16" s="58"/>
+      <c r="F16" s="56"/>
       <c r="G16" s="27"/>
-      <c r="H16" s="58"/>
+      <c r="H16" s="56"/>
       <c r="I16" s="27"/>
-      <c r="J16" s="58"/>
+      <c r="J16" s="56"/>
     </row>
     <row r="17" spans="2:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="36" t="s">
@@ -5924,28 +6325,28 @@
       <c r="C17" s="27">
         <v>1003</v>
       </c>
-      <c r="D17" s="58">
+      <c r="D17" s="56">
         <f t="shared" si="4"/>
         <v>0.18153846153846154</v>
       </c>
       <c r="E17" s="27">
         <v>512</v>
       </c>
-      <c r="F17" s="58">
+      <c r="F17" s="56">
         <f t="shared" si="5"/>
         <v>0.34782608695652173</v>
       </c>
       <c r="G17" s="27">
         <v>2214</v>
       </c>
-      <c r="H17" s="58">
+      <c r="H17" s="56">
         <f t="shared" si="6"/>
         <v>0.25474628926475662</v>
       </c>
       <c r="I17" s="27">
         <v>27519</v>
       </c>
-      <c r="J17" s="58">
+      <c r="J17" s="56">
         <f t="shared" si="7"/>
         <v>0.18899763057587307</v>
       </c>
@@ -5957,28 +6358,28 @@
       <c r="C18" s="27">
         <v>4427</v>
       </c>
-      <c r="D18" s="58">
+      <c r="D18" s="56">
         <f t="shared" si="4"/>
         <v>0.80126696832579181</v>
       </c>
       <c r="E18" s="27">
         <v>954</v>
       </c>
-      <c r="F18" s="58">
+      <c r="F18" s="56">
         <f t="shared" si="5"/>
         <v>0.64809782608695654</v>
       </c>
       <c r="G18" s="27">
         <v>6376</v>
       </c>
-      <c r="H18" s="58">
+      <c r="H18" s="56">
         <f t="shared" si="6"/>
         <v>0.73363249338396042</v>
       </c>
       <c r="I18" s="27">
         <v>116191</v>
       </c>
-      <c r="J18" s="58">
+      <c r="J18" s="56">
         <f t="shared" si="7"/>
         <v>0.79798770646612416</v>
       </c>
@@ -5990,28 +6391,28 @@
       <c r="C19" s="27">
         <v>3188</v>
       </c>
-      <c r="D19" s="58">
+      <c r="D19" s="56">
         <f t="shared" si="4"/>
         <v>0.57701357466063352</v>
       </c>
       <c r="E19" s="27">
         <v>598</v>
       </c>
-      <c r="F19" s="58">
+      <c r="F19" s="56">
         <f t="shared" si="5"/>
         <v>0.40625</v>
       </c>
       <c r="G19" s="27">
         <v>4413</v>
       </c>
-      <c r="H19" s="58">
+      <c r="H19" s="56">
         <f t="shared" si="6"/>
         <v>0.50776665516051089</v>
       </c>
       <c r="I19" s="27">
         <v>64122</v>
       </c>
-      <c r="J19" s="58">
+      <c r="J19" s="56">
         <f t="shared" si="7"/>
         <v>0.44038322859791901</v>
       </c>
@@ -6023,33 +6424,70 @@
       <c r="C20" s="33">
         <v>1239</v>
       </c>
-      <c r="D20" s="60">
+      <c r="D20" s="57">
         <f t="shared" si="4"/>
         <v>0.22425339366515837</v>
       </c>
       <c r="E20" s="33">
         <v>356</v>
       </c>
-      <c r="F20" s="60">
+      <c r="F20" s="57">
         <f t="shared" si="5"/>
         <v>0.24184782608695651</v>
       </c>
       <c r="G20" s="33">
         <v>1963</v>
       </c>
-      <c r="H20" s="60">
+      <c r="H20" s="57">
         <f t="shared" si="6"/>
         <v>0.22586583822344955</v>
       </c>
       <c r="I20" s="33">
         <v>52069</v>
       </c>
-      <c r="J20" s="60">
+      <c r="J20" s="57">
         <f t="shared" si="7"/>
         <v>0.3576044778682051</v>
       </c>
     </row>
     <row r="21" spans="2:10" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C24" s="95" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25">
+        <v>17834</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26">
+        <v>5267</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27">
+        <v>29450</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28">
+        <v>611404</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="B2:J2"/>
@@ -6090,61 +6528,61 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="83" t="s">
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="83"/>
-      <c r="L2" s="83"/>
-      <c r="M2" s="83"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
     </row>
     <row r="3" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="84"/>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="85" t="s">
+      <c r="A3" s="81"/>
+      <c r="B3" s="81"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="86"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="91" t="s">
+      <c r="F3" s="83"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="92"/>
-      <c r="J3" s="92"/>
-      <c r="K3" s="92"/>
-      <c r="L3" s="92"/>
-      <c r="M3" s="93"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="90"/>
     </row>
     <row r="4" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="84"/>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="89"/>
-      <c r="G4" s="90"/>
-      <c r="H4" s="94" t="s">
+      <c r="A4" s="81"/>
+      <c r="B4" s="81"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="95"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="94" t="s">
+      <c r="I4" s="92"/>
+      <c r="J4" s="93"/>
+      <c r="K4" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="95"/>
-      <c r="M4" s="96"/>
+      <c r="L4" s="92"/>
+      <c r="M4" s="93"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>

</xml_diff>

<commit_message>
updates to percentages (fixing data inaccuracies)
</commit_message>
<xml_diff>
--- a/AAJC Vis/case_studies/citizenship_english_ability_tables.xlsx
+++ b/AAJC Vis/case_studies/citizenship_english_ability_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anamkhan/Documents/Demo Advisors/AAJC/AAJC Vis/case_studies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F365CCB8-50C9-BB4A-9071-6626EC7FE0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3B507A-758F-104E-B9BA-2FDC57BD9AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17200" activeTab="3" xr2:uid="{7F9E964A-6C9F-BE4C-A5F8-FD2379A71560}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17140" xr2:uid="{7F9E964A-6C9F-BE4C-A5F8-FD2379A71560}"/>
   </bookViews>
   <sheets>
     <sheet name="Los Angeles CA" sheetId="2" r:id="rId1"/>
@@ -889,6 +889,11 @@
     </xf>
     <xf numFmtId="1" fontId="7" fillId="5" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="7" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="7" fillId="5" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -972,11 +977,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="7" fillId="5" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1309,8 +1309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93FEEA31-4AC1-9A41-82B8-056A272FB033}">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1326,31 +1326,31 @@
   <sheetData>
     <row r="1" spans="2:12" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:12" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="71"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="74"/>
       <c r="L2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
       <c r="K3" t="s">
         <v>69</v>
       </c>
@@ -1359,19 +1359,19 @@
       </c>
     </row>
     <row r="4" spans="2:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="68"/>
-      <c r="C4" s="72" t="s">
+      <c r="B4" s="71"/>
+      <c r="C4" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="73"/>
-      <c r="E4" s="72" t="s">
+      <c r="D4" s="76"/>
+      <c r="E4" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="73"/>
-      <c r="G4" s="72" t="s">
+      <c r="F4" s="76"/>
+      <c r="G4" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="73"/>
+      <c r="H4" s="76"/>
       <c r="K4" t="s">
         <v>68</v>
       </c>
@@ -1453,22 +1453,22 @@
         <v>249508</v>
       </c>
       <c r="D8" s="53">
-        <f>C8/$C$6</f>
-        <v>0.4769193716717065</v>
+        <f>C8/SUM($C$8:$C$9)</f>
+        <v>0.55514690340308603</v>
       </c>
       <c r="E8" s="27">
         <v>1076101</v>
       </c>
       <c r="F8" s="53">
-        <f>E8/$E$6</f>
-        <v>0.49038484761900858</v>
+        <f>E8/SUM($E$8:$E$9)</f>
+        <v>0.56477627826371735</v>
       </c>
       <c r="G8" s="27">
         <v>3006846</v>
       </c>
       <c r="H8" s="56">
-        <f>G8/$G$6</f>
-        <v>0.4709236355161952</v>
+        <f>G8/SUM($G$8:$G$9)</f>
+        <v>0.55072436692759186</v>
       </c>
       <c r="J8" s="26"/>
       <c r="K8" s="26"/>
@@ -1482,22 +1482,22 @@
         <v>199937</v>
       </c>
       <c r="D9" s="53">
-        <f t="shared" ref="D9:D11" si="0">C9/$C$6</f>
-        <v>0.38216741913656471</v>
+        <f t="shared" ref="D9:D11" si="0">C9/SUM($C$8:$C$9)</f>
+        <v>0.44485309659691397</v>
       </c>
       <c r="E9" s="27">
         <v>829257</v>
       </c>
       <c r="F9" s="53">
-        <f t="shared" ref="F9:F11" si="1">E9/$E$6</f>
-        <v>0.37789674722167915</v>
+        <f t="shared" ref="F9:F11" si="1">E9/SUM($E$8:$E$9)</f>
+        <v>0.43522372173628265</v>
       </c>
       <c r="G9" s="27">
         <v>2452956</v>
       </c>
       <c r="H9" s="56">
-        <f t="shared" ref="H9:H11" si="2">G9/$G$6</f>
-        <v>0.38417496515660071</v>
+        <f t="shared" ref="H9:H11" si="2">G9/SUM($G$8:$G$9)</f>
+        <v>0.44927563307240814</v>
       </c>
       <c r="J9" s="26"/>
       <c r="K9" s="26"/>
@@ -1512,21 +1512,21 @@
       </c>
       <c r="D10" s="53">
         <f t="shared" si="0"/>
-        <v>0.31991184442414072</v>
+        <v>0.37238594266261721</v>
       </c>
       <c r="E10" s="27">
         <v>692291</v>
       </c>
       <c r="F10" s="53">
         <f t="shared" si="1"/>
-        <v>0.31548062546453454</v>
+        <v>0.36333906803865729</v>
       </c>
       <c r="G10" s="27">
         <v>2058825</v>
       </c>
       <c r="H10" s="56">
         <f t="shared" si="2"/>
-        <v>0.32244729324070159</v>
+        <v>0.37708785043853238</v>
       </c>
       <c r="J10" s="26"/>
       <c r="K10" s="26"/>
@@ -1541,21 +1541,21 @@
       </c>
       <c r="D11" s="53">
         <f t="shared" si="0"/>
-        <v>6.2255574712423975E-2</v>
+        <v>7.2467153934296744E-2</v>
       </c>
       <c r="E11" s="27">
         <v>136966</v>
       </c>
       <c r="F11" s="53">
         <f t="shared" si="1"/>
-        <v>6.2416121757144657E-2</v>
+        <v>7.1884653697625325E-2</v>
       </c>
       <c r="G11" s="27">
         <v>394131</v>
       </c>
-      <c r="H11" s="56">
+      <c r="H11" s="57">
         <f t="shared" si="2"/>
-        <v>6.1727671915899097E-2</v>
+        <v>7.2187782633875736E-2</v>
       </c>
       <c r="J11" s="26"/>
       <c r="K11" s="26"/>
@@ -1686,22 +1686,22 @@
         <v>90751</v>
       </c>
       <c r="D17" s="53">
-        <f t="shared" si="3"/>
-        <v>9.3997679862448988E-2</v>
+        <f>C17/SUM($C$17:$C$18)</f>
+        <v>9.4446895931595179E-2</v>
       </c>
       <c r="E17" s="27">
         <v>383034</v>
       </c>
       <c r="F17" s="53">
-        <f t="shared" si="4"/>
-        <v>0.10523169385185517</v>
+        <f>E17/SUM($E$17:$E$18)</f>
+        <v>0.10586992477545407</v>
       </c>
       <c r="G17" s="27">
         <v>1552111</v>
       </c>
       <c r="H17" s="56">
-        <f t="shared" si="5"/>
-        <v>0.12894885948238047</v>
+        <f>G17/SUM($G$17:$G$18)</f>
+        <v>0.13003683918131914</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
@@ -1712,22 +1712,22 @@
         <v>870117</v>
       </c>
       <c r="D18" s="53">
-        <f t="shared" si="3"/>
-        <v>0.90124603815797655</v>
+        <f t="shared" ref="D18:D20" si="7">C18/SUM($C$17:$C$18)</f>
+        <v>0.90555310406840483</v>
       </c>
       <c r="E18" s="27">
         <v>3234934</v>
       </c>
       <c r="F18" s="53">
-        <f t="shared" si="4"/>
-        <v>0.88873986204607747</v>
+        <f t="shared" ref="F18:F20" si="8">E18/SUM($E$17:$E$18)</f>
+        <v>0.89413007522454591</v>
       </c>
       <c r="G18" s="27">
         <v>10383822</v>
       </c>
       <c r="H18" s="56">
-        <f t="shared" si="5"/>
-        <v>0.86268443685280938</v>
+        <f t="shared" ref="H18:H20" si="9">G18/SUM($G$17:$G$18)</f>
+        <v>0.86996316081868086</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
@@ -1738,22 +1738,22 @@
         <v>365473</v>
       </c>
       <c r="D19" s="53">
-        <f t="shared" si="3"/>
-        <v>0.37854804963437116</v>
+        <f t="shared" si="7"/>
+        <v>0.380357135423388</v>
       </c>
       <c r="E19" s="27">
         <v>1529010</v>
       </c>
       <c r="F19" s="53">
-        <f t="shared" si="4"/>
-        <v>0.42006796320019912</v>
+        <f t="shared" si="8"/>
+        <v>0.42261567819284196</v>
       </c>
       <c r="G19" s="27">
         <v>5231985</v>
       </c>
       <c r="H19" s="56">
-        <f t="shared" si="5"/>
-        <v>0.43467155285860504</v>
+        <f t="shared" si="9"/>
+        <v>0.43833900542169596</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
@@ -1764,22 +1764,22 @@
         <v>504644</v>
       </c>
       <c r="D20" s="61">
-        <f t="shared" si="3"/>
-        <v>0.52269798852360527</v>
+        <f t="shared" si="7"/>
+        <v>0.52519596864501683</v>
       </c>
       <c r="E20" s="33">
         <v>1705924</v>
       </c>
       <c r="F20" s="61">
-        <f t="shared" si="4"/>
-        <v>0.4686718988458784</v>
+        <f t="shared" si="8"/>
+        <v>0.471514397031704</v>
       </c>
       <c r="G20" s="33">
         <v>5151837</v>
       </c>
       <c r="H20" s="57">
-        <f t="shared" si="5"/>
-        <v>0.42801288399420434</v>
+        <f t="shared" si="9"/>
+        <v>0.4316241553969849</v>
       </c>
     </row>
     <row r="21" spans="2:12" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -1790,43 +1790,43 @@
     </row>
     <row r="25" spans="2:12" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="26" spans="2:12" ht="21" x14ac:dyDescent="0.2">
-      <c r="B26" s="69" t="s">
+      <c r="B26" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="70"/>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70"/>
-      <c r="F26" s="70"/>
-      <c r="G26" s="70"/>
-      <c r="H26" s="71"/>
+      <c r="C26" s="73"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="73"/>
+      <c r="F26" s="73"/>
+      <c r="G26" s="73"/>
+      <c r="H26" s="74"/>
     </row>
     <row r="27" spans="2:12" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="67" t="s">
+      <c r="B27" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="66" t="s">
+      <c r="C27" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="66"/>
-      <c r="E27" s="66"/>
-      <c r="F27" s="66"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="66"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="69"/>
+      <c r="G27" s="69"/>
+      <c r="H27" s="69"/>
     </row>
     <row r="28" spans="2:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="68"/>
-      <c r="C28" s="72" t="s">
+      <c r="B28" s="71"/>
+      <c r="C28" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="73"/>
-      <c r="E28" s="72" t="s">
+      <c r="D28" s="76"/>
+      <c r="E28" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="F28" s="73"/>
-      <c r="G28" s="72" t="s">
+      <c r="F28" s="76"/>
+      <c r="G28" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="H28" s="73"/>
+      <c r="H28" s="76"/>
       <c r="L28" t="s">
         <v>62</v>
       </c>
@@ -1919,22 +1919,22 @@
         <v>11244</v>
       </c>
       <c r="D32" s="56">
-        <f>C32/$C$30</f>
-        <v>0.59385232914334007</v>
+        <f>C32/SUM($C$32:$C$33)</f>
+        <v>0.63944494995450407</v>
       </c>
       <c r="E32" s="27">
         <v>69262</v>
       </c>
       <c r="F32" s="56">
-        <f>E32/$E$30</f>
-        <v>0.6480897530667814</v>
+        <f>E32/SUM($E$32:$E$33)</f>
+        <v>0.6968568898905344</v>
       </c>
       <c r="G32" s="27">
         <v>313546</v>
       </c>
       <c r="H32" s="56">
-        <f>G32/$G$30</f>
-        <v>0.67313583756083628</v>
+        <f>G32/SUM($G$32:$G$33)</f>
+        <v>0.73742041849230822</v>
       </c>
       <c r="J32" s="25"/>
       <c r="K32" s="25"/>
@@ -1948,22 +1948,22 @@
         <v>6340</v>
       </c>
       <c r="D33" s="56">
-        <f t="shared" ref="D33:D35" si="7">C33/$C$30</f>
-        <v>0.33484736452941799</v>
+        <f t="shared" ref="D33:D35" si="10">C33/SUM($C$32:$C$33)</f>
+        <v>0.36055505004549593</v>
       </c>
       <c r="E33" s="27">
         <v>30130</v>
       </c>
       <c r="F33" s="56">
-        <f t="shared" ref="F33:F35" si="8">E33/$E$30</f>
-        <v>0.28192868037166302</v>
+        <f t="shared" ref="F33:F35" si="11">E33/SUM($E$32:$E$33)</f>
+        <v>0.30314311010946554</v>
       </c>
       <c r="G33" s="27">
         <v>111647</v>
       </c>
       <c r="H33" s="56">
-        <f t="shared" ref="H33:H35" si="9">G33/$G$30</f>
-        <v>0.23968922217523009</v>
+        <f t="shared" ref="H33:H35" si="12">G33/SUM($G$32:$G$33)</f>
+        <v>0.26257958150769178</v>
       </c>
       <c r="J33" s="25"/>
       <c r="K33" s="25"/>
@@ -1977,22 +1977,22 @@
         <v>5673</v>
       </c>
       <c r="D34" s="56">
-        <f t="shared" si="7"/>
-        <v>0.29961973169958805</v>
+        <f t="shared" si="10"/>
+        <v>0.32262283894449501</v>
       </c>
       <c r="E34" s="27">
         <v>25191</v>
       </c>
       <c r="F34" s="56">
-        <f t="shared" si="8"/>
-        <v>0.23571408520552817</v>
+        <f t="shared" si="11"/>
+        <v>0.25345098197037991</v>
       </c>
       <c r="G34" s="27">
         <v>92192</v>
       </c>
       <c r="H34" s="56">
-        <f t="shared" si="9"/>
-        <v>0.19792227978162255</v>
+        <f t="shared" si="12"/>
+        <v>0.21682388938670205</v>
       </c>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.2">
@@ -2003,22 +2003,22 @@
         <v>667</v>
       </c>
       <c r="D35" s="56">
-        <f t="shared" si="7"/>
-        <v>3.5227632829829936E-2</v>
+        <f t="shared" si="10"/>
+        <v>3.7932211101000909E-2</v>
       </c>
       <c r="E35" s="27">
         <v>4939</v>
       </c>
       <c r="F35" s="56">
-        <f t="shared" si="8"/>
-        <v>4.6214595166134874E-2</v>
+        <f t="shared" si="11"/>
+        <v>4.9692128139085641E-2</v>
       </c>
       <c r="G35" s="27">
         <v>19455</v>
       </c>
       <c r="H35" s="56">
-        <f t="shared" si="9"/>
-        <v>4.1766942393607544E-2</v>
+        <f t="shared" si="12"/>
+        <v>4.575569212098976E-2</v>
       </c>
     </row>
     <row r="36" spans="2:12" ht="43" x14ac:dyDescent="0.2">
@@ -2078,21 +2078,21 @@
         <v>2735</v>
       </c>
       <c r="D38" s="56">
-        <f t="shared" ref="D38:D44" si="10">C38/$C$39</f>
+        <f t="shared" ref="D38:D44" si="13">C38/$C$39</f>
         <v>0.4458754483208347</v>
       </c>
       <c r="E38" s="27">
         <v>17066</v>
       </c>
       <c r="F38" s="56">
-        <f t="shared" ref="F38:F44" si="11">E38/$E$39</f>
+        <f t="shared" ref="F38:F44" si="14">E38/$E$39</f>
         <v>0.39906465567637084</v>
       </c>
       <c r="G38" s="27">
         <v>86117</v>
       </c>
       <c r="H38" s="56">
-        <f t="shared" ref="H38:H44" si="12">G38/$G$39</f>
+        <f t="shared" ref="H38:H44" si="15">G38/$G$39</f>
         <v>0.5914426015590124</v>
       </c>
     </row>
@@ -2109,7 +2109,7 @@
         <v>0.2446944311472794</v>
       </c>
       <c r="E39" s="27">
-        <f t="shared" ref="E39" si="13">SUM(E37:E38)</f>
+        <f t="shared" ref="E39" si="16">SUM(E37:E38)</f>
         <v>42765</v>
       </c>
       <c r="F39" s="60">
@@ -2143,22 +2143,22 @@
         <v>933</v>
       </c>
       <c r="D41" s="56">
-        <f t="shared" si="10"/>
+        <f>C41/SUM($C$41:$C$42)</f>
         <v>0.1521030322791001</v>
       </c>
       <c r="E41" s="27">
         <v>6348</v>
       </c>
       <c r="F41" s="56">
-        <f t="shared" si="11"/>
-        <v>0.14843914415994389</v>
+        <f>E41/SUM($E$41:$E$42)</f>
+        <v>0.14967109141065241</v>
       </c>
       <c r="G41" s="27">
         <v>27519</v>
       </c>
       <c r="H41" s="56">
-        <f t="shared" si="12"/>
-        <v>0.18899763057587307</v>
+        <f>G41/SUM($G$41:$G$42)</f>
+        <v>0.19148980585902164</v>
       </c>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.2">
@@ -2169,22 +2169,22 @@
         <v>5201</v>
       </c>
       <c r="D42" s="56">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="D42:D44" si="17">C42/SUM($C$41:$C$42)</f>
         <v>0.84789696772089995</v>
       </c>
       <c r="E42" s="27">
         <v>36065</v>
       </c>
       <c r="F42" s="56">
-        <f t="shared" si="11"/>
-        <v>0.84332982579211968</v>
+        <f t="shared" ref="F42:F44" si="18">E42/SUM($E$41:$E$42)</f>
+        <v>0.85032890858934762</v>
       </c>
       <c r="G42" s="27">
         <v>116191</v>
       </c>
       <c r="H42" s="56">
-        <f t="shared" si="12"/>
-        <v>0.79798770646612416</v>
+        <f t="shared" ref="H42:H44" si="19">G42/SUM($G$41:$G$42)</f>
+        <v>0.80851019414097836</v>
       </c>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.2">
@@ -2195,22 +2195,22 @@
         <v>3413</v>
       </c>
       <c r="D43" s="56">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>0.55640691229214212</v>
       </c>
       <c r="E43" s="27">
         <v>23906</v>
       </c>
       <c r="F43" s="56">
-        <f t="shared" si="11"/>
-        <v>0.55900853501695313</v>
+        <f t="shared" si="18"/>
+        <v>0.56364793813217651</v>
       </c>
       <c r="G43" s="27">
         <v>64122</v>
       </c>
       <c r="H43" s="56">
-        <f t="shared" si="12"/>
-        <v>0.44038322859791901</v>
+        <f t="shared" si="19"/>
+        <v>0.44619024424187598</v>
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.2">
@@ -2221,22 +2221,22 @@
         <v>1788</v>
       </c>
       <c r="D44" s="57">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>0.29149005542875772</v>
       </c>
       <c r="E44" s="33">
         <v>12159</v>
       </c>
       <c r="F44" s="57">
-        <f t="shared" si="11"/>
-        <v>0.2843212907751666</v>
+        <f t="shared" si="18"/>
+        <v>0.28668097045717117</v>
       </c>
       <c r="G44" s="33">
         <v>52069</v>
       </c>
       <c r="H44" s="57">
-        <f t="shared" si="12"/>
-        <v>0.3576044778682051</v>
+        <f t="shared" si="19"/>
+        <v>0.36231994989910238</v>
       </c>
     </row>
     <row r="45" spans="2:12" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -2265,7 +2265,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2280,43 +2280,43 @@
   <sheetData>
     <row r="1" spans="2:12" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:12" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="71"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="74"/>
     </row>
     <row r="3" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
     </row>
     <row r="4" spans="2:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="68"/>
-      <c r="C4" s="72" t="s">
+      <c r="B4" s="71"/>
+      <c r="C4" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="73"/>
-      <c r="E4" s="74" t="s">
+      <c r="D4" s="76"/>
+      <c r="E4" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="73"/>
-      <c r="G4" s="72" t="s">
+      <c r="F4" s="76"/>
+      <c r="G4" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="73"/>
+      <c r="H4" s="76"/>
     </row>
     <row r="5" spans="2:12" ht="43" x14ac:dyDescent="0.2">
       <c r="B5" s="39" t="s">
@@ -2386,22 +2386,22 @@
         <v>36276</v>
       </c>
       <c r="D8" s="56">
-        <f>C8/$C$6</f>
-        <v>0.35834518729255571</v>
+        <f>C8/SUM($C$8:$C$9)</f>
+        <v>0.43212464859198552</v>
       </c>
       <c r="E8" s="27">
         <v>178909</v>
       </c>
       <c r="F8" s="56">
-        <f>E8/$E$6</f>
-        <v>0.39557220211418176</v>
+        <f>E8/SUM($E$8:$E$9)</f>
+        <v>0.4829752369537107</v>
       </c>
       <c r="G8" s="27">
         <v>3006846</v>
       </c>
       <c r="H8" s="56">
-        <f>G8/$G$6</f>
-        <v>0.4709236355161952</v>
+        <f>G8/SUM($G$8:$G$9)</f>
+        <v>0.55072436692759186</v>
       </c>
       <c r="J8" s="41"/>
       <c r="K8" s="41"/>
@@ -2415,22 +2415,22 @@
         <v>47672</v>
       </c>
       <c r="D9" s="56">
-        <f t="shared" ref="D9:D11" si="0">C9/$C$6</f>
-        <v>0.47091828670776037</v>
+        <f t="shared" ref="D9:D11" si="0">C9/SUM($C$8:$C$9)</f>
+        <v>0.56787535140801448</v>
       </c>
       <c r="E9" s="27">
         <v>191522</v>
       </c>
       <c r="F9" s="56">
-        <f t="shared" ref="F9:F11" si="1">E9/$E$6</f>
-        <v>0.42345985553165194</v>
+        <f t="shared" ref="F9:F11" si="1">E9/SUM($E$8:$E$9)</f>
+        <v>0.5170247630462893</v>
       </c>
       <c r="G9" s="27">
         <v>2452956</v>
       </c>
       <c r="H9" s="56">
-        <f t="shared" ref="H9:H11" si="2">G9/$G$6</f>
-        <v>0.38417496515660071</v>
+        <f t="shared" ref="H9:H11" si="2">G9/SUM($G$8:$G$9)</f>
+        <v>0.44927563307240814</v>
       </c>
       <c r="J9" s="41"/>
       <c r="K9" s="41"/>
@@ -2445,21 +2445,21 @@
       </c>
       <c r="D10" s="56">
         <f t="shared" si="0"/>
-        <v>0.40336059743954483</v>
+        <v>0.48640825272787919</v>
       </c>
       <c r="E10" s="27">
         <v>165329</v>
       </c>
       <c r="F10" s="56">
         <f t="shared" si="1"/>
-        <v>0.3655464878979568</v>
+        <v>0.44631523819550739</v>
       </c>
       <c r="G10" s="27">
         <v>2058825</v>
       </c>
       <c r="H10" s="56">
         <f t="shared" si="2"/>
-        <v>0.32244729324070159</v>
+        <v>0.37708785043853238</v>
       </c>
       <c r="J10" s="41"/>
       <c r="K10" s="41"/>
@@ -2474,21 +2474,21 @@
       </c>
       <c r="D11" s="56">
         <f t="shared" si="0"/>
-        <v>6.7557689268215579E-2</v>
+        <v>8.1467098680135325E-2</v>
       </c>
       <c r="E11" s="27">
         <v>26193</v>
       </c>
       <c r="F11" s="56">
         <f t="shared" si="1"/>
-        <v>5.7913367633695131E-2</v>
+        <v>7.0709524850781927E-2</v>
       </c>
       <c r="G11" s="27">
         <v>394131</v>
       </c>
       <c r="H11" s="56">
         <f t="shared" si="2"/>
-        <v>6.1727671915899097E-2</v>
+        <v>7.2187782633875736E-2</v>
       </c>
       <c r="J11" s="41"/>
       <c r="K11" s="41"/>
@@ -2619,22 +2619,22 @@
         <v>22501</v>
       </c>
       <c r="D17" s="56">
-        <f t="shared" si="3"/>
-        <v>9.8224614430955537E-2</v>
+        <f>C17/SUM($C$17:$C$18)</f>
+        <v>9.9368924964339175E-2</v>
       </c>
       <c r="E17" s="27">
         <v>106935</v>
       </c>
       <c r="F17" s="56">
-        <f t="shared" si="4"/>
-        <v>0.1109992370651401</v>
+        <f>E17/SUM($E$17:$E$18)</f>
+        <v>0.1122290696746947</v>
       </c>
       <c r="G17" s="27">
         <v>1552111</v>
       </c>
       <c r="H17" s="56">
-        <f t="shared" si="5"/>
-        <v>0.12894885948238047</v>
+        <f>G17/SUM($G$17:$G$18)</f>
+        <v>0.13003683918131914</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
@@ -2645,22 +2645,22 @@
         <v>203938</v>
       </c>
       <c r="D18" s="56">
-        <f t="shared" si="3"/>
-        <v>0.89025960703169682</v>
+        <f t="shared" ref="D18:D20" si="7">C18/SUM($C$17:$C$18)</f>
+        <v>0.90063107503566087</v>
       </c>
       <c r="E18" s="27">
         <v>845893</v>
       </c>
       <c r="F18" s="56">
-        <f t="shared" si="4"/>
-        <v>0.87804252713089781</v>
+        <f t="shared" ref="F18:F20" si="8">E18/SUM($E$17:$E$18)</f>
+        <v>0.8877709303253053</v>
       </c>
       <c r="G18" s="27">
         <v>10383822</v>
       </c>
       <c r="H18" s="56">
-        <f t="shared" si="5"/>
-        <v>0.86268443685280938</v>
+        <f t="shared" ref="H18:H20" si="9">G18/SUM($G$17:$G$18)</f>
+        <v>0.86996316081868086</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
@@ -2671,22 +2671,22 @@
         <v>98551</v>
       </c>
       <c r="D19" s="56">
-        <f t="shared" si="3"/>
-        <v>0.43020905634350021</v>
+        <f t="shared" si="7"/>
+        <v>0.43522096458648907</v>
       </c>
       <c r="E19" s="27">
         <v>466614</v>
       </c>
       <c r="F19" s="56">
-        <f t="shared" si="4"/>
-        <v>0.48434841729941819</v>
+        <f t="shared" si="8"/>
+        <v>0.48971482785980258</v>
       </c>
       <c r="G19" s="27">
         <v>5231985</v>
       </c>
       <c r="H19" s="56">
-        <f t="shared" si="5"/>
-        <v>0.43467155285860504</v>
+        <f t="shared" si="9"/>
+        <v>0.43833900542169596</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
@@ -2697,22 +2697,22 @@
         <v>105387</v>
       </c>
       <c r="D20" s="57">
-        <f t="shared" si="3"/>
-        <v>0.46005055068819656</v>
+        <f t="shared" si="7"/>
+        <v>0.46541011044917174</v>
       </c>
       <c r="E20" s="33">
         <v>379279</v>
       </c>
       <c r="F20" s="57">
-        <f t="shared" si="4"/>
-        <v>0.39369410983147962</v>
+        <f t="shared" si="8"/>
+        <v>0.39805610246550271</v>
       </c>
       <c r="G20" s="33">
         <v>5151837</v>
       </c>
       <c r="H20" s="57">
-        <f t="shared" si="5"/>
-        <v>0.42801288399420434</v>
+        <f t="shared" si="9"/>
+        <v>0.4316241553969849</v>
       </c>
     </row>
     <row r="21" spans="2:8" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -2763,7 +2763,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2778,43 +2778,43 @@
   <sheetData>
     <row r="1" spans="2:12" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:12" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="71"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="74"/>
     </row>
     <row r="3" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
     </row>
     <row r="4" spans="2:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="68"/>
-      <c r="C4" s="72" t="s">
+      <c r="B4" s="71"/>
+      <c r="C4" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="73"/>
-      <c r="E4" s="72" t="s">
+      <c r="D4" s="76"/>
+      <c r="E4" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="73"/>
-      <c r="G4" s="72" t="s">
+      <c r="F4" s="76"/>
+      <c r="G4" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="73"/>
+      <c r="H4" s="76"/>
     </row>
     <row r="5" spans="2:12" ht="43" x14ac:dyDescent="0.2">
       <c r="B5" s="39" t="s">
@@ -2890,22 +2890,22 @@
         <v>68022</v>
       </c>
       <c r="D8" s="56">
-        <f>C8/$C$6</f>
-        <v>0.50438599743439538</v>
+        <f>C8/SUM($C$8:$C$9)</f>
+        <v>0.59072514112027785</v>
       </c>
       <c r="E8" s="27">
         <v>118071</v>
       </c>
       <c r="F8" s="56">
-        <f>E8/$E$6</f>
-        <v>0.5200105701261809</v>
+        <f>E8/SUM($E$8:$E$9)</f>
+        <v>0.60074488274711124</v>
       </c>
       <c r="G8" s="27">
         <v>3006846</v>
       </c>
       <c r="H8" s="56">
-        <f>G8/$G$6</f>
-        <v>0.4709236355161952</v>
+        <f>G8/SUM($G$8:$G$9)</f>
+        <v>0.55072436692759186</v>
       </c>
       <c r="J8" s="42"/>
       <c r="K8" s="42"/>
@@ -2919,22 +2919,22 @@
         <v>47128</v>
       </c>
       <c r="D9" s="56">
-        <f t="shared" ref="D9:D11" si="0">C9/$C$6</f>
-        <v>0.34945610665796634</v>
+        <f t="shared" ref="D9:D11" si="0">C9/SUM($C$8:$C$9)</f>
+        <v>0.40927485887972209</v>
       </c>
       <c r="E9" s="27">
         <v>78470</v>
       </c>
       <c r="F9" s="56">
-        <f t="shared" ref="F9:F11" si="1">E9/$E$6</f>
-        <v>0.34559908392239763</v>
+        <f t="shared" ref="F9:F11" si="1">E9/SUM($E$8:$E$9)</f>
+        <v>0.3992551172528887</v>
       </c>
       <c r="G9" s="27">
         <v>2452956</v>
       </c>
       <c r="H9" s="56">
-        <f t="shared" ref="H9:H11" si="2">G9/$G$6</f>
-        <v>0.38417496515660071</v>
+        <f t="shared" ref="H9:H11" si="2">G9/SUM($G$8:$G$9)</f>
+        <v>0.44927563307240814</v>
       </c>
       <c r="J9" s="42"/>
       <c r="K9" s="42"/>
@@ -2949,21 +2949,21 @@
       </c>
       <c r="D10" s="56">
         <f t="shared" si="0"/>
-        <v>0.29625317919932376</v>
+        <v>0.34696482848458532</v>
       </c>
       <c r="E10" s="27">
         <v>66322</v>
       </c>
       <c r="F10" s="56">
         <f t="shared" si="1"/>
-        <v>0.29209662857017021</v>
+        <v>0.33744613083275243</v>
       </c>
       <c r="G10" s="27">
         <v>2058825</v>
       </c>
       <c r="H10" s="56">
         <f t="shared" si="2"/>
-        <v>0.32244729324070159</v>
+        <v>0.37708785043853238</v>
       </c>
       <c r="J10" s="41"/>
       <c r="K10" s="41"/>
@@ -2978,21 +2978,21 @@
       </c>
       <c r="D11" s="56">
         <f t="shared" si="0"/>
-        <v>5.32029274586426E-2</v>
+        <v>6.231003039513678E-2</v>
       </c>
       <c r="E11" s="27">
         <v>12148</v>
       </c>
       <c r="F11" s="56">
         <f t="shared" si="1"/>
-        <v>5.3502455352227432E-2</v>
+        <v>6.1808986420136255E-2</v>
       </c>
       <c r="G11" s="27">
         <v>394131</v>
       </c>
       <c r="H11" s="56">
         <f t="shared" si="2"/>
-        <v>6.1727671915899097E-2</v>
+        <v>7.2187782633875736E-2</v>
       </c>
       <c r="J11" s="41"/>
       <c r="K11" s="41"/>
@@ -3123,22 +3123,22 @@
         <v>34045</v>
       </c>
       <c r="D17" s="56">
-        <f t="shared" si="3"/>
-        <v>0.12460791239198146</v>
+        <f>C17/SUM($C$17:$C$18)</f>
+        <v>0.12582974822962403</v>
       </c>
       <c r="E17" s="27">
         <v>59266</v>
       </c>
       <c r="F17" s="56">
-        <f t="shared" si="4"/>
-        <v>0.1359789100303547</v>
+        <f>E17/SUM($E$17:$E$18)</f>
+        <v>0.13709239036147922</v>
       </c>
       <c r="G17" s="27">
         <v>1552111</v>
       </c>
       <c r="H17" s="56">
-        <f t="shared" si="5"/>
-        <v>0.12894885948238047</v>
+        <f>G17/SUM($G$17:$G$18)</f>
+        <v>0.13003683918131914</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -3149,22 +3149,22 @@
         <v>236519</v>
       </c>
       <c r="D18" s="56">
-        <f t="shared" si="3"/>
-        <v>0.86568185727828062</v>
+        <f t="shared" ref="D18:D20" si="6">C18/SUM($C$17:$C$18)</f>
+        <v>0.87417025177037599</v>
       </c>
       <c r="E18" s="27">
         <v>373041</v>
       </c>
       <c r="F18" s="56">
-        <f t="shared" si="4"/>
-        <v>0.85589897372243007</v>
+        <f t="shared" ref="F18:F20" si="7">E18/SUM($E$17:$E$18)</f>
+        <v>0.86290760963852076</v>
       </c>
       <c r="G18" s="27">
         <v>10383822</v>
       </c>
       <c r="H18" s="56">
-        <f t="shared" si="5"/>
-        <v>0.86268443685280938</v>
+        <f t="shared" ref="H18:H20" si="8">G18/SUM($G$17:$G$18)</f>
+        <v>0.86996316081868086</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -3175,22 +3175,22 @@
         <v>127154</v>
       </c>
       <c r="D19" s="56">
-        <f t="shared" si="3"/>
-        <v>0.46539563789954502</v>
+        <f t="shared" si="6"/>
+        <v>0.46995904850608361</v>
       </c>
       <c r="E19" s="27">
         <v>192966</v>
       </c>
       <c r="F19" s="56">
-        <f t="shared" si="4"/>
-        <v>0.44273793326557254</v>
+        <f t="shared" si="7"/>
+        <v>0.44636334826870722</v>
       </c>
       <c r="G19" s="27">
         <v>5231985</v>
       </c>
       <c r="H19" s="56">
-        <f t="shared" si="5"/>
-        <v>0.43467155285860504</v>
+        <f t="shared" si="8"/>
+        <v>0.43833900542169596</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
@@ -3201,22 +3201,22 @@
         <v>109365</v>
       </c>
       <c r="D20" s="57">
-        <f t="shared" si="3"/>
-        <v>0.4002862193787356</v>
+        <f t="shared" si="6"/>
+        <v>0.40421120326429238</v>
       </c>
       <c r="E20" s="33">
         <v>180075</v>
       </c>
       <c r="F20" s="57">
-        <f t="shared" si="4"/>
-        <v>0.41316104045685759</v>
+        <f t="shared" si="7"/>
+        <v>0.4165442613698136</v>
       </c>
       <c r="G20" s="33">
         <v>5151837</v>
       </c>
       <c r="H20" s="57">
-        <f t="shared" si="5"/>
-        <v>0.42801288399420434</v>
+        <f t="shared" si="8"/>
+        <v>0.4316241553969849</v>
       </c>
     </row>
     <row r="21" spans="2:8" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -3261,8 +3261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55AFC039-7414-7645-9812-2C75554B8DE7}">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="B2" zoomScale="91" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3292,83 +3292,83 @@
   <sheetData>
     <row r="1" spans="2:22" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:22" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="71"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="73"/>
+      <c r="R2" s="74"/>
     </row>
     <row r="3" spans="2:22" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="66"/>
-      <c r="N3" s="66"/>
-      <c r="O3" s="66"/>
-      <c r="P3" s="66"/>
-      <c r="Q3" s="66"/>
-      <c r="R3" s="66"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="69"/>
+      <c r="Q3" s="69"/>
+      <c r="R3" s="69"/>
     </row>
     <row r="4" spans="2:22" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="68"/>
-      <c r="C4" s="75" t="s">
+      <c r="B4" s="71"/>
+      <c r="C4" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="76"/>
-      <c r="E4" s="75" t="s">
+      <c r="D4" s="79"/>
+      <c r="E4" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="77"/>
-      <c r="G4" s="75" t="s">
+      <c r="F4" s="80"/>
+      <c r="G4" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="77"/>
-      <c r="I4" s="75" t="s">
+      <c r="H4" s="80"/>
+      <c r="I4" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="J4" s="77"/>
-      <c r="K4" s="75" t="s">
+      <c r="J4" s="80"/>
+      <c r="K4" s="78" t="s">
         <v>46</v>
       </c>
-      <c r="L4" s="77"/>
-      <c r="M4" s="72" t="s">
+      <c r="L4" s="80"/>
+      <c r="M4" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="N4" s="73"/>
-      <c r="O4" s="72" t="s">
+      <c r="N4" s="76"/>
+      <c r="O4" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="P4" s="73"/>
-      <c r="Q4" s="74" t="s">
+      <c r="P4" s="76"/>
+      <c r="Q4" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="73"/>
+      <c r="R4" s="76"/>
     </row>
     <row r="5" spans="2:22" ht="43" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="43" t="s">
@@ -3444,7 +3444,7 @@
       <c r="G6" s="27">
         <v>67929</v>
       </c>
-      <c r="H6" s="96">
+      <c r="H6" s="68">
         <f>G6/C26</f>
         <v>0.34190499199710084</v>
       </c>
@@ -3479,7 +3479,7 @@
       <c r="Q6" s="28">
         <v>6384997</v>
       </c>
-      <c r="R6" s="96">
+      <c r="R6" s="68">
         <f>Q6/C31</f>
         <v>0.34660312761564022</v>
       </c>
@@ -3520,57 +3520,57 @@
         <v>5820</v>
       </c>
       <c r="D8" s="53">
-        <f>C8/$C$6</f>
-        <v>0.32770270270270269</v>
+        <f>C8/SUM($C$8:$C$9)</f>
+        <v>0.40919637207340226</v>
       </c>
       <c r="E8" s="27">
         <v>26353</v>
       </c>
-      <c r="F8" s="56">
-        <f>E8/$E$6</f>
-        <v>0.25928549642354654</v>
+      <c r="F8" s="53">
+        <f>E8/SUM($E$8:$E$9)</f>
+        <v>0.32014821114013242</v>
       </c>
       <c r="G8" s="27">
         <v>33061</v>
       </c>
-      <c r="H8" s="56">
-        <f>G8/$G$6</f>
-        <v>0.48669934784848884</v>
+      <c r="H8" s="53">
+        <f>G8/SUM($G$8:$G$9)</f>
+        <v>0.53680040266930784</v>
       </c>
       <c r="I8" s="27">
         <v>5356</v>
       </c>
-      <c r="J8" s="56">
-        <f>I8/$I$6</f>
-        <v>0.35371813498877297</v>
+      <c r="J8" s="53">
+        <f>I8/SUM($I$8:$I$9)</f>
+        <v>0.4224641110585266</v>
       </c>
       <c r="K8" s="27">
         <v>46567</v>
       </c>
-      <c r="L8" s="56">
-        <f>K8/$K$6</f>
-        <v>0.28727683253340569</v>
+      <c r="L8" s="53">
+        <f>K8/SUM($K$8:$K$9)</f>
+        <v>0.36571612568816708</v>
       </c>
       <c r="M8" s="27">
         <v>117157</v>
       </c>
-      <c r="N8" s="56">
-        <f>M8/$M$6</f>
-        <v>0.3213601926674457</v>
+      <c r="N8" s="53">
+        <f>M8/SUM($M$8:$M$9)</f>
+        <v>0.39296495559073713</v>
       </c>
       <c r="O8" s="27">
         <v>182826</v>
       </c>
       <c r="P8" s="56">
-        <f>O8/$O$6</f>
-        <v>0.34967132127508604</v>
+        <f>O8/SUM($O$8:$O$9)</f>
+        <v>0.42382051852676089</v>
       </c>
       <c r="Q8" s="28">
         <v>3006846</v>
       </c>
       <c r="R8" s="56">
-        <f>Q8/$Q$6</f>
-        <v>0.4709236355161952</v>
+        <f>Q8/SUM($Q$8:$Q$9)</f>
+        <v>0.55072436692759186</v>
       </c>
       <c r="S8" s="50"/>
       <c r="T8" s="42"/>
@@ -3585,57 +3585,57 @@
         <v>8403</v>
       </c>
       <c r="D9" s="53">
-        <f t="shared" ref="D9:D11" si="0">C9/$C$6</f>
-        <v>0.47314189189189187</v>
+        <f>C9/SUM($C$8:$C$9)</f>
+        <v>0.5908036279265978</v>
       </c>
       <c r="E9" s="27">
         <v>55962</v>
       </c>
-      <c r="F9" s="56">
-        <f t="shared" ref="F9:F10" si="1">E9/$E$6</f>
-        <v>0.55060657044186667</v>
+      <c r="F9" s="53">
+        <f t="shared" ref="F9:F11" si="0">E9/SUM($E$8:$E$9)</f>
+        <v>0.67985178885986763</v>
       </c>
       <c r="G9" s="27">
         <v>28528</v>
       </c>
       <c r="H9" s="56">
-        <f t="shared" ref="H9:H11" si="2">G9/$G$6</f>
-        <v>0.41996790766830072</v>
+        <f t="shared" ref="H9:H11" si="1">G9/SUM($G$8:$G$9)</f>
+        <v>0.46319959733069216</v>
       </c>
       <c r="I9" s="27">
         <v>7322</v>
       </c>
-      <c r="J9" s="56">
-        <f t="shared" ref="J9:J11" si="3">I9/$I$6</f>
-        <v>0.48355567296262053</v>
+      <c r="J9" s="53">
+        <f t="shared" ref="J9:J11" si="2">I9/SUM($I$8:$I$9)</f>
+        <v>0.57753588894147345</v>
       </c>
       <c r="K9" s="27">
         <v>80764</v>
       </c>
-      <c r="L9" s="56">
-        <f t="shared" ref="L9:L11" si="4">K9/$K$6</f>
-        <v>0.49824180434058407</v>
+      <c r="L9" s="53">
+        <f t="shared" ref="L9:L11" si="3">K9/SUM($K$8:$K$9)</f>
+        <v>0.63428387431183297</v>
       </c>
       <c r="M9" s="27">
         <v>180979</v>
       </c>
-      <c r="N9" s="56">
-        <f t="shared" ref="N9:N11" si="5">M9/$M$6</f>
-        <v>0.49642314423177147</v>
+      <c r="N9" s="53">
+        <f t="shared" ref="N9:N11" si="4">M9/SUM($M$8:$M$9)</f>
+        <v>0.60703504440926292</v>
       </c>
       <c r="O9" s="27">
         <v>248550</v>
       </c>
       <c r="P9" s="56">
-        <f t="shared" ref="P9:P11" si="6">O9/$O$6</f>
-        <v>0.47537443745923791</v>
+        <f t="shared" ref="P9:P11" si="5">O9/SUM($O$8:$O$9)</f>
+        <v>0.57617948147323916</v>
       </c>
       <c r="Q9" s="28">
         <v>2452956</v>
       </c>
       <c r="R9" s="56">
-        <f t="shared" ref="R9:R11" si="7">Q9/$Q$6</f>
-        <v>0.38417496515660071</v>
+        <f t="shared" ref="R9:R11" si="6">Q9/SUM($Q$8:$Q$9)</f>
+        <v>0.44927563307240814</v>
       </c>
       <c r="S9" s="50"/>
       <c r="T9" s="42"/>
@@ -3650,57 +3650,57 @@
         <v>6484</v>
       </c>
       <c r="D10" s="53">
-        <f t="shared" si="0"/>
-        <v>0.36509009009009008</v>
+        <f t="shared" ref="D9:D11" si="7">C10/SUM($C$8:$C$9)</f>
+        <v>0.45588131899036771</v>
       </c>
       <c r="E10" s="27">
         <v>43837</v>
       </c>
-      <c r="F10" s="56">
-        <f t="shared" si="1"/>
-        <v>0.43130946407312298</v>
+      <c r="F10" s="53">
+        <f t="shared" si="0"/>
+        <v>0.53255178278564053</v>
       </c>
       <c r="G10" s="27">
         <v>24866</v>
       </c>
       <c r="H10" s="56">
-        <f t="shared" si="2"/>
-        <v>0.36605867891474925</v>
+        <f t="shared" si="1"/>
+        <v>0.40374092776307458</v>
       </c>
       <c r="I10" s="27">
         <v>5810</v>
       </c>
-      <c r="J10" s="56">
-        <f t="shared" si="3"/>
-        <v>0.38370096420552108</v>
+      <c r="J10" s="53">
+        <f t="shared" si="2"/>
+        <v>0.45827417573749801</v>
       </c>
       <c r="K10" s="27">
         <v>63324</v>
       </c>
-      <c r="L10" s="56">
-        <f t="shared" si="4"/>
-        <v>0.39065256819948424</v>
+      <c r="L10" s="53">
+        <f t="shared" si="3"/>
+        <v>0.49731801368087897</v>
       </c>
       <c r="M10" s="27">
         <v>144321</v>
       </c>
-      <c r="N10" s="56">
-        <f t="shared" si="5"/>
-        <v>0.39587070653873374</v>
+      <c r="N10" s="53">
+        <f t="shared" si="4"/>
+        <v>0.48407773633509538</v>
       </c>
       <c r="O10" s="27">
         <v>202821</v>
       </c>
       <c r="P10" s="56">
-        <f t="shared" si="6"/>
-        <v>0.38791357384799874</v>
+        <f t="shared" si="5"/>
+        <v>0.4701721931679092</v>
       </c>
       <c r="Q10" s="28">
         <v>2058825</v>
       </c>
       <c r="R10" s="56">
-        <f t="shared" si="7"/>
-        <v>0.32244729324070159</v>
+        <f t="shared" si="6"/>
+        <v>0.37708785043853238</v>
       </c>
       <c r="S10" s="50"/>
       <c r="T10" s="42"/>
@@ -3715,57 +3715,57 @@
         <v>1919</v>
       </c>
       <c r="D11" s="53">
-        <f t="shared" si="0"/>
-        <v>0.10805180180180181</v>
+        <f t="shared" si="7"/>
+        <v>0.13492230893623006</v>
       </c>
       <c r="E11" s="27">
         <v>12125</v>
       </c>
-      <c r="F11" s="56">
-        <f>E11/$E$6</f>
-        <v>0.11929710636874366</v>
+      <c r="F11" s="53">
+        <f t="shared" si="0"/>
+        <v>0.14730000607422705</v>
       </c>
       <c r="G11" s="27">
         <v>3662</v>
       </c>
       <c r="H11" s="57">
-        <f t="shared" si="2"/>
-        <v>5.3909228753551502E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.9458669567617597E-2</v>
       </c>
       <c r="I11" s="27">
         <v>1512</v>
       </c>
-      <c r="J11" s="56">
-        <f t="shared" si="3"/>
-        <v>9.9854708757099453E-2</v>
+      <c r="J11" s="53">
+        <f t="shared" si="2"/>
+        <v>0.11926171320397538</v>
       </c>
       <c r="K11" s="27">
         <v>17440</v>
       </c>
-      <c r="L11" s="56">
-        <f t="shared" si="4"/>
-        <v>0.10758923614109983</v>
+      <c r="L11" s="53">
+        <f t="shared" si="3"/>
+        <v>0.13696586063095398</v>
       </c>
       <c r="M11" s="27">
         <v>36658</v>
       </c>
-      <c r="N11" s="56">
-        <f t="shared" si="5"/>
-        <v>0.10055243769303775</v>
+      <c r="N11" s="53">
+        <f t="shared" si="4"/>
+        <v>0.12295730807416749</v>
       </c>
       <c r="O11" s="27">
         <v>45729</v>
       </c>
       <c r="P11" s="56">
-        <f t="shared" si="6"/>
-        <v>8.7460863611239142E-2</v>
+        <f t="shared" si="5"/>
+        <v>0.10600728830532992</v>
       </c>
       <c r="Q11" s="28">
         <v>394131</v>
       </c>
       <c r="R11" s="57">
-        <f t="shared" si="7"/>
-        <v>6.1727671915899097E-2</v>
+        <f t="shared" si="6"/>
+        <v>7.2187782633875736E-2</v>
       </c>
       <c r="T11" s="41"/>
       <c r="U11" s="41"/>
@@ -4047,57 +4047,57 @@
         <v>5487</v>
       </c>
       <c r="D17" s="53">
-        <f t="shared" si="8"/>
-        <v>0.14592308919738312</v>
+        <f>C17/SUM($C$17:$C$18)</f>
+        <v>0.14717558070918943</v>
       </c>
       <c r="E17" s="27">
         <v>18488</v>
       </c>
-      <c r="F17" s="56">
-        <f t="shared" si="9"/>
-        <v>9.0139636477104296E-2</v>
+      <c r="F17" s="53">
+        <f>E17/SUM($E$17:$E$18)</f>
+        <v>9.0728853817011165E-2</v>
       </c>
       <c r="G17" s="27">
         <v>23389</v>
       </c>
-      <c r="H17" s="56">
-        <f t="shared" si="10"/>
-        <v>0.17888473334404087</v>
+      <c r="H17" s="53">
+        <f>G17/SUM($G$17:$G$18)</f>
+        <v>0.17980197106440554</v>
       </c>
       <c r="I17" s="27">
         <v>3146</v>
       </c>
-      <c r="J17" s="56">
-        <f t="shared" si="11"/>
-        <v>9.6910328681883998E-2</v>
+      <c r="J17" s="53">
+        <f>I17/SUM($I$17:$I$18)</f>
+        <v>9.7254853468529745E-2</v>
       </c>
       <c r="K17" s="27">
         <v>53067</v>
       </c>
-      <c r="L17" s="56">
-        <f t="shared" si="12"/>
-        <v>0.12434362676526617</v>
+      <c r="L17" s="53">
+        <f>K17/SUM($K$17:$K$18)</f>
+        <v>0.12502503233588799</v>
       </c>
       <c r="M17" s="27">
         <v>103577</v>
       </c>
-      <c r="N17" s="56">
-        <f t="shared" ref="N17:N20" si="16">M17/$M$15</f>
-        <v>0.12438768096361813</v>
+      <c r="N17" s="53">
+        <f>M17/SUM($M$17:$M$18)</f>
+        <v>0.12510281604232215</v>
       </c>
       <c r="O17" s="27">
         <v>153570</v>
       </c>
       <c r="P17" s="56">
-        <f t="shared" si="13"/>
-        <v>0.13338081320866971</v>
+        <f>O17/SUM($O$17:$O$18)</f>
+        <v>0.13425253674089008</v>
       </c>
       <c r="Q17" s="28">
         <v>1552111</v>
       </c>
       <c r="R17" s="56">
-        <f t="shared" si="14"/>
-        <v>0.12894885948238047</v>
+        <f>Q17/SUM($Q$17:$Q$18)</f>
+        <v>0.13003683918131914</v>
       </c>
     </row>
     <row r="18" spans="2:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -4108,57 +4108,57 @@
         <v>31795</v>
       </c>
       <c r="D18" s="53">
-        <f>C18/$C$15</f>
-        <v>0.84556672517419285</v>
+        <f t="shared" ref="D18:D20" si="16">C18/SUM($C$17:$C$18)</f>
+        <v>0.85282441929081054</v>
       </c>
       <c r="E18" s="27">
         <v>185284</v>
       </c>
       <c r="F18" s="56">
-        <f t="shared" si="9"/>
-        <v>0.90336609719946959</v>
+        <f t="shared" ref="F18:F20" si="17">E18/SUM($E$17:$E$18)</f>
+        <v>0.90927114618298888</v>
       </c>
       <c r="G18" s="27">
         <v>106693</v>
       </c>
       <c r="H18" s="56">
-        <f t="shared" si="10"/>
-        <v>0.81601388920756568</v>
+        <f t="shared" ref="H18:H20" si="18">G18/SUM($G$17:$G$18)</f>
+        <v>0.82019802893559446</v>
       </c>
       <c r="I18" s="27">
         <v>29202</v>
       </c>
       <c r="J18" s="56">
-        <f t="shared" si="11"/>
-        <v>0.89954717678587925</v>
+        <f t="shared" ref="J18:J20" si="19">I18/SUM($I$17:$I$18)</f>
+        <v>0.90274514653147031</v>
       </c>
       <c r="K18" s="27">
         <v>371384</v>
       </c>
       <c r="L18" s="56">
-        <f t="shared" si="12"/>
-        <v>0.87020622011026838</v>
+        <f t="shared" ref="L18:L20" si="20">K18/SUM($K$17:$K$18)</f>
+        <v>0.87497496766411198</v>
       </c>
       <c r="M18" s="27">
         <v>724358</v>
       </c>
       <c r="N18" s="56">
-        <f t="shared" si="16"/>
-        <v>0.86989594029026229</v>
+        <f t="shared" ref="N18:N20" si="21">M18/SUM($M$17:$M$18)</f>
+        <v>0.87489718395767779</v>
       </c>
       <c r="O18" s="27">
         <v>990319</v>
       </c>
       <c r="P18" s="56">
-        <f t="shared" si="13"/>
-        <v>0.86012602432764584</v>
+        <f t="shared" ref="P18:P20" si="22">O18/SUM($O$17:$O$18)</f>
+        <v>0.8657474632591099</v>
       </c>
       <c r="Q18" s="28">
         <v>10383822</v>
       </c>
       <c r="R18" s="56">
-        <f t="shared" si="14"/>
-        <v>0.86268443685280938</v>
+        <f t="shared" ref="R18:R20" si="23">Q18/SUM($Q$17:$Q$18)</f>
+        <v>0.86996316081868086</v>
       </c>
     </row>
     <row r="19" spans="2:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -4169,57 +4169,57 @@
         <v>11348</v>
       </c>
       <c r="D19" s="53">
-        <f t="shared" si="8"/>
-        <v>0.30179245784798681</v>
+        <f t="shared" si="16"/>
+        <v>0.30438281208089696</v>
       </c>
       <c r="E19" s="27">
         <v>44982</v>
       </c>
       <c r="F19" s="56">
-        <f t="shared" si="9"/>
-        <v>0.21931312894921601</v>
+        <f t="shared" si="17"/>
+        <v>0.22074671691890937</v>
       </c>
       <c r="G19" s="27">
         <v>46788</v>
       </c>
       <c r="H19" s="56">
-        <f t="shared" si="10"/>
-        <v>0.35784594910859741</v>
+        <f t="shared" si="18"/>
+        <v>0.35968081671561014</v>
       </c>
       <c r="I19" s="27">
         <v>11586</v>
       </c>
       <c r="J19" s="56">
-        <f t="shared" si="11"/>
-        <v>0.35689862304777747</v>
+        <f t="shared" si="19"/>
+        <v>0.35816742920736983</v>
       </c>
       <c r="K19" s="27">
         <v>118565</v>
       </c>
       <c r="L19" s="56">
-        <f t="shared" si="12"/>
-        <v>0.27781487755900625</v>
+        <f t="shared" si="20"/>
+        <v>0.27933730866460438</v>
       </c>
       <c r="M19" s="27">
         <v>233269</v>
       </c>
       <c r="N19" s="56">
-        <f t="shared" si="16"/>
-        <v>0.28013738523709159</v>
+        <f t="shared" si="21"/>
+        <v>0.2817479633062982</v>
       </c>
       <c r="O19" s="27">
         <v>373144</v>
       </c>
       <c r="P19" s="56">
-        <f t="shared" si="13"/>
-        <v>0.32408836468018398</v>
+        <f t="shared" si="22"/>
+        <v>0.32620647632768562</v>
       </c>
       <c r="Q19" s="28">
         <v>5231985</v>
       </c>
       <c r="R19" s="56">
-        <f t="shared" si="14"/>
-        <v>0.43467155285860504</v>
+        <f t="shared" si="23"/>
+        <v>0.43833900542169596</v>
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.2">
@@ -4230,57 +4230,57 @@
         <v>20447</v>
       </c>
       <c r="D20" s="61">
-        <f t="shared" si="8"/>
-        <v>0.54377426732620604</v>
+        <f t="shared" si="16"/>
+        <v>0.54844160720991364</v>
       </c>
       <c r="E20" s="33">
         <v>140302</v>
       </c>
       <c r="F20" s="57">
-        <f t="shared" si="9"/>
-        <v>0.68405296825025352</v>
+        <f t="shared" si="17"/>
+        <v>0.68852442926407942</v>
       </c>
       <c r="G20" s="33">
         <v>59905</v>
       </c>
       <c r="H20" s="57">
-        <f t="shared" si="10"/>
-        <v>0.45816794009896827</v>
+        <f t="shared" si="18"/>
+        <v>0.46051721221998432</v>
       </c>
       <c r="I20" s="33">
         <v>17616</v>
       </c>
       <c r="J20" s="57">
-        <f t="shared" si="11"/>
-        <v>0.54264855373810184</v>
+        <f t="shared" si="19"/>
+        <v>0.54457771732410043</v>
       </c>
       <c r="K20" s="33">
         <v>252819</v>
       </c>
       <c r="L20" s="57">
-        <f t="shared" si="12"/>
-        <v>0.59239134255126213</v>
+        <f t="shared" si="20"/>
+        <v>0.5956376589995076</v>
       </c>
       <c r="M20" s="33">
         <v>491089</v>
       </c>
       <c r="N20" s="57">
-        <f t="shared" si="16"/>
-        <v>0.58975855505317076</v>
+        <f t="shared" si="21"/>
+        <v>0.59314922065137965</v>
       </c>
       <c r="O20" s="33">
         <v>617175</v>
       </c>
       <c r="P20" s="57">
-        <f t="shared" si="13"/>
-        <v>0.53603765964746197</v>
+        <f t="shared" si="22"/>
+        <v>0.53954098693142427</v>
       </c>
       <c r="Q20" s="34">
         <v>5151837</v>
       </c>
       <c r="R20" s="57">
-        <f t="shared" si="14"/>
-        <v>0.42801288399420434</v>
+        <f t="shared" si="23"/>
+        <v>0.4316241553969849</v>
       </c>
     </row>
     <row r="21" spans="2:18" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -4371,8 +4371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B48D4E-D75D-404D-AC01-9AD0F7A038FD}">
   <dimension ref="A1:T32"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4387,75 +4387,75 @@
   <sheetData>
     <row r="1" spans="2:20" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:20" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="71"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="74"/>
     </row>
     <row r="3" spans="2:20" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="79" t="s">
+      <c r="C3" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="79"/>
-      <c r="M3" s="79"/>
-      <c r="N3" s="79"/>
-      <c r="O3" s="79"/>
-      <c r="P3" s="66"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
+      <c r="N3" s="82"/>
+      <c r="O3" s="82"/>
+      <c r="P3" s="69"/>
     </row>
     <row r="4" spans="2:20" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="78"/>
-      <c r="C4" s="72" t="s">
+      <c r="B4" s="81"/>
+      <c r="C4" s="75" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="73"/>
-      <c r="E4" s="72" t="s">
+      <c r="D4" s="76"/>
+      <c r="E4" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="73"/>
-      <c r="G4" s="72" t="s">
+      <c r="F4" s="76"/>
+      <c r="G4" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="74"/>
-      <c r="I4" s="72" t="s">
+      <c r="H4" s="77"/>
+      <c r="I4" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="J4" s="73"/>
-      <c r="K4" s="72" t="s">
+      <c r="J4" s="76"/>
+      <c r="K4" s="75" t="s">
         <v>54</v>
       </c>
-      <c r="L4" s="73"/>
-      <c r="M4" s="72" t="s">
+      <c r="L4" s="76"/>
+      <c r="M4" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="N4" s="73"/>
-      <c r="O4" s="74" t="s">
+      <c r="N4" s="76"/>
+      <c r="O4" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="73"/>
+      <c r="P4" s="76"/>
     </row>
     <row r="5" spans="2:20" ht="43" x14ac:dyDescent="0.25">
       <c r="B5" s="39" t="s">
@@ -4597,50 +4597,50 @@
         <v>13270</v>
       </c>
       <c r="D8" s="56">
-        <f>C8/$C$6</f>
-        <v>0.63091332667712641</v>
+        <f>C8/SUM($C$8:$C$9)</f>
+        <v>0.67780161405659411</v>
       </c>
       <c r="E8" s="27">
         <v>55956</v>
       </c>
       <c r="F8" s="56">
-        <f>E8/$E$6</f>
-        <v>0.7027705910426767</v>
+        <f>E8/SUM($E$8:$E$9)</f>
+        <v>0.78089762197164225</v>
       </c>
       <c r="G8" s="64">
         <v>266</v>
       </c>
       <c r="H8" s="56">
-        <f>G8/$G$6</f>
+        <f>G8/SUM($G$8:$G$9)</f>
         <v>0.98884758364312264</v>
       </c>
       <c r="I8" s="27">
         <v>4520</v>
       </c>
       <c r="J8" s="56">
-        <f>I8/$I$6</f>
-        <v>0.76506431956668919</v>
+        <f>I8/SUM($I$8:$I$9)</f>
+        <v>0.83936861652739092</v>
       </c>
       <c r="K8" s="27">
         <v>12862</v>
       </c>
       <c r="L8" s="56">
-        <f>K8/$K$6</f>
-        <v>0.79346082665021589</v>
+        <f>K8/SUM($K$8:$K$9)</f>
+        <v>0.85695249516956495</v>
       </c>
       <c r="M8" s="27">
         <v>86874</v>
       </c>
       <c r="N8" s="56">
-        <f>M8/$M$6</f>
-        <v>0.70605159213926949</v>
+        <f>M8/SUM($M$8:$M$9)</f>
+        <v>0.77637470173463097</v>
       </c>
       <c r="O8" s="27">
         <v>313546</v>
       </c>
       <c r="P8" s="56">
-        <f>O8/$O$6</f>
-        <v>0.67313583756083628</v>
+        <f>O8/SUM($O$8:$O$9)</f>
+        <v>0.73742041849230822</v>
       </c>
       <c r="Q8" s="50"/>
       <c r="R8" s="42"/>
@@ -4655,50 +4655,50 @@
         <v>6308</v>
       </c>
       <c r="D9" s="56">
-        <f t="shared" ref="D9:D11" si="0">C9/$C$6</f>
-        <v>0.29990966576332428</v>
+        <f t="shared" ref="D9:D11" si="0">C9/SUM($C$8:$C$9)</f>
+        <v>0.32219838594340589</v>
       </c>
       <c r="E9" s="27">
         <v>15700</v>
       </c>
       <c r="F9" s="56">
-        <f t="shared" ref="F9:F11" si="1">E9/$E$6</f>
-        <v>0.19718168345432166</v>
+        <f t="shared" ref="F9:F11" si="1">E9/SUM($E$8:$E$9)</f>
+        <v>0.21910237802835772</v>
       </c>
       <c r="G9" s="64">
         <v>3</v>
       </c>
       <c r="H9" s="56">
-        <f t="shared" ref="H9:H11" si="2">G9/$G$6</f>
+        <f t="shared" ref="H9:H11" si="2">G9/SUM($G$8:$G$9)</f>
         <v>1.1152416356877323E-2</v>
       </c>
       <c r="I9" s="27">
         <v>865</v>
       </c>
       <c r="J9" s="56">
-        <f t="shared" ref="J9:J11" si="3">I9/$I$6</f>
-        <v>0.1464116452268111</v>
+        <f t="shared" ref="J9:J11" si="3">I9/SUM($I$8:$I$9)</f>
+        <v>0.16063138347260911</v>
       </c>
       <c r="K9" s="27">
         <v>2147</v>
       </c>
       <c r="L9" s="56">
-        <f t="shared" ref="L9:L11" si="4">K9/$K$6</f>
-        <v>0.13244910549043801</v>
+        <f t="shared" ref="L9:L11" si="4">K9/SUM($K$8:$K$9)</f>
+        <v>0.14304750483043507</v>
       </c>
       <c r="M9" s="27">
         <v>25023</v>
       </c>
       <c r="N9" s="56">
-        <f t="shared" ref="N9:N11" si="5">M9/$M$6</f>
-        <v>0.20336958111864242</v>
+        <f t="shared" ref="N9:N11" si="5">M9/SUM($M$8:$M$9)</f>
+        <v>0.22362529826536903</v>
       </c>
       <c r="O9" s="27">
         <v>111647</v>
       </c>
       <c r="P9" s="56">
-        <f t="shared" ref="P9:P11" si="6">O9/$O$6</f>
-        <v>0.23968922217523009</v>
+        <f t="shared" ref="P9:P11" si="6">O9/SUM($O$8:$O$9)</f>
+        <v>0.26257958150769178</v>
       </c>
       <c r="Q9" s="50"/>
       <c r="R9" s="42"/>
@@ -4714,14 +4714,14 @@
       </c>
       <c r="D10" s="56">
         <f t="shared" si="0"/>
-        <v>0.2454238577473494</v>
+        <v>0.26366329553580548</v>
       </c>
       <c r="E10" s="27">
         <v>12057</v>
       </c>
       <c r="F10" s="56">
         <f t="shared" si="1"/>
-        <v>0.15142799728718193</v>
+        <v>0.168262252986491</v>
       </c>
       <c r="G10" s="64">
         <v>3</v>
@@ -4735,28 +4735,28 @@
       </c>
       <c r="J10" s="56">
         <f t="shared" si="3"/>
-        <v>0.12897765741367637</v>
+        <v>0.14150417827298051</v>
       </c>
       <c r="K10" s="27">
         <v>1938</v>
       </c>
       <c r="L10" s="56">
         <f t="shared" si="4"/>
-        <v>0.11955582973473165</v>
+        <v>0.12912252648410955</v>
       </c>
       <c r="M10" s="27">
         <v>19922</v>
       </c>
       <c r="N10" s="56">
         <f t="shared" si="5"/>
-        <v>0.1619121925846459</v>
+        <v>0.17803873204822293</v>
       </c>
       <c r="O10" s="27">
         <v>92192</v>
       </c>
       <c r="P10" s="56">
         <f t="shared" si="6"/>
-        <v>0.19792227978162255</v>
+        <v>0.21682388938670205</v>
       </c>
       <c r="T10" s="42"/>
     </row>
@@ -4769,14 +4769,14 @@
       </c>
       <c r="D11" s="56">
         <f t="shared" si="0"/>
-        <v>5.4485808015974899E-2</v>
+        <v>5.8535090407600368E-2</v>
       </c>
       <c r="E11" s="27">
         <v>3643</v>
       </c>
       <c r="F11" s="56">
         <f t="shared" si="1"/>
-        <v>4.5753686167139734E-2</v>
+        <v>5.0840125041866698E-2</v>
       </c>
       <c r="G11" s="64">
         <v>0</v>
@@ -4790,28 +4790,28 @@
       </c>
       <c r="J11" s="56">
         <f t="shared" si="3"/>
-        <v>1.7433987813134731E-2</v>
+        <v>1.91272051996286E-2</v>
       </c>
       <c r="K11" s="27">
         <v>209</v>
       </c>
       <c r="L11" s="56">
         <f t="shared" si="4"/>
-        <v>1.2893275755706354E-2</v>
+        <v>1.3924978346325539E-2</v>
       </c>
       <c r="M11" s="27">
         <v>5101</v>
       </c>
       <c r="N11" s="56">
         <f t="shared" si="5"/>
-        <v>4.1457388533996518E-2</v>
+        <v>4.5586566217146123E-2</v>
       </c>
       <c r="O11" s="27">
         <v>19455</v>
       </c>
       <c r="P11" s="56">
         <f t="shared" si="6"/>
-        <v>4.1766942393607544E-2</v>
+        <v>4.575569212098976E-2</v>
       </c>
       <c r="T11" s="41"/>
     </row>
@@ -5059,50 +5059,50 @@
         <v>175</v>
       </c>
       <c r="D17" s="56">
-        <f t="shared" ref="D17:D20" si="14">C17/$C$15</f>
+        <f>C17/SUM($C$17:$C$18)</f>
         <v>5.5732484076433123E-2</v>
       </c>
       <c r="E17" s="27">
         <v>2159</v>
       </c>
       <c r="F17" s="56">
-        <f t="shared" si="7"/>
-        <v>0.11784934497816595</v>
+        <f>E17/SUM($E$17:$E$18)</f>
+        <v>0.11963870109719606</v>
       </c>
       <c r="G17" s="64">
         <v>0</v>
       </c>
       <c r="H17" s="56">
-        <f t="shared" si="8"/>
+        <f>G17/SUM($G$17:$G$18)</f>
         <v>0</v>
       </c>
       <c r="I17" s="27">
         <v>122</v>
       </c>
       <c r="J17" s="56">
-        <f t="shared" si="9"/>
-        <v>0.18541033434650456</v>
+        <f>I17/SUM($I$17:$I$18)</f>
+        <v>0.19457735247208932</v>
       </c>
       <c r="K17" s="27">
         <v>831</v>
       </c>
       <c r="L17" s="56">
-        <f t="shared" si="10"/>
+        <f>K17/SUM($K$17:$K$18)</f>
         <v>0.32768138801261831</v>
       </c>
       <c r="M17" s="27">
         <v>3287</v>
       </c>
       <c r="N17" s="56">
-        <f t="shared" si="11"/>
-        <v>0.13331440622972096</v>
+        <f>M17/SUM($M$17:$M$18)</f>
+        <v>0.13498418956100366</v>
       </c>
       <c r="O17" s="27">
         <v>27519</v>
       </c>
       <c r="P17" s="56">
-        <f t="shared" si="12"/>
-        <v>0.18899763057587307</v>
+        <f>O17/SUM($O$17:$O$18)</f>
+        <v>0.19148980585902164</v>
       </c>
       <c r="R17" s="49"/>
       <c r="S17" s="49"/>
@@ -5115,50 +5115,50 @@
         <v>2965</v>
       </c>
       <c r="D18" s="56">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="D18:D20" si="14">C18/SUM($C$17:$C$18)</f>
         <v>0.94426751592356684</v>
       </c>
       <c r="E18" s="27">
         <v>15887</v>
       </c>
       <c r="F18" s="56">
-        <f t="shared" si="7"/>
-        <v>0.86719432314410483</v>
+        <f t="shared" ref="F18:F20" si="15">E18/SUM($E$17:$E$18)</f>
+        <v>0.8803612989028039</v>
       </c>
       <c r="G18" s="64">
         <v>2</v>
       </c>
       <c r="H18" s="56">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="H18:H20" si="16">G18/SUM($G$17:$G$18)</f>
         <v>1</v>
       </c>
       <c r="I18" s="27">
         <v>505</v>
       </c>
       <c r="J18" s="56">
-        <f t="shared" si="9"/>
-        <v>0.76747720364741645</v>
+        <f t="shared" ref="J18:J20" si="17">I18/SUM($I$17:$I$18)</f>
+        <v>0.80542264752791071</v>
       </c>
       <c r="K18" s="27">
         <v>1705</v>
       </c>
       <c r="L18" s="56">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="L18:L20" si="18">K18/SUM($K$17:$K$18)</f>
         <v>0.67231861198738174</v>
       </c>
       <c r="M18" s="27">
         <v>21064</v>
       </c>
       <c r="N18" s="56">
-        <f t="shared" si="11"/>
-        <v>0.85431537962362103</v>
+        <f t="shared" ref="N18:N20" si="19">M18/SUM($M$17:$M$18)</f>
+        <v>0.86501581043899634</v>
       </c>
       <c r="O18" s="27">
         <v>116191</v>
       </c>
       <c r="P18" s="56">
-        <f t="shared" si="12"/>
-        <v>0.79798770646612416</v>
+        <f t="shared" ref="P18:P20" si="20">O18/SUM($O$17:$O$18)</f>
+        <v>0.80851019414097836</v>
       </c>
     </row>
     <row r="19" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5176,43 +5176,43 @@
         <v>6333</v>
       </c>
       <c r="F19" s="56">
-        <f t="shared" si="7"/>
-        <v>0.34568777292576419</v>
+        <f t="shared" si="15"/>
+        <v>0.35093649562229856</v>
       </c>
       <c r="G19" s="64">
         <v>0</v>
       </c>
       <c r="H19" s="56">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="I19" s="27">
         <v>165</v>
       </c>
       <c r="J19" s="56">
-        <f t="shared" si="9"/>
-        <v>0.25075987841945291</v>
+        <f t="shared" si="17"/>
+        <v>0.26315789473684209</v>
       </c>
       <c r="K19" s="27">
         <v>922</v>
       </c>
       <c r="L19" s="56">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>0.3635646687697161</v>
       </c>
       <c r="M19" s="27">
         <v>8890</v>
       </c>
       <c r="N19" s="56">
-        <f t="shared" si="11"/>
-        <v>0.3605613238157041</v>
+        <f t="shared" si="19"/>
+        <v>0.3650774095519691</v>
       </c>
       <c r="O19" s="27">
         <v>64122</v>
       </c>
       <c r="P19" s="56">
-        <f t="shared" si="12"/>
-        <v>0.44038322859791901</v>
+        <f t="shared" si="20"/>
+        <v>0.44619024424187598</v>
       </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.2">
@@ -5230,43 +5230,43 @@
         <v>9554</v>
       </c>
       <c r="F20" s="57">
-        <f t="shared" si="7"/>
-        <v>0.52150655021834058</v>
+        <f t="shared" si="15"/>
+        <v>0.52942480328050534</v>
       </c>
       <c r="G20" s="65">
         <v>2</v>
       </c>
       <c r="H20" s="57">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="I20" s="33">
         <v>340</v>
       </c>
       <c r="J20" s="57">
-        <f t="shared" si="9"/>
-        <v>0.51671732522796354</v>
+        <f t="shared" si="17"/>
+        <v>0.54226475279106856</v>
       </c>
       <c r="K20" s="33">
         <v>783</v>
       </c>
       <c r="L20" s="57">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>0.30875394321766564</v>
       </c>
       <c r="M20" s="33">
         <v>12174</v>
       </c>
       <c r="N20" s="57">
-        <f t="shared" si="11"/>
-        <v>0.49375405580791693</v>
+        <f t="shared" si="19"/>
+        <v>0.49993840088702723</v>
       </c>
       <c r="O20" s="33">
         <v>52069</v>
       </c>
       <c r="P20" s="57">
-        <f t="shared" si="12"/>
-        <v>0.3576044778682051</v>
+        <f t="shared" si="20"/>
+        <v>0.36231994989910238</v>
       </c>
     </row>
     <row r="21" spans="2:19" s="49" customFormat="1" x14ac:dyDescent="0.2">
@@ -5274,63 +5274,63 @@
       <c r="S21"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B25" s="95" t="s">
+      <c r="B25" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="95" t="s">
+      <c r="C25" s="67" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B26" s="94" t="s">
+      <c r="B26" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="94">
+      <c r="C26" s="66">
         <v>24173</v>
       </c>
-      <c r="D26" s="94"/>
-      <c r="E26" s="94"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="66"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B27" s="94" t="s">
+      <c r="B27" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="94">
+      <c r="C27" s="66">
         <v>97942</v>
       </c>
-      <c r="D27" s="94"/>
-      <c r="E27" s="94"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="66"/>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B28" s="94" t="s">
+      <c r="B28" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="94">
+      <c r="C28" s="66">
         <v>271</v>
       </c>
-      <c r="D28" s="94"/>
-      <c r="E28" s="94"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B29" s="94" t="s">
+      <c r="B29" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="94">
+      <c r="C29" s="66">
         <v>6566</v>
       </c>
-      <c r="D29" s="94"/>
-      <c r="E29" s="94"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="66"/>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B30" s="94" t="s">
+      <c r="B30" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="94">
+      <c r="C30" s="66">
         <v>18746</v>
       </c>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B31" s="94" t="s">
+      <c r="B31" s="66" t="s">
         <v>63</v>
       </c>
       <c r="C31">
@@ -5339,7 +5339,7 @@
       </c>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B32" s="94" t="s">
+      <c r="B32" s="66" t="s">
         <v>64</v>
       </c>
       <c r="C32">
@@ -5368,7 +5368,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5383,43 +5383,43 @@
   <sheetData>
     <row r="1" spans="2:12" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:12" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="71"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="74"/>
     </row>
     <row r="3" spans="2:12" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="79" t="s">
+      <c r="C3" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="66"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="69"/>
     </row>
     <row r="4" spans="2:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="68"/>
-      <c r="C4" s="72" t="s">
+      <c r="B4" s="71"/>
+      <c r="C4" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="73"/>
-      <c r="E4" s="72" t="s">
+      <c r="D4" s="76"/>
+      <c r="E4" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="73"/>
-      <c r="G4" s="72" t="s">
+      <c r="F4" s="76"/>
+      <c r="G4" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="73"/>
+      <c r="H4" s="76"/>
     </row>
     <row r="5" spans="2:12" ht="43" x14ac:dyDescent="0.25">
       <c r="B5" s="43" t="s">
@@ -5501,22 +5501,22 @@
         <v>166</v>
       </c>
       <c r="D8" s="56">
-        <f>C8/$C$6</f>
-        <v>0.33535353535353535</v>
+        <f>C8/SUM($C$8:$C$9)</f>
+        <v>0.44504021447721182</v>
       </c>
       <c r="E8" s="27">
         <v>1341</v>
       </c>
       <c r="F8" s="56">
-        <f>E8/$E$6</f>
-        <v>0.34544049459041731</v>
+        <f>E8/SUM($E$8:$E$9)</f>
+        <v>0.45581237253569001</v>
       </c>
       <c r="G8" s="27">
         <v>313546</v>
       </c>
       <c r="H8" s="56">
-        <f>G8/$G$6</f>
-        <v>0.67313583756083628</v>
+        <f>G8/SUM($G$8:$G$9)</f>
+        <v>0.73742041849230822</v>
       </c>
       <c r="I8" s="50"/>
       <c r="J8" s="42"/>
@@ -5531,22 +5531,22 @@
         <v>207</v>
       </c>
       <c r="D9" s="56">
-        <f t="shared" ref="D9:D11" si="0">C9/$C$6</f>
-        <v>0.41818181818181815</v>
+        <f>C9/SUM($C$8:$C$9)</f>
+        <v>0.55495978552278824</v>
       </c>
       <c r="E9" s="27">
         <v>1601</v>
       </c>
       <c r="F9" s="56">
-        <f t="shared" ref="F9:F11" si="1">E9/$E$6</f>
-        <v>0.41241628026790317</v>
+        <f t="shared" ref="F9:F11" si="0">E9/SUM($E$8:$E$9)</f>
+        <v>0.54418762746431004</v>
       </c>
       <c r="G9" s="27">
         <v>111647</v>
       </c>
       <c r="H9" s="56">
-        <f t="shared" ref="H9:H11" si="2">G9/$G$6</f>
-        <v>0.23968922217523009</v>
+        <f t="shared" ref="H9:H11" si="1">G9/SUM($G$8:$G$9)</f>
+        <v>0.26257958150769178</v>
       </c>
       <c r="I9" s="50"/>
       <c r="J9" s="42"/>
@@ -5561,22 +5561,22 @@
         <v>138</v>
       </c>
       <c r="D10" s="56">
-        <f t="shared" si="0"/>
-        <v>0.27878787878787881</v>
+        <f t="shared" ref="D10:D11" si="2">C10/SUM($C$8:$C$9)</f>
+        <v>0.36997319034852549</v>
       </c>
       <c r="E10" s="27">
         <v>1263</v>
       </c>
       <c r="F10" s="56">
-        <f t="shared" si="1"/>
-        <v>0.32534775888717155</v>
+        <f t="shared" si="0"/>
+        <v>0.429299796057104</v>
       </c>
       <c r="G10" s="27">
         <v>92192</v>
       </c>
       <c r="H10" s="56">
-        <f t="shared" si="2"/>
-        <v>0.19792227978162255</v>
+        <f t="shared" si="1"/>
+        <v>0.21682388938670205</v>
       </c>
       <c r="I10" s="50"/>
       <c r="J10" s="42"/>
@@ -5591,22 +5591,22 @@
         <v>69</v>
       </c>
       <c r="D11" s="56">
-        <f t="shared" si="0"/>
-        <v>0.1393939393939394</v>
+        <f>C11/SUM($C$8:$C$9)</f>
+        <v>0.18498659517426275</v>
       </c>
       <c r="E11" s="27">
         <v>338</v>
       </c>
       <c r="F11" s="56">
-        <f t="shared" si="1"/>
-        <v>8.7068521380731581E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.11488783140720599</v>
       </c>
       <c r="G11" s="27">
         <v>19455</v>
       </c>
       <c r="H11" s="56">
-        <f t="shared" si="2"/>
-        <v>4.1766942393607544E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.575569212098976E-2</v>
       </c>
       <c r="J11" s="41"/>
       <c r="K11" s="41"/>
@@ -5737,22 +5737,22 @@
         <v>175</v>
       </c>
       <c r="D17" s="56">
-        <f t="shared" si="3"/>
-        <v>0.13148009015777612</v>
+        <f>C17/SUM($C$17:$C$18)</f>
+        <v>0.13503086419753085</v>
       </c>
       <c r="E17" s="27">
         <v>326</v>
       </c>
       <c r="F17" s="56">
-        <f>E17/$E$15</f>
-        <v>4.9596835539327554E-2</v>
+        <f>E17/SUM($E$17:$E$18)</f>
+        <v>5.1185429423771391E-2</v>
       </c>
       <c r="G17" s="27">
         <v>27519</v>
       </c>
       <c r="H17" s="56">
-        <f t="shared" si="4"/>
-        <v>0.18899763057587307</v>
+        <f>G17/SUM($G$17:$G$18)</f>
+        <v>0.19148980585902164</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5763,22 +5763,22 @@
         <v>1121</v>
       </c>
       <c r="D18" s="56">
-        <f t="shared" si="3"/>
-        <v>0.8422238918106687</v>
+        <f t="shared" ref="D18:D20" si="5">C18/SUM($C$17:$C$18)</f>
+        <v>0.86496913580246915</v>
       </c>
       <c r="E18" s="27">
         <v>6043</v>
       </c>
       <c r="F18" s="56">
-        <f t="shared" ref="F18:F19" si="5">E18/$E$15</f>
-        <v>0.91936710786551046</v>
+        <f t="shared" ref="F18:F20" si="6">E18/SUM($E$17:$E$18)</f>
+        <v>0.94881457057622864</v>
       </c>
       <c r="G18" s="27">
         <v>116191</v>
       </c>
       <c r="H18" s="56">
-        <f t="shared" si="4"/>
-        <v>0.79798770646612416</v>
+        <f t="shared" ref="H18:H20" si="7">G18/SUM($G$17:$G$18)</f>
+        <v>0.80851019414097836</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5789,22 +5789,22 @@
         <v>327</v>
       </c>
       <c r="D19" s="56">
-        <f t="shared" si="3"/>
-        <v>0.24567993989481593</v>
+        <f t="shared" si="5"/>
+        <v>0.25231481481481483</v>
       </c>
       <c r="E19" s="27">
         <v>2167</v>
       </c>
       <c r="F19" s="56">
-        <f t="shared" si="5"/>
-        <v>0.32968203255743189</v>
+        <f t="shared" si="6"/>
+        <v>0.34024179620034545</v>
       </c>
       <c r="G19" s="27">
         <v>64122</v>
       </c>
       <c r="H19" s="56">
-        <f t="shared" si="4"/>
-        <v>0.44038322859791901</v>
+        <f t="shared" si="7"/>
+        <v>0.44619024424187598</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
@@ -5812,30 +5812,30 @@
         <v>22</v>
       </c>
       <c r="C20" s="33">
-        <v>69</v>
+        <v>794</v>
       </c>
       <c r="D20" s="57">
-        <f t="shared" si="3"/>
-        <v>5.1840721262208865E-2</v>
+        <f t="shared" si="5"/>
+        <v>0.61265432098765427</v>
       </c>
       <c r="E20" s="33">
         <v>3876</v>
       </c>
       <c r="F20" s="57">
-        <f>E20/$E$15</f>
-        <v>0.58968507530807845</v>
+        <f t="shared" si="6"/>
+        <v>0.6085727743758832</v>
       </c>
       <c r="G20" s="33">
         <v>52069</v>
       </c>
       <c r="H20" s="57">
-        <f t="shared" si="4"/>
-        <v>0.3576044778682051</v>
+        <f t="shared" si="7"/>
+        <v>0.36231994989910238</v>
       </c>
     </row>
     <row r="21" spans="2:8" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C23" s="95" t="s">
+      <c r="C23" s="67" t="s">
         <v>62</v>
       </c>
     </row>
@@ -5880,8 +5880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6087B295-164D-4F4E-913D-9E8EE4331FFD}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5896,51 +5896,51 @@
   <sheetData>
     <row r="1" spans="2:14" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:14" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="71"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="74"/>
     </row>
     <row r="3" spans="2:14" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
     </row>
     <row r="4" spans="2:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="68"/>
-      <c r="C4" s="72" t="s">
+      <c r="B4" s="71"/>
+      <c r="C4" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="73"/>
-      <c r="E4" s="72" t="s">
+      <c r="D4" s="76"/>
+      <c r="E4" s="75" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="73"/>
-      <c r="G4" s="72" t="s">
+      <c r="F4" s="76"/>
+      <c r="G4" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="73"/>
-      <c r="I4" s="72" t="s">
+      <c r="H4" s="76"/>
+      <c r="I4" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="73"/>
+      <c r="J4" s="76"/>
     </row>
     <row r="5" spans="2:14" ht="43" x14ac:dyDescent="0.2">
       <c r="B5" s="39" t="s">
@@ -6032,29 +6032,29 @@
         <v>7218</v>
       </c>
       <c r="D8" s="56">
-        <f>C8/$C$6</f>
-        <v>0.58640019497928342</v>
+        <f>C8/SUM($C$8:$C$9)</f>
+        <v>0.68339329672410531</v>
       </c>
       <c r="E8" s="27">
         <v>2244</v>
       </c>
       <c r="F8" s="56">
-        <f>E8/$E$6</f>
-        <v>0.59130434782608698</v>
+        <f>E8/SUM($E$8:$E$9)</f>
+        <v>0.67025089605734767</v>
       </c>
       <c r="G8" s="27">
         <v>12806</v>
       </c>
       <c r="H8" s="56">
-        <f>G8/$G$6</f>
-        <v>0.61688906016667466</v>
+        <f>G8/SUM($G$8:$G$9)</f>
+        <v>0.70024059492563429</v>
       </c>
       <c r="I8" s="27">
         <v>313546</v>
       </c>
       <c r="J8" s="56">
-        <f>I8/$I$6</f>
-        <v>0.67313583756083628</v>
+        <f>I8/SUM($I$8:$I$9)</f>
+        <v>0.73742041849230822</v>
       </c>
       <c r="K8" s="50"/>
       <c r="L8" s="42"/>
@@ -6069,29 +6069,29 @@
         <v>3344</v>
       </c>
       <c r="D9" s="56">
-        <f t="shared" ref="D9:D11" si="0">C9/$C$6</f>
-        <v>0.27167113494191242</v>
+        <f t="shared" ref="D9:D11" si="0">C9/SUM($C$8:$C$9)</f>
+        <v>0.31660670327589474</v>
       </c>
       <c r="E9" s="27">
         <v>1104</v>
       </c>
       <c r="F9" s="56">
-        <f t="shared" ref="F9:F11" si="1">E9/$E$6</f>
-        <v>0.29090909090909089</v>
+        <f t="shared" ref="F9:F11" si="1">E9/SUM($E$8:$E$9)</f>
+        <v>0.32974910394265233</v>
       </c>
       <c r="G9" s="27">
         <v>5482</v>
       </c>
       <c r="H9" s="56">
-        <f t="shared" ref="H9:H11" si="2">G9/$G$6</f>
-        <v>0.26407823112866707</v>
+        <f t="shared" ref="H9:H11" si="2">G9/SUM($G$8:$G$9)</f>
+        <v>0.29975940507436571</v>
       </c>
       <c r="I9" s="27">
         <v>111647</v>
       </c>
       <c r="J9" s="56">
-        <f t="shared" ref="J9:J11" si="3">I9/$I$6</f>
-        <v>0.23968922217523009</v>
+        <f t="shared" ref="J9:J11" si="3">I9/SUM($I$8:$I$9)</f>
+        <v>0.26257958150769178</v>
       </c>
       <c r="K9" s="50"/>
       <c r="L9" s="42"/>
@@ -6107,28 +6107,28 @@
       </c>
       <c r="D10" s="56">
         <f t="shared" si="0"/>
-        <v>0.25696644731497276</v>
+        <v>0.29946979738685853</v>
       </c>
       <c r="E10" s="27">
         <v>1048</v>
       </c>
       <c r="F10" s="56">
         <f t="shared" si="1"/>
-        <v>0.2761528326745718</v>
+        <v>0.31302270011947431</v>
       </c>
       <c r="G10" s="27">
         <v>5195</v>
       </c>
       <c r="H10" s="56">
         <f t="shared" si="2"/>
-        <v>0.25025290235560482</v>
+        <v>0.28406605424321962</v>
       </c>
       <c r="I10" s="27">
         <v>92192</v>
       </c>
       <c r="J10" s="56">
         <f t="shared" si="3"/>
-        <v>0.19792227978162255</v>
+        <v>0.21682388938670205</v>
       </c>
       <c r="K10" s="50"/>
       <c r="L10" s="42"/>
@@ -6144,28 +6144,28 @@
       </c>
       <c r="D11" s="56">
         <f t="shared" si="0"/>
-        <v>1.4704687626939638E-2</v>
+        <v>1.7136905889036168E-2</v>
       </c>
       <c r="E11" s="27">
         <v>56</v>
       </c>
       <c r="F11" s="56">
         <f t="shared" si="1"/>
-        <v>1.4756258234519103E-2</v>
+        <v>1.6726403823178016E-2</v>
       </c>
       <c r="G11" s="27">
         <v>287</v>
       </c>
       <c r="H11" s="56">
         <f t="shared" si="2"/>
-        <v>1.3825328773062286E-2</v>
+        <v>1.5693350831146105E-2</v>
       </c>
       <c r="I11" s="27">
         <v>19455</v>
       </c>
       <c r="J11" s="56">
         <f t="shared" si="3"/>
-        <v>4.1766942393607544E-2</v>
+        <v>4.575569212098976E-2</v>
       </c>
       <c r="L11" s="41"/>
       <c r="M11" s="41"/>
@@ -6326,29 +6326,29 @@
         <v>1003</v>
       </c>
       <c r="D17" s="56">
-        <f t="shared" si="4"/>
-        <v>0.18153846153846154</v>
+        <f>C17/SUM($C$17:$C$18)</f>
+        <v>0.1847145488029466</v>
       </c>
       <c r="E17" s="27">
         <v>512</v>
       </c>
       <c r="F17" s="56">
-        <f t="shared" si="5"/>
-        <v>0.34782608695652173</v>
+        <f>E17/SUM($E$17:$E$18)</f>
+        <v>0.34924965893587995</v>
       </c>
       <c r="G17" s="27">
         <v>2214</v>
       </c>
       <c r="H17" s="56">
-        <f t="shared" si="6"/>
-        <v>0.25474628926475662</v>
+        <f>G17/SUM($G$17:$G$18)</f>
+        <v>0.25774155995343423</v>
       </c>
       <c r="I17" s="27">
         <v>27519</v>
       </c>
       <c r="J17" s="56">
-        <f t="shared" si="7"/>
-        <v>0.18899763057587307</v>
+        <f>I17/SUM($I$17:$I$18)</f>
+        <v>0.19148980585902164</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6359,29 +6359,29 @@
         <v>4427</v>
       </c>
       <c r="D18" s="56">
-        <f t="shared" si="4"/>
-        <v>0.80126696832579181</v>
+        <f t="shared" ref="D18:D20" si="9">C18/SUM($C$17:$C$18)</f>
+        <v>0.81528545119705342</v>
       </c>
       <c r="E18" s="27">
         <v>954</v>
       </c>
       <c r="F18" s="56">
-        <f t="shared" si="5"/>
-        <v>0.64809782608695654</v>
+        <f t="shared" ref="F18:F20" si="10">E18/SUM($E$17:$E$18)</f>
+        <v>0.65075034106412011</v>
       </c>
       <c r="G18" s="27">
         <v>6376</v>
       </c>
       <c r="H18" s="56">
-        <f t="shared" si="6"/>
-        <v>0.73363249338396042</v>
+        <f t="shared" ref="H18:H20" si="11">G18/SUM($G$17:$G$18)</f>
+        <v>0.74225844004656583</v>
       </c>
       <c r="I18" s="27">
         <v>116191</v>
       </c>
       <c r="J18" s="56">
-        <f t="shared" si="7"/>
-        <v>0.79798770646612416</v>
+        <f t="shared" ref="J18:J20" si="12">I18/SUM($I$17:$I$18)</f>
+        <v>0.80851019414097836</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6392,29 +6392,29 @@
         <v>3188</v>
       </c>
       <c r="D19" s="56">
-        <f t="shared" si="4"/>
-        <v>0.57701357466063352</v>
+        <f t="shared" si="9"/>
+        <v>0.58710865561694292</v>
       </c>
       <c r="E19" s="27">
         <v>598</v>
       </c>
       <c r="F19" s="56">
-        <f t="shared" si="5"/>
-        <v>0.40625</v>
+        <f t="shared" si="10"/>
+        <v>0.40791268758526605</v>
       </c>
       <c r="G19" s="27">
         <v>4413</v>
       </c>
       <c r="H19" s="56">
-        <f t="shared" si="6"/>
-        <v>0.50776665516051089</v>
+        <f t="shared" si="11"/>
+        <v>0.51373690337601863</v>
       </c>
       <c r="I19" s="27">
         <v>64122</v>
       </c>
       <c r="J19" s="56">
-        <f t="shared" si="7"/>
-        <v>0.44038322859791901</v>
+        <f t="shared" si="12"/>
+        <v>0.44619024424187598</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
@@ -6425,34 +6425,34 @@
         <v>1239</v>
       </c>
       <c r="D20" s="57">
-        <f t="shared" si="4"/>
-        <v>0.22425339366515837</v>
+        <f t="shared" si="9"/>
+        <v>0.2281767955801105</v>
       </c>
       <c r="E20" s="33">
         <v>356</v>
       </c>
       <c r="F20" s="57">
-        <f t="shared" si="5"/>
-        <v>0.24184782608695651</v>
+        <f t="shared" si="10"/>
+        <v>0.24283765347885403</v>
       </c>
       <c r="G20" s="33">
         <v>1963</v>
       </c>
       <c r="H20" s="57">
-        <f t="shared" si="6"/>
-        <v>0.22586583822344955</v>
+        <f t="shared" si="11"/>
+        <v>0.22852153667054714</v>
       </c>
       <c r="I20" s="33">
         <v>52069</v>
       </c>
       <c r="J20" s="57">
-        <f t="shared" si="7"/>
-        <v>0.3576044778682051</v>
+        <f t="shared" si="12"/>
+        <v>0.36231994989910238</v>
       </c>
     </row>
     <row r="21" spans="2:10" s="49" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C24" s="95" t="s">
+      <c r="C24" s="67" t="s">
         <v>62</v>
       </c>
     </row>
@@ -6528,61 +6528,61 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="80" t="s">
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
     </row>
     <row r="3" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="81"/>
-      <c r="B3" s="81"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="82" t="s">
+      <c r="A3" s="84"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="83"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="88" t="s">
+      <c r="F3" s="86"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="90"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="92"/>
+      <c r="K3" s="92"/>
+      <c r="L3" s="92"/>
+      <c r="M3" s="93"/>
     </row>
     <row r="4" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="81"/>
-      <c r="B4" s="81"/>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="87"/>
-      <c r="H4" s="91" t="s">
+      <c r="A4" s="84"/>
+      <c r="B4" s="84"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="84"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="89"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="92"/>
-      <c r="J4" s="93"/>
-      <c r="K4" s="91" t="s">
+      <c r="I4" s="95"/>
+      <c r="J4" s="96"/>
+      <c r="K4" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="92"/>
-      <c r="M4" s="93"/>
+      <c r="L4" s="95"/>
+      <c r="M4" s="96"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>

</xml_diff>